<commit_message>
updated report for example purposes, including expanding left margin of title to better allow for longer city names
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/ghsci-3.0.0/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CED04CE-3476-4A81-BA3D-7F271E4F6C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{2CED04CE-3476-4A81-BA3D-7F271E4F6C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F19BCD-9B4F-44D2-8636-A09B3BF0E6B0}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_web" sheetId="1" r:id="rId1"/>
@@ -8076,11 +8076,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V194"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B176" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A191" sqref="A191"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8162,7 +8162,7 @@
         <v>19</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>110</v>
@@ -31128,7 +31128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
updated spatial report template detail, including high resolution contextual map showing study region
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38A126A7-9E6F-4B70-827A-8A7A6EB60C50}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE6CD053-7C18-45E7-B747-E669C22D447E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">languages!$B$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">policy_spatial!$A$1:$T$188</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">print_not_implemented!$A$1:$T$194</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">spatial!$A$1:$T$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">spatial!$A$1:$T$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="1711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="1712">
   <si>
     <t>name</t>
   </si>
@@ -5300,6 +5300,9 @@
   </si>
   <si>
     <t>Español de España</t>
+  </si>
+  <si>
+    <t>study_region_context</t>
   </si>
 </sst>
 </file>
@@ -17735,13 +17738,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275ED209-18EA-43FD-841F-C491018348BF}">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18970,7 +18973,7 @@
         <v>13</v>
       </c>
       <c r="F22">
-        <f>D26-3</f>
+        <f>D25-3</f>
         <v>131</v>
       </c>
       <c r="G22">
@@ -19073,40 +19076,37 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>1711</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <f>D22</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>75</v>
+        <f>E23</f>
+        <v>41</v>
       </c>
       <c r="F24">
-        <f>D24+92</f>
-        <v>99</v>
+        <f>D25</f>
+        <v>134</v>
       </c>
       <c r="G24">
-        <f>E24+3</f>
-        <v>78</v>
-      </c>
-      <c r="H24" t="s">
-        <v>180</v>
+        <f>F24/192*144</f>
+        <v>100.5</v>
       </c>
       <c r="I24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -19118,10 +19118,10 @@
         <v>26</v>
       </c>
       <c r="Q24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" t="s">
         <v>208</v>
@@ -19132,35 +19132,32 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>1670</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D25">
-        <f>D24-2</f>
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="E25">
-        <f>E24</f>
-        <v>75</v>
+        <f>E22</f>
+        <v>13</v>
       </c>
       <c r="F25">
-        <f>D25+90</f>
-        <v>95</v>
+        <v>210</v>
       </c>
       <c r="G25">
-        <f>E25+90</f>
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -19168,14 +19165,17 @@
       <c r="L25">
         <v>0</v>
       </c>
+      <c r="M25" t="s">
+        <v>1319</v>
+      </c>
       <c r="N25" t="s">
-        <v>21</v>
+        <v>1319</v>
       </c>
       <c r="O25" t="s">
         <v>26</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R25" t="b">
         <v>0</v>
@@ -19189,29 +19189,34 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D26">
-        <v>134</v>
+        <f>D25+1</f>
+        <v>135</v>
       </c>
       <c r="E26">
-        <f>E22</f>
-        <v>13</v>
+        <f>E25+3</f>
+        <v>16</v>
       </c>
       <c r="F26">
         <v>210</v>
       </c>
       <c r="G26">
-        <v>161</v>
+        <f>E26+3</f>
+        <v>19</v>
+      </c>
+      <c r="H26" t="s">
+        <v>180</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -19221,9 +19226,6 @@
       </c>
       <c r="L26">
         <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>1319</v>
       </c>
       <c r="N26" t="s">
         <v>1319</v>
@@ -19231,8 +19233,11 @@
       <c r="O26" t="s">
         <v>26</v>
       </c>
+      <c r="P26" t="s">
+        <v>1677</v>
+      </c>
       <c r="Q26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R26" t="b">
         <v>0</v>
@@ -19246,7 +19251,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1671</v>
+        <v>1679</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -19255,28 +19260,29 @@
         <v>19</v>
       </c>
       <c r="D27">
-        <f>D26+1</f>
+        <f>$D$26</f>
         <v>135</v>
       </c>
       <c r="E27">
-        <f>E26+3</f>
-        <v>16</v>
+        <f>G26+5</f>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>210</v>
+        <f>D27+74</f>
+        <v>209</v>
       </c>
       <c r="G27">
         <f>E27+3</f>
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H27" t="s">
         <v>180</v>
       </c>
       <c r="I27">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -19290,14 +19296,11 @@
       <c r="O27" t="s">
         <v>26</v>
       </c>
-      <c r="P27" t="s">
-        <v>1677</v>
-      </c>
       <c r="Q27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27" t="s">
         <v>208</v>
@@ -19308,7 +19311,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -19317,20 +19320,20 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <f>$D$27</f>
+        <f>$D$26</f>
         <v>135</v>
       </c>
       <c r="E28">
-        <f>G27+5</f>
-        <v>24</v>
+        <f>G27+1</f>
+        <v>28</v>
       </c>
       <c r="F28">
         <f>D28+74</f>
         <v>209</v>
       </c>
       <c r="G28">
-        <f>E28+3</f>
-        <v>27</v>
+        <f>E28+4</f>
+        <v>32</v>
       </c>
       <c r="H28" t="s">
         <v>180</v>
@@ -19342,7 +19345,7 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -19368,7 +19371,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -19377,20 +19380,20 @@
         <v>19</v>
       </c>
       <c r="D29">
-        <f>$D$27</f>
-        <v>135</v>
+        <f>$D25</f>
+        <v>134</v>
       </c>
       <c r="E29">
-        <f>G28+1</f>
-        <v>28</v>
+        <f>G28+12</f>
+        <v>44</v>
       </c>
       <c r="F29">
-        <f>D29+74</f>
+        <f t="shared" ref="F29:F40" si="2">F27</f>
         <v>209</v>
       </c>
       <c r="G29">
-        <f>E29+4</f>
-        <v>32</v>
+        <f>E29+3</f>
+        <v>47</v>
       </c>
       <c r="H29" t="s">
         <v>180</v>
@@ -19402,7 +19405,7 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -19428,7 +19431,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -19438,19 +19441,19 @@
       </c>
       <c r="D30">
         <f>$D26</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E30">
-        <f>G29+12</f>
-        <v>44</v>
+        <f>G29+1</f>
+        <v>48</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:F41" si="2">F28</f>
+        <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G30">
-        <f>E30+3</f>
-        <v>47</v>
+        <f>E30+4</f>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
         <v>180</v>
@@ -19462,7 +19465,7 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -19488,7 +19491,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -19497,20 +19500,20 @@
         <v>19</v>
       </c>
       <c r="D31">
-        <f>$D27</f>
+        <f t="shared" ref="D31:D40" si="3">$D$26</f>
         <v>135</v>
       </c>
       <c r="E31">
-        <f>G30+1</f>
-        <v>48</v>
+        <f>G30+12</f>
+        <v>64</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G31">
-        <f>E31+4</f>
-        <v>52</v>
+        <f>E31+3</f>
+        <v>67</v>
       </c>
       <c r="H31" t="s">
         <v>180</v>
@@ -19522,7 +19525,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -19548,7 +19551,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -19557,20 +19560,20 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <f t="shared" ref="D32:D41" si="3">$D$27</f>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="E32">
-        <f>G31+12</f>
-        <v>64</v>
+        <f>G31+1</f>
+        <v>68</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G32">
-        <f>E32+3</f>
-        <v>67</v>
+        <f>E32+4</f>
+        <v>72</v>
       </c>
       <c r="H32" t="s">
         <v>180</v>
@@ -19582,7 +19585,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -19608,7 +19611,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -19621,16 +19624,16 @@
         <v>135</v>
       </c>
       <c r="E33">
-        <f>G32+1</f>
-        <v>68</v>
+        <f>G32+12</f>
+        <v>84</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G33">
-        <f>E33+4</f>
-        <v>72</v>
+        <f>E33+3</f>
+        <v>87</v>
       </c>
       <c r="H33" t="s">
         <v>180</v>
@@ -19642,7 +19645,7 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -19668,7 +19671,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -19681,16 +19684,16 @@
         <v>135</v>
       </c>
       <c r="E34">
-        <f>G33+12</f>
-        <v>84</v>
+        <f>G33+1</f>
+        <v>88</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G34">
-        <f>E34+3</f>
-        <v>87</v>
+        <f>E34+4</f>
+        <v>92</v>
       </c>
       <c r="H34" t="s">
         <v>180</v>
@@ -19702,7 +19705,7 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -19728,7 +19731,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -19741,16 +19744,16 @@
         <v>135</v>
       </c>
       <c r="E35">
-        <f>G34+1</f>
-        <v>88</v>
+        <f>G34+12</f>
+        <v>104</v>
       </c>
       <c r="F35">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G35">
-        <f>E35+4</f>
-        <v>92</v>
+        <f>E35+3</f>
+        <v>107</v>
       </c>
       <c r="H35" t="s">
         <v>180</v>
@@ -19762,7 +19765,7 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -19788,7 +19791,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -19801,16 +19804,16 @@
         <v>135</v>
       </c>
       <c r="E36">
-        <f>G35+12</f>
-        <v>104</v>
+        <f>G35+1</f>
+        <v>108</v>
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G36">
-        <f>E36+3</f>
-        <v>107</v>
+        <f>E36+4</f>
+        <v>112</v>
       </c>
       <c r="H36" t="s">
         <v>180</v>
@@ -19822,7 +19825,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -19848,7 +19851,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -19861,16 +19864,16 @@
         <v>135</v>
       </c>
       <c r="E37">
-        <f>G36+1</f>
-        <v>108</v>
+        <f>G36+12</f>
+        <v>124</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G37">
-        <f>E37+4</f>
-        <v>112</v>
+        <f>E37+3</f>
+        <v>127</v>
       </c>
       <c r="H37" t="s">
         <v>180</v>
@@ -19882,7 +19885,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -19908,7 +19911,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -19921,16 +19924,16 @@
         <v>135</v>
       </c>
       <c r="E38">
-        <f>G37+12</f>
-        <v>124</v>
+        <f>G37+1</f>
+        <v>128</v>
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G38">
-        <f>E38+3</f>
-        <v>127</v>
+        <f>E38+4</f>
+        <v>132</v>
       </c>
       <c r="H38" t="s">
         <v>180</v>
@@ -19942,7 +19945,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -19968,7 +19971,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -19981,16 +19984,16 @@
         <v>135</v>
       </c>
       <c r="E39">
-        <f>G38+1</f>
-        <v>128</v>
+        <f>G38+12</f>
+        <v>144</v>
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G39">
-        <f>E39+4</f>
-        <v>132</v>
+        <f>E39+3</f>
+        <v>147</v>
       </c>
       <c r="H39" t="s">
         <v>180</v>
@@ -20002,7 +20005,7 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -20028,7 +20031,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -20041,16 +20044,16 @@
         <v>135</v>
       </c>
       <c r="E40">
-        <f>G39+12</f>
-        <v>144</v>
+        <f>G39+1</f>
+        <v>148</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
       <c r="G40">
-        <f>E40+3</f>
-        <v>147</v>
+        <f>E40+4</f>
+        <v>152</v>
       </c>
       <c r="H40" t="s">
         <v>180</v>
@@ -20062,7 +20065,7 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40">
         <v>0</v>
@@ -20088,7 +20091,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1692</v>
+        <v>34</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -20097,20 +20100,17 @@
         <v>19</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="E41">
-        <f>G40+1</f>
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G41">
-        <f>E41+4</f>
-        <v>152</v>
+        <f>E41+3</f>
+        <v>168</v>
       </c>
       <c r="H41" t="s">
         <v>180</v>
@@ -20119,25 +20119,25 @@
         <v>10</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>1319</v>
+        <v>21</v>
       </c>
       <c r="O41" t="s">
         <v>26</v>
       </c>
       <c r="Q41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" t="s">
         <v>208</v>
@@ -20148,7 +20148,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -20157,26 +20157,28 @@
         <v>19</v>
       </c>
       <c r="D42">
+        <f>D41</f>
         <v>7</v>
       </c>
       <c r="E42">
-        <v>165</v>
+        <f>G41+3</f>
+        <v>171</v>
       </c>
       <c r="F42">
         <v>203</v>
       </c>
       <c r="G42">
-        <f>E42+3</f>
-        <v>168</v>
+        <f>E42+4</f>
+        <v>175</v>
       </c>
       <c r="H42" t="s">
         <v>180</v>
       </c>
       <c r="I42">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -20188,13 +20190,14 @@
         <v>21</v>
       </c>
       <c r="O42" t="s">
-        <v>26</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="P42" s="1"/>
       <c r="Q42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" t="s">
         <v>208</v>
@@ -20205,34 +20208,28 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D43">
-        <f>D42</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E43">
-        <f>G42+3</f>
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="F43">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="G43">
-        <f>E43+4</f>
-        <v>175</v>
-      </c>
-      <c r="H43" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="I43">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -20247,14 +20244,13 @@
         <v>21</v>
       </c>
       <c r="O43" t="s">
-        <v>179</v>
-      </c>
-      <c r="P43" s="1"/>
+        <v>26</v>
+      </c>
       <c r="Q43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43" t="s">
         <v>208</v>
@@ -20265,34 +20261,37 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>449</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D44">
         <v>5</v>
       </c>
       <c r="E44">
-        <v>203</v>
+        <v>283</v>
       </c>
       <c r="F44">
         <v>93</v>
       </c>
       <c r="G44">
-        <v>283</v>
+        <v>286</v>
+      </c>
+      <c r="H44" t="s">
+        <v>180</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -20301,13 +20300,13 @@
         <v>21</v>
       </c>
       <c r="O44" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="Q44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>208</v>
@@ -20318,7 +20317,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>449</v>
+        <v>33</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -20327,16 +20326,19 @@
         <v>19</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E45">
-        <v>283</v>
+        <f>E43</f>
+        <v>203</v>
       </c>
       <c r="F45">
-        <v>93</v>
+        <f>D45+92</f>
+        <v>192</v>
       </c>
       <c r="G45">
-        <v>286</v>
+        <f>E45+3</f>
+        <v>206</v>
       </c>
       <c r="H45" t="s">
         <v>180</v>
@@ -20357,10 +20359,10 @@
         <v>21</v>
       </c>
       <c r="O45" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="Q45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R45" t="b">
         <v>1</v>
@@ -20374,35 +20376,35 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>7</v>
+        <f>D45-2</f>
+        <v>98</v>
       </c>
       <c r="E46">
-        <v>13</v>
+        <f>E45</f>
+        <v>203</v>
       </c>
       <c r="F46">
-        <f>D46+100</f>
-        <v>107</v>
+        <f>D46+90</f>
+        <v>188</v>
       </c>
       <c r="G46">
-        <v>16</v>
-      </c>
-      <c r="H46" t="s">
-        <v>180</v>
+        <f>E46+90</f>
+        <v>293</v>
       </c>
       <c r="I46">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -20417,7 +20419,7 @@
         <v>26</v>
       </c>
       <c r="Q46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R46" t="b">
         <v>0</v>
@@ -20431,33 +20433,35 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E47">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F47">
-        <f>D47+88</f>
-        <v>93</v>
+        <f>D47+100</f>
+        <v>107</v>
       </c>
       <c r="G47">
-        <f>E47+80</f>
-        <v>98</v>
+        <v>16</v>
+      </c>
+      <c r="H47" t="s">
+        <v>180</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -20486,41 +20490,36 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>446</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D48">
-        <f>D47-2</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48">
-        <f>G47</f>
+        <v>18</v>
+      </c>
+      <c r="F48">
+        <f>D48+88</f>
+        <v>93</v>
+      </c>
+      <c r="G48">
+        <f>E48+80</f>
         <v>98</v>
       </c>
-      <c r="F48">
-        <f>F47+2</f>
-        <v>95</v>
-      </c>
-      <c r="G48">
-        <f>E48+3</f>
-        <v>101</v>
-      </c>
-      <c r="H48" t="s">
-        <v>180</v>
-      </c>
       <c r="I48">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J48">
         <v>0</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48">
         <v>0</v>
@@ -20529,13 +20528,13 @@
         <v>21</v>
       </c>
       <c r="O48" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="Q48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" t="s">
         <v>208</v>
@@ -20546,7 +20545,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>446</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -20555,29 +20554,32 @@
         <v>19</v>
       </c>
       <c r="D49">
-        <v>111</v>
+        <f>D48-2</f>
+        <v>3</v>
       </c>
       <c r="E49">
-        <v>13</v>
+        <f>G48</f>
+        <v>98</v>
       </c>
       <c r="F49">
-        <f>D49+92</f>
-        <v>203</v>
+        <f>F48+2</f>
+        <v>95</v>
       </c>
       <c r="G49">
-        <v>16</v>
+        <f>E49+3</f>
+        <v>101</v>
       </c>
       <c r="H49" t="s">
         <v>180</v>
       </c>
       <c r="I49">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -20586,13 +20588,13 @@
         <v>21</v>
       </c>
       <c r="O49" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="Q49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S49" t="s">
         <v>208</v>
@@ -20603,34 +20605,35 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50">
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D50">
-        <f>D49-2</f>
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E50">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F50">
-        <f>D50+88</f>
-        <v>197</v>
+        <f>D50+92</f>
+        <v>203</v>
       </c>
       <c r="G50">
-        <f>E50+80</f>
-        <v>98</v>
+        <v>16</v>
+      </c>
+      <c r="H50" t="s">
+        <v>180</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -20659,41 +20662,37 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>447</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D51">
         <f>D50-2</f>
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E51">
-        <f>G50</f>
+        <v>18</v>
+      </c>
+      <c r="F51">
+        <f>D51+88</f>
+        <v>197</v>
+      </c>
+      <c r="G51">
+        <f>E51+80</f>
         <v>98</v>
       </c>
-      <c r="F51">
-        <f>F50+2</f>
-        <v>199</v>
-      </c>
-      <c r="G51">
-        <f>E51+3</f>
-        <v>101</v>
-      </c>
-      <c r="H51" t="s">
-        <v>180</v>
-      </c>
       <c r="I51">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <v>0</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -20702,13 +20701,13 @@
         <v>21</v>
       </c>
       <c r="O51" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="Q51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S51" t="s">
         <v>208</v>
@@ -20718,8 +20717,8 @@
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>203</v>
+      <c r="A52" t="s">
+        <v>447</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -20728,32 +20727,32 @@
         <v>19</v>
       </c>
       <c r="D52">
-        <f>D46</f>
-        <v>7</v>
+        <f>D51-2</f>
+        <v>107</v>
       </c>
       <c r="E52">
-        <f>G50+7</f>
-        <v>105</v>
+        <f>G51</f>
+        <v>98</v>
       </c>
       <c r="F52">
-        <f>F49</f>
-        <v>203</v>
+        <f>F51+2</f>
+        <v>199</v>
       </c>
       <c r="G52">
         <f>E52+3</f>
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H52" t="s">
         <v>180</v>
       </c>
       <c r="I52">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J52">
         <v>0</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -20762,7 +20761,7 @@
         <v>21</v>
       </c>
       <c r="O52" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="Q52">
         <v>3</v>
@@ -20779,41 +20778,44 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>448</v>
+        <v>203</v>
       </c>
       <c r="B53">
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <f>D47</f>
+        <v>7</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <f>G51+7</f>
+        <v>105</v>
       </c>
       <c r="F53">
-        <v>210</v>
+        <f>F50</f>
+        <v>203</v>
       </c>
       <c r="G53">
-        <f>G52+9</f>
-        <v>117</v>
+        <f>E53+3</f>
+        <v>108</v>
+      </c>
+      <c r="H53" t="s">
+        <v>180</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
         <v>0</v>
-      </c>
-      <c r="M53" t="s">
-        <v>21</v>
       </c>
       <c r="N53" t="s">
         <v>21</v>
@@ -20822,10 +20824,10 @@
         <v>26</v>
       </c>
       <c r="Q53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S53" t="s">
         <v>208</v>
@@ -20835,39 +20837,42 @@
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>177</v>
+      <c r="A54" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="B54">
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="F54">
         <v>210</v>
       </c>
       <c r="G54">
-        <f>E54+210</f>
-        <v>318</v>
+        <f>G53+9</f>
+        <v>117</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
         <v>0</v>
+      </c>
+      <c r="M54" t="s">
+        <v>21</v>
       </c>
       <c r="N54" t="s">
         <v>21</v>
@@ -20876,7 +20881,7 @@
         <v>26</v>
       </c>
       <c r="Q54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R54" t="b">
         <v>0</v>
@@ -20890,38 +20895,35 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D55">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="F55">
         <v>210</v>
       </c>
       <c r="G55">
-        <f>E55+5</f>
-        <v>216</v>
-      </c>
-      <c r="H55" t="s">
-        <v>180</v>
+        <f>E55+210</f>
+        <v>318</v>
       </c>
       <c r="I55">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J55">
         <v>0</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -20936,7 +20938,7 @@
         <v>0</v>
       </c>
       <c r="R55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S55" t="s">
         <v>208</v>
@@ -20947,7 +20949,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1512</v>
+        <v>178</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -20956,23 +20958,23 @@
         <v>19</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E56">
-        <f>G56-3</f>
-        <v>294</v>
+        <v>211</v>
       </c>
       <c r="F56">
         <v>210</v>
       </c>
       <c r="G56">
-        <v>297</v>
+        <f>E56+5</f>
+        <v>216</v>
       </c>
       <c r="H56" t="s">
         <v>180</v>
       </c>
       <c r="I56">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -20984,13 +20986,13 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>677</v>
+        <v>21</v>
       </c>
       <c r="O56" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Q56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R56" t="b">
         <v>1</v>
@@ -21004,52 +21006,53 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>1512</v>
       </c>
       <c r="B57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
       </c>
       <c r="D57">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>13</v>
+        <f>G57-3</f>
+        <v>294</v>
       </c>
       <c r="F57">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="G57">
-        <v>16</v>
+        <v>297</v>
       </c>
       <c r="H57" t="s">
         <v>180</v>
       </c>
       <c r="I57">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L57">
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>21</v>
+        <v>677</v>
       </c>
       <c r="O57" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="Q57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S57" t="s">
         <v>208</v>
@@ -21060,7 +21063,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -21069,27 +21072,25 @@
         <v>19</v>
       </c>
       <c r="D58">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E58">
-        <f>G57+4</f>
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F58">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G58">
-        <f>E58+4</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H58" t="s">
         <v>180</v>
       </c>
       <c r="I58">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -21101,14 +21102,13 @@
         <v>21</v>
       </c>
       <c r="O58" t="s">
-        <v>179</v>
-      </c>
-      <c r="P58" s="1"/>
+        <v>26</v>
+      </c>
       <c r="Q58">
         <v>2</v>
       </c>
       <c r="R58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S58" t="s">
         <v>208</v>
@@ -21119,31 +21119,33 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B59">
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="E59">
-        <f>G57+4</f>
+        <f>G58+4</f>
         <v>20</v>
       </c>
       <c r="F59">
-        <f>D59+88</f>
-        <v>93</v>
+        <v>205</v>
       </c>
       <c r="G59">
-        <f>E59+80</f>
-        <v>100</v>
+        <f>E59+4</f>
+        <v>24</v>
+      </c>
+      <c r="H59" t="s">
+        <v>180</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -21158,13 +21160,14 @@
         <v>21</v>
       </c>
       <c r="O59" t="s">
-        <v>26</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="P59" s="1"/>
       <c r="Q59">
         <v>2</v>
       </c>
       <c r="R59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S59" t="s">
         <v>208</v>
@@ -21175,34 +21178,34 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="B60">
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E60">
-        <v>134</v>
+        <f>G58+4</f>
+        <v>20</v>
       </c>
       <c r="F60">
-        <v>203</v>
+        <f>D60+88</f>
+        <v>93</v>
       </c>
       <c r="G60">
-        <v>137</v>
-      </c>
-      <c r="H60" t="s">
-        <v>180</v>
+        <f>E60+80</f>
+        <v>100</v>
       </c>
       <c r="I60">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -21231,7 +21234,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -21240,25 +21243,25 @@
         <v>19</v>
       </c>
       <c r="D61">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E61">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F61">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G61">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H61" t="s">
         <v>180</v>
       </c>
       <c r="I61">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -21270,14 +21273,13 @@
         <v>21</v>
       </c>
       <c r="O61" t="s">
-        <v>179</v>
-      </c>
-      <c r="P61" s="1"/>
+        <v>26</v>
+      </c>
       <c r="Q61">
         <v>2</v>
       </c>
       <c r="R61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" t="s">
         <v>208</v>
@@ -21288,28 +21290,31 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="B62">
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="E62">
         <v>141</v>
       </c>
       <c r="F62">
-        <v>93</v>
+        <v>205</v>
       </c>
       <c r="G62">
-        <v>221</v>
+        <v>145</v>
+      </c>
+      <c r="H62" t="s">
+        <v>180</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -21324,13 +21329,14 @@
         <v>21</v>
       </c>
       <c r="O62" t="s">
-        <v>26</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="P62" s="1"/>
       <c r="Q62">
         <v>2</v>
       </c>
       <c r="R62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62" t="s">
         <v>208</v>
@@ -21341,31 +21347,31 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>223</v>
+        <v>49</v>
       </c>
       <c r="B63">
         <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E63">
-        <v>222</v>
+        <v>141</v>
       </c>
       <c r="F63">
-        <v>210</v>
+        <v>93</v>
       </c>
       <c r="G63">
-        <v>298</v>
+        <v>221</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -21373,11 +21379,8 @@
       <c r="L63">
         <v>0</v>
       </c>
-      <c r="M63" t="s">
-        <v>1319</v>
-      </c>
       <c r="N63" t="s">
-        <v>1319</v>
+        <v>21</v>
       </c>
       <c r="O63" t="s">
         <v>26</v>
@@ -21397,31 +21400,28 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B64">
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D64">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F64">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="G64">
-        <v>229</v>
-      </c>
-      <c r="H64" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="I64">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -21431,18 +21431,21 @@
       </c>
       <c r="L64">
         <v>0</v>
+      </c>
+      <c r="M64" t="s">
+        <v>1319</v>
       </c>
       <c r="N64" t="s">
         <v>1319</v>
       </c>
       <c r="O64" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="Q64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S64" t="s">
         <v>208</v>
@@ -21453,7 +21456,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -21465,22 +21468,22 @@
         <v>13</v>
       </c>
       <c r="E65">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F65">
         <v>199</v>
       </c>
       <c r="G65">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H65" t="s">
         <v>180</v>
       </c>
       <c r="I65">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65">
         <v>0</v>
@@ -21509,29 +21512,31 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D66">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E66">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F66">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="G66">
-        <f>E66</f>
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H66" t="s">
+        <v>180</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -21543,16 +21548,16 @@
         <v>0</v>
       </c>
       <c r="N66" t="s">
-        <v>677</v>
+        <v>1319</v>
       </c>
       <c r="O66" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="Q66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S66" t="s">
         <v>208</v>
@@ -21563,37 +21568,32 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>546</v>
+        <v>30</v>
       </c>
       <c r="B67">
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D67">
         <v>20</v>
       </c>
       <c r="E67">
-        <f>E66+5</f>
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F67">
-        <f>F66</f>
         <v>190</v>
       </c>
       <c r="G67">
-        <f>E67+4</f>
-        <v>229</v>
-      </c>
-      <c r="H67" t="s">
-        <v>180</v>
+        <f>E67</f>
+        <v>220</v>
       </c>
       <c r="I67">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -21607,12 +21607,11 @@
       <c r="O67" t="s">
         <v>26</v>
       </c>
-      <c r="P67" s="1"/>
       <c r="Q67">
         <v>2</v>
       </c>
       <c r="R67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S67" t="s">
         <v>208</v>
@@ -21623,7 +21622,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1321</v>
+        <v>546</v>
       </c>
       <c r="B68">
         <v>6</v>
@@ -21635,8 +21634,8 @@
         <v>20</v>
       </c>
       <c r="E68">
-        <f>G67</f>
-        <v>229</v>
+        <f>E67+5</f>
+        <v>225</v>
       </c>
       <c r="F68">
         <f>F67</f>
@@ -21644,7 +21643,7 @@
       </c>
       <c r="G68">
         <f>E68+4</f>
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H68" t="s">
         <v>180</v>
@@ -21653,7 +21652,7 @@
         <v>8</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -21683,27 +21682,31 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>1321</v>
       </c>
       <c r="B69">
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D69">
         <v>20</v>
       </c>
       <c r="E69">
-        <v>260</v>
+        <f>G68</f>
+        <v>229</v>
       </c>
       <c r="F69">
-        <f>D69+40</f>
-        <v>60</v>
+        <f>F68</f>
+        <v>190</v>
       </c>
       <c r="G69">
-        <f>E69+14</f>
-        <v>274</v>
+        <f>E69+4</f>
+        <v>233</v>
+      </c>
+      <c r="H69" t="s">
+        <v>180</v>
       </c>
       <c r="I69">
         <v>8</v>
@@ -21723,9 +21726,7 @@
       <c r="O69" t="s">
         <v>26</v>
       </c>
-      <c r="P69" s="6" t="s">
-        <v>1510</v>
-      </c>
+      <c r="P69" s="1"/>
       <c r="Q69">
         <v>2</v>
       </c>
@@ -21733,38 +21734,35 @@
         <v>1</v>
       </c>
       <c r="S69" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>25</v>
       </c>
       <c r="D70">
         <v>20</v>
       </c>
       <c r="E70">
-        <f>G69+5</f>
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="F70">
-        <f>F68</f>
-        <v>190</v>
+        <f>D70+40</f>
+        <v>60</v>
       </c>
       <c r="G70">
-        <v>288</v>
-      </c>
-      <c r="H70" t="s">
-        <v>180</v>
+        <f>E70+14</f>
+        <v>274</v>
       </c>
       <c r="I70">
         <v>8</v>
@@ -21776,7 +21774,7 @@
         <v>0</v>
       </c>
       <c r="L70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N70" t="s">
         <v>677</v>
@@ -21785,7 +21783,7 @@
         <v>26</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>209</v>
+        <v>1510</v>
       </c>
       <c r="Q70">
         <v>2</v>
@@ -21800,30 +21798,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>678</v>
+        <v>204</v>
       </c>
       <c r="B71">
         <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>205</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <f>G70+5</f>
+        <v>279</v>
       </c>
       <c r="F71">
-        <v>211</v>
+        <f>F69</f>
+        <v>190</v>
       </c>
       <c r="G71">
-        <v>298</v>
+        <v>288</v>
+      </c>
+      <c r="H71" t="s">
+        <v>180</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -21832,7 +21835,7 @@
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N71" t="s">
         <v>677</v>
@@ -21840,22 +21843,78 @@
       <c r="O71" t="s">
         <v>26</v>
       </c>
+      <c r="P71" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="Q71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T71">
         <v>0</v>
       </c>
     </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>678</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>211</v>
+      </c>
+      <c r="G72">
+        <v>298</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="N72" t="s">
+        <v>677</v>
+      </c>
+      <c r="O72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="R72" t="b">
+        <v>0</v>
+      </c>
+      <c r="S72" t="s">
+        <v>208</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T68" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A52:A53">
+  <autoFilter ref="A1:T69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A53:A54">
     <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33391,11 +33450,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated configuration files to make sure latest changes have been committed
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3485" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C6CBAF7-E8DA-454D-827E-18BD2504C3FC}"/>
+  <xr:revisionPtr revIDLastSave="3488" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A030B283-2B7B-475B-B805-164A50C45D59}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -4796,9 +4796,6 @@
     <t>The findings could inform changes needed to local city policies. The maps show the distribution of urban design and transport features across {city_name} and identify areas that could benefit the most from interventions to create healthy and sustainable environments.</t>
   </si>
   <si>
-    <t>Public policies are essential for supporting the design and creation of healthy and sustainable cities and neighbourhoods. The 1000 Cities Challenge Checklist was used to assesses the presence and quality of policies aligned with evidence and principles for healthy and sustainable cities.</t>
-  </si>
-  <si>
     <t>Thresholds for 80% probability of engaging in walking for transport</t>
   </si>
   <si>
@@ -4838,9 +4835,6 @@
     <t>hero_alt_1</t>
   </si>
   <si>
-    <t>GoHSC principles alignment</t>
-  </si>
-  <si>
     <t>Climate disaster risk reduction</t>
   </si>
   <si>
@@ -4848,6 +4842,12 @@
   </si>
   <si>
     <t>In the face of climate change, built environments need to be designed to reduce the health impacts of increasingly frequent and severe extreme weather events, such as heat waves, flooding, bushfire/wildfire and extreme storms.</t>
+  </si>
+  <si>
+    <t>Aligns with health evidence</t>
+  </si>
+  <si>
+    <t>Public policies are essential for supporting the design and creation of healthy and sustainable cities and neighbourhoods. The 1000 Cities Challenge Policy Checklist was used to assess the presence and quality of policies aligned with evidence and principles for healthy and sustainable cities for {policy jurisdiction}.</t>
   </si>
 </sst>
 </file>
@@ -5540,12 +5540,9 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5578,9 +5575,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5926,7 +5926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T288"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6489,7 +6489,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6546,7 +6546,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -6600,7 +6600,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6810,7 +6810,7 @@
         <v>27</v>
       </c>
       <c r="P15" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -20001,7 +20001,7 @@
     </row>
     <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B238">
         <v>8</v>
@@ -21597,7 +21597,7 @@
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="B265">
         <v>8</v>
@@ -21655,7 +21655,7 @@
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="B266">
         <v>8</v>
@@ -22478,7 +22478,7 @@
     </row>
     <row r="280" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B280">
         <v>8</v>
@@ -22534,7 +22534,7 @@
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B281">
         <v>8</v>
@@ -22593,7 +22593,7 @@
     </row>
     <row r="282" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B282">
         <v>8</v>
@@ -23579,7 +23579,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -23636,7 +23636,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -23690,7 +23690,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -23900,7 +23900,7 @@
         <v>27</v>
       </c>
       <c r="P15" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -27883,11 +27883,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U136"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D91" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B109" sqref="B109"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28249,7 +28249,7 @@
         <v>1515</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -28278,7 +28278,7 @@
         <v>1516</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -28307,7 +28307,7 @@
         <v>1517</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -28333,7 +28333,7 @@
         <v>77</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1306</v>
@@ -30391,7 +30391,7 @@
         <v>1420</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1548</v>
+        <v>1565</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -31422,7 +31422,7 @@
         <v>1462</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
@@ -31541,7 +31541,7 @@
         <v>1325</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1562</v>
+        <v>1564</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
@@ -32635,13 +32635,13 @@
     </row>
     <row r="99" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="18"/>
@@ -32809,13 +32809,13 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
@@ -32841,10 +32841,10 @@
         <v>77</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
@@ -34306,36 +34306,36 @@
   <conditionalFormatting sqref="B7:B10">
     <cfRule type="duplicateValues" dxfId="7" priority="108"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B72 B1:B6 B74:B136">
+    <cfRule type="duplicateValues" dxfId="6" priority="136"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:U43 B44:L49 M44:U69 K50:L69 B50:J72 K70:U72 B74:D74 G74:U74 D74:J83 B75:C81 M75:U81 K75:L83 B80:D80 G80:U80 B82:U83 D84:L87 B84:C94 M84:U94 B114:C119 L114:L119 M114:U131 D116:J119 K117:K119 B120:L122 B123:J131 B132:U134 B135:J136 M135:U136 K136:L136 B88:U113">
-    <cfRule type="containsBlanks" dxfId="5" priority="19">
+  <conditionalFormatting sqref="B1:U43 B44:L49 M44:U69 K50:L69 B50:J72 K70:U72 B74:D74 G74:U74 D74:J83 B75:C81 M75:U81 K75:L83 B80:D80 G80:U80 B82:U83 D84:L87 B84:C94 M84:U94 B88:U113 B114:C119 L114:L119 M114:U131 D116:J119 K117:K119 B120:L122 B123:J131 B132:U134 B135:J136 M135:U136 K136:L136">
+    <cfRule type="containsBlanks" dxfId="4" priority="19">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73:U73">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B73))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114:K116 K131:K135">
-    <cfRule type="containsBlanks" dxfId="3" priority="71">
+    <cfRule type="containsBlanks" dxfId="2" priority="71">
       <formula>LEN(TRIM(D114))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K123:L130">
-    <cfRule type="containsBlanks" dxfId="2" priority="5">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(K123))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L131:L134">
-    <cfRule type="containsBlanks" dxfId="1" priority="9">
+    <cfRule type="containsBlanks" dxfId="0" priority="9">
       <formula>LEN(TRIM(L131))=0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B72 B1:B6 B74:B136">
-    <cfRule type="duplicateValues" dxfId="0" priority="136"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
updated report page 1
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3511" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{939A0A60-FEA3-41AD-8AA6-EE19F3E5FBC6}"/>
+  <xr:revisionPtr revIDLastSave="3559" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E16CB73C-CCBC-46DC-8F7F-B1F795D1AB44}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4067" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4068" uniqueCount="1574">
   <si>
     <t>name</t>
   </si>
@@ -4853,9 +4853,6 @@
     <t>Old English</t>
   </si>
   <si>
-    <t>configuration/assets/cover_background - sage - base box.svg</t>
-  </si>
-  <si>
     <t>Policy indicators for healthy and sustainable cities</t>
   </si>
   <si>
@@ -4869,6 +4866,12 @@
   </si>
   <si>
     <t>configuration/assets/GOHSC - colour logo transparent.svg</t>
+  </si>
+  <si>
+    <t>configuration/assets/cover_background - fawn - base box.svg</t>
+  </si>
+  <si>
+    <t>Preliminary findings are not intended for public release until results and interpretations are validated and approved.</t>
   </si>
 </sst>
 </file>
@@ -5951,7 +5954,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6036,14 +6039,14 @@
         <v>28</v>
       </c>
       <c r="E2">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F2">
         <v>200</v>
       </c>
       <c r="G2">
         <f>E2+8</f>
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
         <v>111</v>
@@ -6097,14 +6100,14 @@
       </c>
       <c r="E3">
         <f>G2+3</f>
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F3">
         <v>200</v>
       </c>
       <c r="G3">
         <f>E3+8</f>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H3" t="s">
         <v>111</v>
@@ -6339,7 +6342,7 @@
       </c>
       <c r="E7">
         <f>G3+5</f>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F7">
         <f>F2</f>
@@ -6347,7 +6350,7 @@
       </c>
       <c r="G7">
         <f>E7+8</f>
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H7" t="s">
         <v>111</v>
@@ -6401,14 +6404,14 @@
       </c>
       <c r="E8">
         <f>G7</f>
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F8">
         <v>200</v>
       </c>
       <c r="G8">
         <f>E8+6</f>
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H8" t="s">
         <v>111</v>
@@ -6462,20 +6465,20 @@
       </c>
       <c r="E9">
         <f>G8</f>
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F9">
         <v>200</v>
       </c>
       <c r="G9">
         <f>E9+6</f>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
         <v>111</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -6519,32 +6522,35 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E10">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="F10">
         <v>200</v>
       </c>
       <c r="G10">
-        <f>E10+10</f>
-        <v>27</v>
+        <f>E10+6</f>
+        <v>173</v>
       </c>
       <c r="H10" t="s">
         <v>111</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1544</v>
       </c>
       <c r="N10" t="s">
         <v>21</v>
@@ -6607,7 +6613,7 @@
         <v>25</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
@@ -6714,13 +6720,13 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O13" t="s">
         <v>22</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" t="b">
         <v>1</v>
@@ -6773,10 +6779,10 @@
         <v>25</v>
       </c>
       <c r="P14" t="s">
-        <v>1567</v>
+        <v>1572</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -6799,18 +6805,18 @@
         <v>24</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E15">
-        <v>159</v>
+        <v>15</v>
       </c>
       <c r="F15">
         <f>D15+106</f>
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="G15">
         <f>E15+30</f>
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -6831,10 +6837,10 @@
         <v>27</v>
       </c>
       <c r="P15" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R15" t="b">
         <v>1</v>
@@ -27908,7 +27914,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28256,7 +28262,7 @@
         <v>231</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1530</v>
@@ -28288,7 +28294,7 @@
         <v>1515</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>1551</v>
@@ -28320,7 +28326,7 @@
         <v>1516</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>1552</v>
@@ -28352,7 +28358,7 @@
         <v>1517</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>1553</v>
@@ -28384,7 +28390,7 @@
         <v>1550</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1306</v>
+        <v>1573</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>1306</v>
@@ -34735,14 +34741,14 @@
   <conditionalFormatting sqref="B73">
     <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N44:V69 L50:M69 L70:V72 H74:V74 E74:K83 N75:V81 L75:M83 H80:V80 E84:M87 N84:V94 M114:M119 N114:V131 E116:K119 L117:L119 N135:V136 L136:M136 D135:K136 D132:V134 D123:K131 D120:M122 D114:D119 D88:V113 D84:D94 D82:V83 D80:E80 D75:D81 D74:E74 D50:K72 D44:M49 D1:V43 B1:C72 B74:C136">
-    <cfRule type="containsBlanks" dxfId="4" priority="19">
-      <formula>LEN(TRIM(B1))=0</formula>
+  <conditionalFormatting sqref="B73:V73">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
+      <formula>LEN(TRIM(B73))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:V73">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(B73))=0</formula>
+  <conditionalFormatting sqref="D1:V43 B1:C72 D44:M49 N44:V69 L50:M69 D50:K72 L70:V72 D74:E74 H74:V74 E74:K83 B74:C136 D75:D81 N75:V81 L75:M83 D80:E80 H80:V80 D82:V83 E84:M87 D84:D94 N84:V94 D88:V113 D114:D119 M114:M119 N114:V131 E116:K119 L117:L119 D120:M122 D123:K131 D132:V134 D135:K136 N135:V136 L136:M136">
+    <cfRule type="containsBlanks" dxfId="3" priority="19">
+      <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E114:L116 L131:L135">

</xml_diff>

<commit_message>
sketched in page 3 of new report design
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3693" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CB406E7-B535-462D-85F0-B4F8FFDF92C9}"/>
+  <xr:revisionPtr revIDLastSave="3800" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA55E127-A042-4366-B08B-EB1B8F92B18B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4120" uniqueCount="1585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1586">
   <si>
     <t>name</t>
   </si>
@@ -4905,6 +4905,9 @@
   </si>
   <si>
     <t>Add author names by editing region configuration reporting settings using a text editor</t>
+  </si>
+  <si>
+    <t>Example report only.  Copy and edit the example .yml file in the configuration/regions folder to define your own study region for analysis and reporting.  Following configuration and analysis, policy and/or spatial indicator reports may be generated according to the directions at</t>
   </si>
 </sst>
 </file>
@@ -5983,16 +5986,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T293"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6136,6 +6139,7 @@
         <v>136</v>
       </c>
       <c r="F3">
+        <f>$F$2</f>
         <v>200</v>
       </c>
       <c r="G3">
@@ -6193,10 +6197,11 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>204</v>
+        <f t="shared" ref="F4:F14" si="0">$F$2</f>
+        <v>200</v>
       </c>
       <c r="G4">
         <v>8</v>
@@ -6255,10 +6260,11 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -6314,14 +6320,15 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G6">
         <f>E6+3</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
         <v>111</v>
@@ -6374,14 +6381,15 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G7">
         <f>E7+3</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
         <v>111</v>
@@ -6434,14 +6442,15 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G8">
         <f>E8+3</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
         <v>111</v>
@@ -6494,14 +6503,15 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G9">
         <f>E9+3</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
         <v>111</v>
@@ -6554,14 +6564,15 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="G10">
         <f>E10+3</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
         <v>111</v>
@@ -6618,7 +6629,7 @@
         <v>149</v>
       </c>
       <c r="F11">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="G11">
@@ -6680,6 +6691,7 @@
         <v>157</v>
       </c>
       <c r="F12">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="G12">
@@ -6741,6 +6753,7 @@
         <v>163</v>
       </c>
       <c r="F13">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="G13">
@@ -6801,6 +6814,7 @@
         <v>171</v>
       </c>
       <c r="F14">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="G14">
@@ -7136,13 +7150,13 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>14</v>
       </c>
       <c r="F20">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G20">
         <f>E20+6</f>
@@ -7196,17 +7210,19 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>14</v>
+        <f>$D$20</f>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F21">
-        <v>190</v>
+        <f>$F$20</f>
+        <v>196</v>
       </c>
       <c r="G21">
         <f>E21+4</f>
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H21" t="s">
         <v>111</v>
@@ -7256,18 +7272,20 @@
         <v>19</v>
       </c>
       <c r="D22">
-        <v>14</v>
+        <f t="shared" ref="D22:D28" si="1">$D$20</f>
+        <v>10</v>
       </c>
       <c r="E22">
         <f>G21+4</f>
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="F22">
-        <v>190</v>
+        <f t="shared" ref="F22:F28" si="2">$F$20</f>
+        <v>196</v>
       </c>
       <c r="G22">
         <f>E22+4</f>
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="H22" t="s">
         <v>111</v>
@@ -7315,18 +7333,20 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E23">
         <f>G22+2</f>
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="F23">
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23" si="0">E23+4</f>
-        <v>142</v>
+        <f t="shared" ref="G23" si="3">E23+4</f>
+        <v>153</v>
       </c>
       <c r="H23" t="s">
         <v>111</v>
@@ -7374,19 +7394,20 @@
         <v>19</v>
       </c>
       <c r="D24">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E24">
-        <f>G23+8</f>
-        <v>150</v>
+        <f>E23+20</f>
+        <v>169</v>
       </c>
       <c r="F24">
-        <f>F26</f>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24" si="1">E24+4</f>
-        <v>154</v>
+        <f t="shared" ref="G24" si="4">E24+4</f>
+        <v>173</v>
       </c>
       <c r="H24" t="s">
         <v>111</v>
@@ -7431,19 +7452,20 @@
         <v>19</v>
       </c>
       <c r="D25">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E25">
         <f>G24+2</f>
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="F25">
-        <f>F24</f>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25" si="2">E25+4</f>
-        <v>160</v>
+        <f t="shared" ref="G25" si="5">E25+4</f>
+        <v>179</v>
       </c>
       <c r="H25" t="s">
         <v>111</v>
@@ -7481,7 +7503,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>983</v>
+        <v>570</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -7490,19 +7512,20 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E26">
-        <f>G28+5</f>
-        <v>183</v>
+        <f>E25+20</f>
+        <v>195</v>
       </c>
       <c r="F26">
-        <f>F28</f>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G26">
         <f>E26+4</f>
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="H26" t="s">
         <v>111</v>
@@ -7511,7 +7534,7 @@
         <v>12</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -7541,7 +7564,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>570</v>
+        <v>551</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -7550,19 +7573,20 @@
         <v>19</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E27">
-        <f>G25+8</f>
-        <v>168</v>
+        <f>G26+2</f>
+        <v>201</v>
       </c>
       <c r="F27">
-        <f>F23</f>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G27">
-        <f>E27+4</f>
-        <v>172</v>
+        <f t="shared" ref="G27" si="6">E27+4</f>
+        <v>205</v>
       </c>
       <c r="H27" t="s">
         <v>111</v>
@@ -7571,7 +7595,7 @@
         <v>12</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -7601,7 +7625,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>551</v>
+        <v>983</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -7610,19 +7634,20 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E28">
-        <f>G27+2</f>
-        <v>174</v>
+        <f>G27+5</f>
+        <v>210</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28" si="3">F27</f>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>196</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28" si="4">E28+4</f>
-        <v>178</v>
+        <f>E28+4</f>
+        <v>214</v>
       </c>
       <c r="H28" t="s">
         <v>111</v>
@@ -7670,7 +7695,7 @@
         <v>24</v>
       </c>
       <c r="D29">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -7779,7 +7804,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>1515</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -7788,18 +7813,17 @@
         <v>19</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E31">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F31">
-        <f>F33-1</f>
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="G31">
         <f>E31+5</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H31" t="s">
         <v>111</v>
@@ -7846,19 +7870,20 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <f>$D$31</f>
+        <v>14</v>
       </c>
       <c r="E32">
-        <f>G31+7</f>
-        <v>24</v>
+        <f>G31+8</f>
+        <v>33</v>
       </c>
       <c r="F32">
-        <f>D37-3</f>
-        <v>131</v>
+        <f>$F$31</f>
+        <v>200</v>
       </c>
       <c r="G32">
-        <f>E32+5</f>
-        <v>29</v>
+        <f>E32+6</f>
+        <v>39</v>
       </c>
       <c r="H32" t="s">
         <v>111</v>
@@ -7905,20 +7930,20 @@
         <v>19</v>
       </c>
       <c r="D33">
-        <f>D32</f>
-        <v>10</v>
+        <f>$D$31</f>
+        <v>14</v>
       </c>
       <c r="E33">
         <f>E32+28</f>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F33">
-        <f>F32</f>
-        <v>131</v>
+        <f>$F$31</f>
+        <v>200</v>
       </c>
       <c r="G33">
         <f>E33+4</f>
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H33" t="s">
         <v>111</v>
@@ -7959,19 +7984,21 @@
         <v>149</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <f>$D$31</f>
+        <v>14</v>
       </c>
       <c r="E34">
         <v>100</v>
       </c>
       <c r="F34">
-        <v>131</v>
+        <f>$F$31</f>
+        <v>200</v>
       </c>
       <c r="G34">
         <f>E34+5</f>
@@ -8016,22 +8043,22 @@
         <v>106</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
       </c>
       <c r="D35">
-        <f>D34</f>
-        <v>10</v>
+        <f>$D$31</f>
+        <v>14</v>
       </c>
       <c r="E35">
         <f>G34+2</f>
         <v>107</v>
       </c>
       <c r="F35">
-        <f>F34</f>
-        <v>131</v>
+        <f>$F$31</f>
+        <v>200</v>
       </c>
       <c r="G35">
         <f>E35+5</f>
@@ -8082,18 +8109,19 @@
         <v>24</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <f>$D$31</f>
+        <v>14</v>
       </c>
       <c r="E36">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F36">
-        <f>D36+170</f>
-        <v>190</v>
+        <f>D36+182</f>
+        <v>196</v>
       </c>
       <c r="G36">
         <f>E36+INT(144*(F36-D36)/192)</f>
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -8131,23 +8159,24 @@
         <v>1288</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
       </c>
       <c r="D37">
-        <v>134</v>
+        <f>$D$31-1</f>
+        <v>13</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="F37">
         <v>210</v>
       </c>
       <c r="G37">
         <f>E36-5</f>
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -8161,11 +8190,8 @@
       <c r="L37">
         <v>0</v>
       </c>
-      <c r="M37" t="s">
-        <v>1094</v>
-      </c>
       <c r="N37" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O37" t="s">
         <v>25</v>
@@ -8195,25 +8221,25 @@
       </c>
       <c r="D38">
         <f>$D$37+1</f>
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="E38">
         <f>E37+4</f>
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="F38">
-        <f>D38+74</f>
-        <v>209</v>
+        <f t="shared" ref="F38:F51" si="7">$F$31</f>
+        <v>200</v>
       </c>
       <c r="G38">
-        <f>E38+3</f>
-        <v>19</v>
+        <f>E38+6</f>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
         <v>111</v>
       </c>
       <c r="I38">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -8225,7 +8251,7 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O38" t="s">
         <v>25</v>
@@ -8255,40 +8281,40 @@
       </c>
       <c r="D39">
         <f>$D$38</f>
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="E39">
-        <f>G38+1</f>
-        <v>20</v>
+        <f>G38+4</f>
+        <v>99</v>
       </c>
       <c r="F39">
-        <f>D39+74</f>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G39">
-        <f>E39+4</f>
-        <v>24</v>
+        <f>E39+6</f>
+        <v>105</v>
       </c>
       <c r="H39" t="s">
         <v>111</v>
       </c>
       <c r="I39">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J39">
         <v>0</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O39" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -8308,26 +8334,26 @@
         <v>1294</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D51" si="5">$D$38</f>
-        <v>135</v>
+        <f t="shared" ref="D40:D51" si="8">$D$38</f>
+        <v>14</v>
       </c>
       <c r="E40">
         <f>G39+12</f>
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="F40">
-        <f t="shared" ref="F40:F51" si="6">F38</f>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G40">
         <f>E40+3</f>
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="H40" t="s">
         <v>111</v>
@@ -8345,7 +8371,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O40" t="s">
         <v>25</v>
@@ -8368,26 +8394,26 @@
         <v>1295</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C41" t="s">
         <v>19</v>
       </c>
       <c r="D41">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E41">
         <f>G40+1</f>
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="F41">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G41">
         <f>E41+4</f>
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="H41" t="s">
         <v>111</v>
@@ -8405,7 +8431,7 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O41" t="s">
         <v>25</v>
@@ -8428,26 +8454,26 @@
         <v>1296</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C42" t="s">
         <v>19</v>
       </c>
       <c r="D42">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E42">
         <f>G41+12</f>
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="F42">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G42">
         <f>E42+3</f>
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="H42" t="s">
         <v>111</v>
@@ -8465,7 +8491,7 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O42" t="s">
         <v>25</v>
@@ -8488,26 +8514,26 @@
         <v>1297</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
       <c r="D43">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E43">
         <f>G42+1</f>
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="F43">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G43">
         <f>E43+4</f>
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="H43" t="s">
         <v>111</v>
@@ -8525,7 +8551,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O43" t="s">
         <v>25</v>
@@ -8548,26 +8574,26 @@
         <v>1298</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
       <c r="D44">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E44">
         <f>G43+12</f>
-        <v>76</v>
+        <v>157</v>
       </c>
       <c r="F44">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G44">
         <f>E44+3</f>
-        <v>79</v>
+        <v>160</v>
       </c>
       <c r="H44" t="s">
         <v>111</v>
@@ -8585,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O44" t="s">
         <v>25</v>
@@ -8608,26 +8634,26 @@
         <v>1299</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
       </c>
       <c r="D45">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E45">
         <f>G44+1</f>
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="F45">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G45">
         <f>E45+4</f>
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="H45" t="s">
         <v>111</v>
@@ -8645,7 +8671,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O45" t="s">
         <v>25</v>
@@ -8668,26 +8694,26 @@
         <v>1300</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
       <c r="D46">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E46">
         <f>G45+12</f>
-        <v>96</v>
+        <v>177</v>
       </c>
       <c r="F46">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G46">
         <f>E46+3</f>
-        <v>99</v>
+        <v>180</v>
       </c>
       <c r="H46" t="s">
         <v>111</v>
@@ -8705,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O46" t="s">
         <v>25</v>
@@ -8728,26 +8754,26 @@
         <v>1301</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
       </c>
       <c r="D47">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E47">
         <f>G46+1</f>
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="F47">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G47">
         <f>E47+4</f>
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="H47" t="s">
         <v>111</v>
@@ -8765,7 +8791,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O47" t="s">
         <v>25</v>
@@ -8788,26 +8814,26 @@
         <v>1302</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
       </c>
       <c r="D48">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E48">
         <f>G47+12</f>
-        <v>116</v>
+        <v>197</v>
       </c>
       <c r="F48">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G48">
         <f>E48+3</f>
-        <v>119</v>
+        <v>200</v>
       </c>
       <c r="H48" t="s">
         <v>111</v>
@@ -8825,7 +8851,7 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O48" t="s">
         <v>25</v>
@@ -8848,26 +8874,26 @@
         <v>1303</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E49">
         <f>G48+1</f>
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="F49">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G49">
         <f>E49+4</f>
-        <v>124</v>
+        <v>205</v>
       </c>
       <c r="H49" t="s">
         <v>111</v>
@@ -8885,7 +8911,7 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O49" t="s">
         <v>25</v>
@@ -8908,26 +8934,26 @@
         <v>1304</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="D50">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E50">
         <f>G49+12</f>
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="F50">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G50">
         <f>E50+3</f>
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="H50" t="s">
         <v>111</v>
@@ -8945,7 +8971,7 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O50" t="s">
         <v>25</v>
@@ -8968,26 +8994,26 @@
         <v>1305</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="C51" t="s">
         <v>19</v>
       </c>
       <c r="D51">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="E51">
         <f>G50+1</f>
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="F51">
-        <f t="shared" si="6"/>
-        <v>209</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="G51">
         <f>E51+4</f>
-        <v>144</v>
+        <v>225</v>
       </c>
       <c r="H51" t="s">
         <v>111</v>
@@ -9005,7 +9031,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>1094</v>
+        <v>21</v>
       </c>
       <c r="O51" t="s">
         <v>25</v>
@@ -10021,7 +10047,7 @@
         <v>19</v>
       </c>
       <c r="D69">
-        <f t="shared" ref="D69" si="7">D72-1</f>
+        <f t="shared" ref="D69" si="9">D72-1</f>
         <v>130</v>
       </c>
       <c r="E69">
@@ -10085,7 +10111,7 @@
         <v>155</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:E74" si="8">E69</f>
+        <f t="shared" ref="E70:E74" si="10">E69</f>
         <v>212</v>
       </c>
       <c r="F70">
@@ -10145,7 +10171,7 @@
         <v>181</v>
       </c>
       <c r="E71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>212</v>
       </c>
       <c r="F71">
@@ -10153,7 +10179,7 @@
         <v>207</v>
       </c>
       <c r="G71">
-        <f t="shared" ref="G71" si="9">G70</f>
+        <f t="shared" ref="G71" si="11">G70</f>
         <v>217</v>
       </c>
       <c r="H71" t="s">
@@ -10262,11 +10288,11 @@
         <v>156</v>
       </c>
       <c r="E73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>212</v>
       </c>
       <c r="F73">
-        <f t="shared" ref="F73:F74" si="10">D73</f>
+        <f t="shared" ref="F73:F74" si="12">D73</f>
         <v>156</v>
       </c>
       <c r="G73">
@@ -10319,11 +10345,11 @@
         <v>181</v>
       </c>
       <c r="E74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>212</v>
       </c>
       <c r="F74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>181</v>
       </c>
       <c r="G74">
@@ -10501,7 +10527,7 @@
         <v>155</v>
       </c>
       <c r="G77">
-        <f t="shared" ref="G77:G103" si="11">E77+3</f>
+        <f t="shared" ref="G77:G103" si="13">E77+3</f>
         <v>234</v>
       </c>
       <c r="H77" t="s">
@@ -10561,7 +10587,7 @@
         <v>182</v>
       </c>
       <c r="G78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="H78" t="s">
@@ -10621,7 +10647,7 @@
         <v>207</v>
       </c>
       <c r="G79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="H79" t="s">
@@ -10669,7 +10695,7 @@
         <v>19</v>
       </c>
       <c r="D80">
-        <f t="shared" ref="D80:D103" si="12">D76</f>
+        <f t="shared" ref="D80:D103" si="14">D76</f>
         <v>10</v>
       </c>
       <c r="E80">
@@ -10677,7 +10703,7 @@
         <v>243</v>
       </c>
       <c r="F80">
-        <f t="shared" ref="F80:F103" si="13">F76</f>
+        <f t="shared" ref="F80:F103" si="15">F76</f>
         <v>129</v>
       </c>
       <c r="G80">
@@ -10729,7 +10755,7 @@
         <v>19</v>
       </c>
       <c r="D81">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E81">
@@ -10737,7 +10763,7 @@
         <v>244</v>
       </c>
       <c r="F81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>155</v>
       </c>
       <c r="G81">
@@ -10789,7 +10815,7 @@
         <v>19</v>
       </c>
       <c r="D82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E82">
@@ -10797,11 +10823,11 @@
         <v>244</v>
       </c>
       <c r="F82">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G82">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G82">
-        <f t="shared" si="11"/>
         <v>247</v>
       </c>
       <c r="H82" t="s">
@@ -10849,7 +10875,7 @@
         <v>19</v>
       </c>
       <c r="D83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E83">
@@ -10857,11 +10883,11 @@
         <v>244</v>
       </c>
       <c r="F83">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G83">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G83">
-        <f t="shared" si="11"/>
         <v>247</v>
       </c>
       <c r="H83" t="s">
@@ -10909,7 +10935,7 @@
         <v>19</v>
       </c>
       <c r="D84">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E84">
@@ -10917,7 +10943,7 @@
         <v>256</v>
       </c>
       <c r="F84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="G84">
@@ -10969,7 +10995,7 @@
         <v>19</v>
       </c>
       <c r="D85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E85">
@@ -10977,11 +11003,11 @@
         <v>257</v>
       </c>
       <c r="F85">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="G85">
         <f t="shared" si="13"/>
-        <v>155</v>
-      </c>
-      <c r="G85">
-        <f t="shared" si="11"/>
         <v>260</v>
       </c>
       <c r="H85" t="s">
@@ -11029,7 +11055,7 @@
         <v>19</v>
       </c>
       <c r="D86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E86">
@@ -11037,11 +11063,11 @@
         <v>257</v>
       </c>
       <c r="F86">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G86">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G86">
-        <f t="shared" si="11"/>
         <v>260</v>
       </c>
       <c r="H86" t="s">
@@ -11089,7 +11115,7 @@
         <v>19</v>
       </c>
       <c r="D87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E87">
@@ -11097,11 +11123,11 @@
         <v>257</v>
       </c>
       <c r="F87">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G87">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="11"/>
         <v>260</v>
       </c>
       <c r="H87" t="s">
@@ -11149,7 +11175,7 @@
         <v>19</v>
       </c>
       <c r="D88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E88">
@@ -11157,7 +11183,7 @@
         <v>269</v>
       </c>
       <c r="F88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="G88">
@@ -11209,7 +11235,7 @@
         <v>19</v>
       </c>
       <c r="D89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E89">
@@ -11217,11 +11243,11 @@
         <v>270</v>
       </c>
       <c r="F89">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="G89">
         <f t="shared" si="13"/>
-        <v>155</v>
-      </c>
-      <c r="G89">
-        <f t="shared" si="11"/>
         <v>273</v>
       </c>
       <c r="H89" t="s">
@@ -11269,7 +11295,7 @@
         <v>19</v>
       </c>
       <c r="D90">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E90">
@@ -11277,11 +11303,11 @@
         <v>270</v>
       </c>
       <c r="F90">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G90">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G90">
-        <f t="shared" si="11"/>
         <v>273</v>
       </c>
       <c r="H90" t="s">
@@ -11329,7 +11355,7 @@
         <v>19</v>
       </c>
       <c r="D91">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E91">
@@ -11337,11 +11363,11 @@
         <v>270</v>
       </c>
       <c r="F91">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G91">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="11"/>
         <v>273</v>
       </c>
       <c r="H91" t="s">
@@ -11389,7 +11415,7 @@
         <v>19</v>
       </c>
       <c r="D92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E92">
@@ -11397,7 +11423,7 @@
         <v>282</v>
       </c>
       <c r="F92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="G92">
@@ -11449,7 +11475,7 @@
         <v>19</v>
       </c>
       <c r="D93">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E93">
@@ -11457,11 +11483,11 @@
         <v>283</v>
       </c>
       <c r="F93">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="G93">
         <f t="shared" si="13"/>
-        <v>155</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="11"/>
         <v>286</v>
       </c>
       <c r="H93" t="s">
@@ -11509,7 +11535,7 @@
         <v>19</v>
       </c>
       <c r="D94">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E94">
@@ -11517,11 +11543,11 @@
         <v>283</v>
       </c>
       <c r="F94">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G94">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G94">
-        <f t="shared" si="11"/>
         <v>286</v>
       </c>
       <c r="H94" t="s">
@@ -11569,7 +11595,7 @@
         <v>19</v>
       </c>
       <c r="D95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E95">
@@ -11577,11 +11603,11 @@
         <v>283</v>
       </c>
       <c r="F95">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G95">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G95">
-        <f t="shared" si="11"/>
         <v>286</v>
       </c>
       <c r="H95" t="s">
@@ -11629,7 +11655,7 @@
         <v>19</v>
       </c>
       <c r="D96">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E96">
@@ -11637,7 +11663,7 @@
         <v>295</v>
       </c>
       <c r="F96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="G96">
@@ -11689,7 +11715,7 @@
         <v>19</v>
       </c>
       <c r="D97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E97">
@@ -11697,11 +11723,11 @@
         <v>296</v>
       </c>
       <c r="F97">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="G97">
         <f t="shared" si="13"/>
-        <v>155</v>
-      </c>
-      <c r="G97">
-        <f t="shared" si="11"/>
         <v>299</v>
       </c>
       <c r="H97" t="s">
@@ -11749,7 +11775,7 @@
         <v>19</v>
       </c>
       <c r="D98">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E98">
@@ -11757,11 +11783,11 @@
         <v>296</v>
       </c>
       <c r="F98">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G98">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G98">
-        <f t="shared" si="11"/>
         <v>299</v>
       </c>
       <c r="H98" t="s">
@@ -11809,7 +11835,7 @@
         <v>19</v>
       </c>
       <c r="D99">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E99">
@@ -11817,11 +11843,11 @@
         <v>296</v>
       </c>
       <c r="F99">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G99">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G99">
-        <f t="shared" si="11"/>
         <v>299</v>
       </c>
       <c r="H99" t="s">
@@ -11869,7 +11895,7 @@
         <v>19</v>
       </c>
       <c r="D100">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E100">
@@ -11877,7 +11903,7 @@
         <v>308</v>
       </c>
       <c r="F100">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="G100">
@@ -11929,7 +11955,7 @@
         <v>19</v>
       </c>
       <c r="D101">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130</v>
       </c>
       <c r="E101">
@@ -11937,11 +11963,11 @@
         <v>309</v>
       </c>
       <c r="F101">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="G101">
         <f t="shared" si="13"/>
-        <v>155</v>
-      </c>
-      <c r="G101">
-        <f t="shared" si="11"/>
         <v>312</v>
       </c>
       <c r="H101" t="s">
@@ -11989,7 +12015,7 @@
         <v>19</v>
       </c>
       <c r="D102">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>155</v>
       </c>
       <c r="E102">
@@ -11997,11 +12023,11 @@
         <v>309</v>
       </c>
       <c r="F102">
+        <f t="shared" si="15"/>
+        <v>182</v>
+      </c>
+      <c r="G102">
         <f t="shared" si="13"/>
-        <v>182</v>
-      </c>
-      <c r="G102">
-        <f t="shared" si="11"/>
         <v>312</v>
       </c>
       <c r="H102" t="s">
@@ -12049,7 +12075,7 @@
         <v>19</v>
       </c>
       <c r="D103">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>181</v>
       </c>
       <c r="E103">
@@ -12057,11 +12083,11 @@
         <v>309</v>
       </c>
       <c r="F103">
+        <f t="shared" si="15"/>
+        <v>207</v>
+      </c>
+      <c r="G103">
         <f t="shared" si="13"/>
-        <v>207</v>
-      </c>
-      <c r="G103">
-        <f t="shared" si="11"/>
         <v>312</v>
       </c>
       <c r="H103" t="s">
@@ -12693,7 +12719,7 @@
         <v>19</v>
       </c>
       <c r="D114">
-        <f t="shared" ref="D114" si="14">D117-1</f>
+        <f t="shared" ref="D114" si="16">D117-1</f>
         <v>59</v>
       </c>
       <c r="E114">
@@ -12757,7 +12783,7 @@
         <v>81</v>
       </c>
       <c r="E115">
-        <f t="shared" ref="E115:E119" si="15">E114</f>
+        <f t="shared" ref="E115:E119" si="17">E114</f>
         <v>23</v>
       </c>
       <c r="F115">
@@ -12817,7 +12843,7 @@
         <v>104</v>
       </c>
       <c r="E116">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>23</v>
       </c>
       <c r="F116">
@@ -12825,7 +12851,7 @@
         <v>125</v>
       </c>
       <c r="G116">
-        <f t="shared" ref="G116" si="16">G115</f>
+        <f t="shared" ref="G116" si="18">G115</f>
         <v>28</v>
       </c>
       <c r="H116" t="s">
@@ -12934,11 +12960,11 @@
         <v>82</v>
       </c>
       <c r="E118">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>23</v>
       </c>
       <c r="F118">
-        <f t="shared" ref="F118:F119" si="17">D118</f>
+        <f t="shared" ref="F118:F119" si="19">D118</f>
         <v>82</v>
       </c>
       <c r="G118">
@@ -12991,11 +13017,11 @@
         <v>104</v>
       </c>
       <c r="E119">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>23</v>
       </c>
       <c r="F119">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>104</v>
       </c>
       <c r="G119">
@@ -13172,7 +13198,7 @@
         <v>81</v>
       </c>
       <c r="G122">
-        <f t="shared" ref="G122:G124" si="18">E122+3</f>
+        <f t="shared" ref="G122:G124" si="20">E122+3</f>
         <v>45</v>
       </c>
       <c r="H122" t="s">
@@ -13232,7 +13258,7 @@
         <v>105</v>
       </c>
       <c r="G123">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>45</v>
       </c>
       <c r="H123" t="s">
@@ -13292,7 +13318,7 @@
         <v>125</v>
       </c>
       <c r="G124">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>45</v>
       </c>
       <c r="H124" t="s">
@@ -13340,7 +13366,7 @@
         <v>19</v>
       </c>
       <c r="D125">
-        <f t="shared" ref="D125:D156" si="19">D121</f>
+        <f t="shared" ref="D125:D156" si="21">D121</f>
         <v>10</v>
       </c>
       <c r="E125">
@@ -13348,7 +13374,7 @@
         <v>56</v>
       </c>
       <c r="F125">
-        <f t="shared" ref="F125:F156" si="20">F121</f>
+        <f t="shared" ref="F125:F156" si="22">F121</f>
         <v>58</v>
       </c>
       <c r="G125">
@@ -13400,7 +13426,7 @@
         <v>19</v>
       </c>
       <c r="D126">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E126">
@@ -13408,7 +13434,7 @@
         <v>57</v>
       </c>
       <c r="F126">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G126">
@@ -13460,7 +13486,7 @@
         <v>19</v>
       </c>
       <c r="D127">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E127">
@@ -13468,11 +13494,11 @@
         <v>57</v>
       </c>
       <c r="F127">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G127">
-        <f t="shared" ref="G127:G128" si="21">E127+3</f>
+        <f t="shared" ref="G127:G128" si="23">E127+3</f>
         <v>60</v>
       </c>
       <c r="H127" t="s">
@@ -13520,7 +13546,7 @@
         <v>19</v>
       </c>
       <c r="D128">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E128">
@@ -13528,11 +13554,11 @@
         <v>57</v>
       </c>
       <c r="F128">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G128">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>60</v>
       </c>
       <c r="H128" t="s">
@@ -13580,7 +13606,7 @@
         <v>19</v>
       </c>
       <c r="D129">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E129">
@@ -13588,7 +13614,7 @@
         <v>71</v>
       </c>
       <c r="F129">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G129">
@@ -13640,7 +13666,7 @@
         <v>19</v>
       </c>
       <c r="D130">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E130">
@@ -13648,11 +13674,11 @@
         <v>72</v>
       </c>
       <c r="F130">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G130">
-        <f t="shared" ref="G130:G132" si="22">E130+3</f>
+        <f t="shared" ref="G130:G132" si="24">E130+3</f>
         <v>75</v>
       </c>
       <c r="H130" t="s">
@@ -13700,7 +13726,7 @@
         <v>19</v>
       </c>
       <c r="D131">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E131">
@@ -13708,11 +13734,11 @@
         <v>72</v>
       </c>
       <c r="F131">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G131">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>75</v>
       </c>
       <c r="H131" t="s">
@@ -13760,7 +13786,7 @@
         <v>19</v>
       </c>
       <c r="D132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E132">
@@ -13768,11 +13794,11 @@
         <v>72</v>
       </c>
       <c r="F132">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>75</v>
       </c>
       <c r="H132" t="s">
@@ -13820,7 +13846,7 @@
         <v>19</v>
       </c>
       <c r="D133">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E133">
@@ -13828,7 +13854,7 @@
         <v>86</v>
       </c>
       <c r="F133">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G133">
@@ -13880,7 +13906,7 @@
         <v>19</v>
       </c>
       <c r="D134">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E134">
@@ -13888,11 +13914,11 @@
         <v>87</v>
       </c>
       <c r="F134">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G134">
-        <f t="shared" ref="G134:G136" si="23">E134+3</f>
+        <f t="shared" ref="G134:G136" si="25">E134+3</f>
         <v>90</v>
       </c>
       <c r="H134" t="s">
@@ -13940,7 +13966,7 @@
         <v>19</v>
       </c>
       <c r="D135">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E135">
@@ -13948,11 +13974,11 @@
         <v>87</v>
       </c>
       <c r="F135">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G135">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>90</v>
       </c>
       <c r="H135" t="s">
@@ -14000,7 +14026,7 @@
         <v>19</v>
       </c>
       <c r="D136">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E136">
@@ -14008,11 +14034,11 @@
         <v>87</v>
       </c>
       <c r="F136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G136">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>90</v>
       </c>
       <c r="H136" t="s">
@@ -14060,7 +14086,7 @@
         <v>19</v>
       </c>
       <c r="D137">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E137">
@@ -14068,7 +14094,7 @@
         <v>101</v>
       </c>
       <c r="F137">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G137">
@@ -14120,7 +14146,7 @@
         <v>19</v>
       </c>
       <c r="D138">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E138">
@@ -14128,11 +14154,11 @@
         <v>102</v>
       </c>
       <c r="F138">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G138">
-        <f t="shared" ref="G138:G140" si="24">E138+3</f>
+        <f t="shared" ref="G138:G140" si="26">E138+3</f>
         <v>105</v>
       </c>
       <c r="H138" t="s">
@@ -14180,7 +14206,7 @@
         <v>19</v>
       </c>
       <c r="D139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E139">
@@ -14188,11 +14214,11 @@
         <v>102</v>
       </c>
       <c r="F139">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G139">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>105</v>
       </c>
       <c r="H139" t="s">
@@ -14240,7 +14266,7 @@
         <v>19</v>
       </c>
       <c r="D140">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E140">
@@ -14248,11 +14274,11 @@
         <v>102</v>
       </c>
       <c r="F140">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G140">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>105</v>
       </c>
       <c r="H140" t="s">
@@ -14300,7 +14326,7 @@
         <v>19</v>
       </c>
       <c r="D141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E141">
@@ -14308,7 +14334,7 @@
         <v>116</v>
       </c>
       <c r="F141">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G141">
@@ -14360,7 +14386,7 @@
         <v>19</v>
       </c>
       <c r="D142">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E142">
@@ -14368,11 +14394,11 @@
         <v>117</v>
       </c>
       <c r="F142">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G142">
-        <f t="shared" ref="G142:G144" si="25">E142+3</f>
+        <f t="shared" ref="G142:G144" si="27">E142+3</f>
         <v>120</v>
       </c>
       <c r="H142" t="s">
@@ -14420,7 +14446,7 @@
         <v>19</v>
       </c>
       <c r="D143">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E143">
@@ -14428,11 +14454,11 @@
         <v>117</v>
       </c>
       <c r="F143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G143">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>120</v>
       </c>
       <c r="H143" t="s">
@@ -14480,7 +14506,7 @@
         <v>19</v>
       </c>
       <c r="D144">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E144">
@@ -14488,11 +14514,11 @@
         <v>117</v>
       </c>
       <c r="F144">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G144">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>120</v>
       </c>
       <c r="H144" t="s">
@@ -14540,7 +14566,7 @@
         <v>19</v>
       </c>
       <c r="D145">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E145">
@@ -14548,7 +14574,7 @@
         <v>131</v>
       </c>
       <c r="F145">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G145">
@@ -14600,7 +14626,7 @@
         <v>19</v>
       </c>
       <c r="D146">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E146">
@@ -14608,11 +14634,11 @@
         <v>132</v>
       </c>
       <c r="F146">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G146">
-        <f t="shared" ref="G146:G148" si="26">E146+3</f>
+        <f t="shared" ref="G146:G148" si="28">E146+3</f>
         <v>135</v>
       </c>
       <c r="H146" t="s">
@@ -14660,7 +14686,7 @@
         <v>19</v>
       </c>
       <c r="D147">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E147">
@@ -14668,11 +14694,11 @@
         <v>132</v>
       </c>
       <c r="F147">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>135</v>
       </c>
       <c r="H147" t="s">
@@ -14720,7 +14746,7 @@
         <v>19</v>
       </c>
       <c r="D148">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E148">
@@ -14728,11 +14754,11 @@
         <v>132</v>
       </c>
       <c r="F148">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G148">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>135</v>
       </c>
       <c r="H148" t="s">
@@ -14781,7 +14807,7 @@
         <v>19</v>
       </c>
       <c r="D149">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E149">
@@ -14789,7 +14815,7 @@
         <v>146</v>
       </c>
       <c r="F149">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G149">
@@ -14842,7 +14868,7 @@
         <v>19</v>
       </c>
       <c r="D150">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E150">
@@ -14850,11 +14876,11 @@
         <v>147</v>
       </c>
       <c r="F150">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G150">
-        <f t="shared" ref="G150:G152" si="27">E150+3</f>
+        <f t="shared" ref="G150:G152" si="29">E150+3</f>
         <v>150</v>
       </c>
       <c r="H150" t="s">
@@ -14903,7 +14929,7 @@
         <v>19</v>
       </c>
       <c r="D151">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E151">
@@ -14911,11 +14937,11 @@
         <v>147</v>
       </c>
       <c r="F151">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G151">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>150</v>
       </c>
       <c r="H151" t="s">
@@ -14964,7 +14990,7 @@
         <v>19</v>
       </c>
       <c r="D152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E152">
@@ -14972,11 +14998,11 @@
         <v>147</v>
       </c>
       <c r="F152">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G152">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>150</v>
       </c>
       <c r="H152" t="s">
@@ -15025,7 +15051,7 @@
         <v>19</v>
       </c>
       <c r="D153">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="E153">
@@ -15033,7 +15059,7 @@
         <v>161</v>
       </c>
       <c r="F153">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>58</v>
       </c>
       <c r="G153">
@@ -15086,7 +15112,7 @@
         <v>19</v>
       </c>
       <c r="D154">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>59</v>
       </c>
       <c r="E154">
@@ -15094,11 +15120,11 @@
         <v>162</v>
       </c>
       <c r="F154">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
       <c r="G154">
-        <f t="shared" ref="G154:G156" si="28">E154+3</f>
+        <f t="shared" ref="G154:G156" si="30">E154+3</f>
         <v>165</v>
       </c>
       <c r="H154" t="s">
@@ -15147,7 +15173,7 @@
         <v>19</v>
       </c>
       <c r="D155">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
       <c r="E155">
@@ -15155,11 +15181,11 @@
         <v>162</v>
       </c>
       <c r="F155">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>105</v>
       </c>
       <c r="G155">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>165</v>
       </c>
       <c r="H155" t="s">
@@ -15208,7 +15234,7 @@
         <v>19</v>
       </c>
       <c r="D156">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>104</v>
       </c>
       <c r="E156">
@@ -15216,11 +15242,11 @@
         <v>162</v>
       </c>
       <c r="F156">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>125</v>
       </c>
       <c r="G156">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>165</v>
       </c>
       <c r="H156" t="s">
@@ -15269,7 +15295,7 @@
         <v>19</v>
       </c>
       <c r="D157">
-        <f t="shared" ref="D157:D184" si="29">D153</f>
+        <f t="shared" ref="D157:D184" si="31">D153</f>
         <v>10</v>
       </c>
       <c r="E157">
@@ -15277,7 +15303,7 @@
         <v>176</v>
       </c>
       <c r="F157">
-        <f t="shared" ref="F157:F188" si="30">F153</f>
+        <f t="shared" ref="F157:F188" si="32">F153</f>
         <v>58</v>
       </c>
       <c r="G157">
@@ -15330,7 +15356,7 @@
         <v>19</v>
       </c>
       <c r="D158">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E158">
@@ -15338,11 +15364,11 @@
         <v>177</v>
       </c>
       <c r="F158">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G158">
-        <f t="shared" ref="G158:G160" si="31">E158+3</f>
+        <f t="shared" ref="G158:G160" si="33">E158+3</f>
         <v>180</v>
       </c>
       <c r="H158" t="s">
@@ -15391,7 +15417,7 @@
         <v>19</v>
       </c>
       <c r="D159">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E159">
@@ -15399,11 +15425,11 @@
         <v>177</v>
       </c>
       <c r="F159">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G159">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>180</v>
       </c>
       <c r="H159" t="s">
@@ -15452,7 +15478,7 @@
         <v>19</v>
       </c>
       <c r="D160">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E160">
@@ -15460,11 +15486,11 @@
         <v>177</v>
       </c>
       <c r="F160">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G160">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>180</v>
       </c>
       <c r="H160" t="s">
@@ -15513,7 +15539,7 @@
         <v>19</v>
       </c>
       <c r="D161">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E161">
@@ -15521,7 +15547,7 @@
         <v>191</v>
       </c>
       <c r="F161">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G161">
@@ -15574,7 +15600,7 @@
         <v>19</v>
       </c>
       <c r="D162">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E162">
@@ -15582,11 +15608,11 @@
         <v>192</v>
       </c>
       <c r="F162">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G162">
-        <f t="shared" ref="G162:G164" si="32">E162+3</f>
+        <f t="shared" ref="G162:G164" si="34">E162+3</f>
         <v>195</v>
       </c>
       <c r="H162" t="s">
@@ -15635,7 +15661,7 @@
         <v>19</v>
       </c>
       <c r="D163">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E163">
@@ -15643,11 +15669,11 @@
         <v>192</v>
       </c>
       <c r="F163">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G163">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>195</v>
       </c>
       <c r="H163" t="s">
@@ -15696,7 +15722,7 @@
         <v>19</v>
       </c>
       <c r="D164">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E164">
@@ -15704,11 +15730,11 @@
         <v>192</v>
       </c>
       <c r="F164">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G164">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>195</v>
       </c>
       <c r="H164" t="s">
@@ -15757,7 +15783,7 @@
         <v>19</v>
       </c>
       <c r="D165">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E165">
@@ -15765,7 +15791,7 @@
         <v>206</v>
       </c>
       <c r="F165">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G165">
@@ -15818,7 +15844,7 @@
         <v>19</v>
       </c>
       <c r="D166">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E166">
@@ -15826,11 +15852,11 @@
         <v>207</v>
       </c>
       <c r="F166">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G166">
-        <f t="shared" ref="G166:G168" si="33">E166+3</f>
+        <f t="shared" ref="G166:G168" si="35">E166+3</f>
         <v>210</v>
       </c>
       <c r="H166" t="s">
@@ -15879,7 +15905,7 @@
         <v>19</v>
       </c>
       <c r="D167">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E167">
@@ -15887,11 +15913,11 @@
         <v>207</v>
       </c>
       <c r="F167">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G167">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>210</v>
       </c>
       <c r="H167" t="s">
@@ -15940,7 +15966,7 @@
         <v>19</v>
       </c>
       <c r="D168">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E168">
@@ -15948,11 +15974,11 @@
         <v>207</v>
       </c>
       <c r="F168">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G168">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>210</v>
       </c>
       <c r="H168" t="s">
@@ -16001,7 +16027,7 @@
         <v>19</v>
       </c>
       <c r="D169">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E169">
@@ -16009,7 +16035,7 @@
         <v>221</v>
       </c>
       <c r="F169">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G169">
@@ -16062,7 +16088,7 @@
         <v>19</v>
       </c>
       <c r="D170">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E170">
@@ -16070,11 +16096,11 @@
         <v>222</v>
       </c>
       <c r="F170">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G170">
-        <f t="shared" ref="G170:G172" si="34">E170+3</f>
+        <f t="shared" ref="G170:G172" si="36">E170+3</f>
         <v>225</v>
       </c>
       <c r="H170" t="s">
@@ -16123,7 +16149,7 @@
         <v>19</v>
       </c>
       <c r="D171">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E171">
@@ -16131,11 +16157,11 @@
         <v>222</v>
       </c>
       <c r="F171">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G171">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>225</v>
       </c>
       <c r="H171" t="s">
@@ -16184,7 +16210,7 @@
         <v>19</v>
       </c>
       <c r="D172">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E172">
@@ -16192,11 +16218,11 @@
         <v>222</v>
       </c>
       <c r="F172">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G172">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>225</v>
       </c>
       <c r="H172" t="s">
@@ -16245,7 +16271,7 @@
         <v>19</v>
       </c>
       <c r="D173">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E173">
@@ -16253,7 +16279,7 @@
         <v>236</v>
       </c>
       <c r="F173">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G173">
@@ -16306,7 +16332,7 @@
         <v>19</v>
       </c>
       <c r="D174">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E174">
@@ -16314,11 +16340,11 @@
         <v>237</v>
       </c>
       <c r="F174">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G174">
-        <f t="shared" ref="G174:G176" si="35">E174+3</f>
+        <f t="shared" ref="G174:G176" si="37">E174+3</f>
         <v>240</v>
       </c>
       <c r="H174" t="s">
@@ -16367,7 +16393,7 @@
         <v>19</v>
       </c>
       <c r="D175">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E175">
@@ -16375,11 +16401,11 @@
         <v>237</v>
       </c>
       <c r="F175">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G175">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>240</v>
       </c>
       <c r="H175" t="s">
@@ -16428,7 +16454,7 @@
         <v>19</v>
       </c>
       <c r="D176">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E176">
@@ -16436,11 +16462,11 @@
         <v>237</v>
       </c>
       <c r="F176">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G176">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>240</v>
       </c>
       <c r="H176" t="s">
@@ -16489,7 +16515,7 @@
         <v>19</v>
       </c>
       <c r="D177">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E177">
@@ -16497,7 +16523,7 @@
         <v>251</v>
       </c>
       <c r="F177">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G177">
@@ -16550,7 +16576,7 @@
         <v>19</v>
       </c>
       <c r="D178">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E178">
@@ -16558,11 +16584,11 @@
         <v>252</v>
       </c>
       <c r="F178">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G178">
-        <f t="shared" ref="G178:G180" si="36">E178+3</f>
+        <f t="shared" ref="G178:G180" si="38">E178+3</f>
         <v>255</v>
       </c>
       <c r="H178" t="s">
@@ -16611,7 +16637,7 @@
         <v>19</v>
       </c>
       <c r="D179">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E179">
@@ -16619,11 +16645,11 @@
         <v>252</v>
       </c>
       <c r="F179">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G179">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>255</v>
       </c>
       <c r="H179" t="s">
@@ -16672,7 +16698,7 @@
         <v>19</v>
       </c>
       <c r="D180">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E180">
@@ -16680,11 +16706,11 @@
         <v>252</v>
       </c>
       <c r="F180">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G180">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>255</v>
       </c>
       <c r="H180" t="s">
@@ -16733,7 +16759,7 @@
         <v>19</v>
       </c>
       <c r="D181">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="E181">
@@ -16741,7 +16767,7 @@
         <v>266</v>
       </c>
       <c r="F181">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G181">
@@ -16794,7 +16820,7 @@
         <v>19</v>
       </c>
       <c r="D182">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>59</v>
       </c>
       <c r="E182">
@@ -16802,11 +16828,11 @@
         <v>267</v>
       </c>
       <c r="F182">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G182">
-        <f t="shared" ref="G182:G184" si="37">E182+3</f>
+        <f t="shared" ref="G182:G184" si="39">E182+3</f>
         <v>270</v>
       </c>
       <c r="H182" t="s">
@@ -16855,7 +16881,7 @@
         <v>19</v>
       </c>
       <c r="D183">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>81</v>
       </c>
       <c r="E183">
@@ -16863,11 +16889,11 @@
         <v>267</v>
       </c>
       <c r="F183">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G183">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>270</v>
       </c>
       <c r="H183" t="s">
@@ -16916,7 +16942,7 @@
         <v>19</v>
       </c>
       <c r="D184">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="E184">
@@ -16924,11 +16950,11 @@
         <v>267</v>
       </c>
       <c r="F184">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G184">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>270</v>
       </c>
       <c r="H184" t="s">
@@ -16977,7 +17003,7 @@
         <v>19</v>
       </c>
       <c r="D185">
-        <f t="shared" ref="D185" si="38">D181</f>
+        <f t="shared" ref="D185" si="40">D181</f>
         <v>10</v>
       </c>
       <c r="E185">
@@ -16985,7 +17011,7 @@
         <v>281</v>
       </c>
       <c r="F185">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="G185">
@@ -17046,11 +17072,11 @@
         <v>282</v>
       </c>
       <c r="F186">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>81</v>
       </c>
       <c r="G186">
-        <f t="shared" ref="G186:G188" si="39">E186+3</f>
+        <f t="shared" ref="G186:G188" si="41">E186+3</f>
         <v>285</v>
       </c>
       <c r="H186" t="s">
@@ -17107,11 +17133,11 @@
         <v>282</v>
       </c>
       <c r="F187">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>105</v>
       </c>
       <c r="G187">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>285</v>
       </c>
       <c r="H187" t="s">
@@ -17168,11 +17194,11 @@
         <v>282</v>
       </c>
       <c r="F188">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>125</v>
       </c>
       <c r="G188">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>285</v>
       </c>
       <c r="H188" t="s">
@@ -18279,7 +18305,7 @@
         <v>19</v>
       </c>
       <c r="D207">
-        <f t="shared" ref="D207" si="40">D210-1</f>
+        <f t="shared" ref="D207" si="42">D210-1</f>
         <v>146</v>
       </c>
       <c r="E207">
@@ -18343,7 +18369,7 @@
         <v>165</v>
       </c>
       <c r="E208">
-        <f t="shared" ref="E208:E212" si="41">E207</f>
+        <f t="shared" ref="E208:E212" si="43">E207</f>
         <v>92</v>
       </c>
       <c r="F208">
@@ -18403,7 +18429,7 @@
         <v>188</v>
       </c>
       <c r="E209">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>92</v>
       </c>
       <c r="F209">
@@ -18411,7 +18437,7 @@
         <v>209</v>
       </c>
       <c r="G209">
-        <f t="shared" ref="G209" si="42">G208</f>
+        <f t="shared" ref="G209" si="44">G208</f>
         <v>97</v>
       </c>
       <c r="H209" t="s">
@@ -18520,11 +18546,11 @@
         <v>166</v>
       </c>
       <c r="E211">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>92</v>
       </c>
       <c r="F211">
-        <f t="shared" ref="F211:F212" si="43">D211</f>
+        <f t="shared" ref="F211:F212" si="45">D211</f>
         <v>166</v>
       </c>
       <c r="G211">
@@ -18577,11 +18603,11 @@
         <v>188</v>
       </c>
       <c r="E212">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>92</v>
       </c>
       <c r="F212">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>188</v>
       </c>
       <c r="G212">
@@ -18758,7 +18784,7 @@
         <v>165</v>
       </c>
       <c r="G215">
-        <f t="shared" ref="G215:G217" si="44">E215+3</f>
+        <f t="shared" ref="G215:G217" si="46">E215+3</f>
         <v>114</v>
       </c>
       <c r="H215" t="s">
@@ -18818,7 +18844,7 @@
         <v>189</v>
       </c>
       <c r="G216">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>114</v>
       </c>
       <c r="H216" t="s">
@@ -18878,7 +18904,7 @@
         <v>209</v>
       </c>
       <c r="G217">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>114</v>
       </c>
       <c r="H217" t="s">
@@ -18997,7 +19023,7 @@
         <v>165</v>
       </c>
       <c r="G219">
-        <f t="shared" ref="G219:G221" si="45">E219+3</f>
+        <f t="shared" ref="G219:G221" si="47">E219+3</f>
         <v>132</v>
       </c>
       <c r="H219" t="s">
@@ -19057,7 +19083,7 @@
         <v>189</v>
       </c>
       <c r="G220">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>132</v>
       </c>
       <c r="H220" t="s">
@@ -19117,7 +19143,7 @@
         <v>209</v>
       </c>
       <c r="G221">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>132</v>
       </c>
       <c r="H221" t="s">
@@ -19236,7 +19262,7 @@
         <v>165</v>
       </c>
       <c r="G223">
-        <f t="shared" ref="G223:G225" si="46">E223+3</f>
+        <f t="shared" ref="G223:G225" si="48">E223+3</f>
         <v>150</v>
       </c>
       <c r="H223" t="s">
@@ -19296,7 +19322,7 @@
         <v>189</v>
       </c>
       <c r="G224">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>150</v>
       </c>
       <c r="H224" t="s">
@@ -19356,7 +19382,7 @@
         <v>209</v>
       </c>
       <c r="G225">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>150</v>
       </c>
       <c r="H225" t="s">
@@ -19414,7 +19440,7 @@
         <v>100</v>
       </c>
       <c r="G226">
-        <f t="shared" ref="G226" si="47">E226+3</f>
+        <f t="shared" ref="G226" si="49">E226+3</f>
         <v>163</v>
       </c>
       <c r="H226" t="s">
@@ -19757,7 +19783,7 @@
         <v>19</v>
       </c>
       <c r="D232">
-        <f t="shared" ref="D232" si="48">D235-1</f>
+        <f t="shared" ref="D232" si="50">D235-1</f>
         <v>146</v>
       </c>
       <c r="E232">
@@ -19821,7 +19847,7 @@
         <v>165</v>
       </c>
       <c r="E233">
-        <f t="shared" ref="E233:E237" si="49">E232</f>
+        <f t="shared" ref="E233:E237" si="51">E232</f>
         <v>233</v>
       </c>
       <c r="F233">
@@ -19881,7 +19907,7 @@
         <v>188</v>
       </c>
       <c r="E234">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>233</v>
       </c>
       <c r="F234">
@@ -19889,7 +19915,7 @@
         <v>209</v>
       </c>
       <c r="G234">
-        <f t="shared" ref="G234" si="50">G233</f>
+        <f t="shared" ref="G234" si="52">G233</f>
         <v>238</v>
       </c>
       <c r="H234" t="s">
@@ -19998,11 +20024,11 @@
         <v>166</v>
       </c>
       <c r="E236">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>233</v>
       </c>
       <c r="F236">
-        <f t="shared" ref="F236:F237" si="51">D236</f>
+        <f t="shared" ref="F236:F237" si="53">D236</f>
         <v>166</v>
       </c>
       <c r="G236">
@@ -20055,11 +20081,11 @@
         <v>188</v>
       </c>
       <c r="E237">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>233</v>
       </c>
       <c r="F237">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>188</v>
       </c>
       <c r="G237">
@@ -20236,7 +20262,7 @@
         <v>165</v>
       </c>
       <c r="G240">
-        <f t="shared" ref="G240:G242" si="52">E240+3</f>
+        <f t="shared" ref="G240:G242" si="54">E240+3</f>
         <v>255</v>
       </c>
       <c r="H240" t="s">
@@ -20296,7 +20322,7 @@
         <v>189</v>
       </c>
       <c r="G241">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>255</v>
       </c>
       <c r="H241" t="s">
@@ -20356,7 +20382,7 @@
         <v>209</v>
       </c>
       <c r="G242">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>255</v>
       </c>
       <c r="H242" t="s">
@@ -20633,7 +20659,7 @@
         <v>19</v>
       </c>
       <c r="D247">
-        <f t="shared" ref="D247" si="53">D250-1</f>
+        <f t="shared" ref="D247" si="55">D250-1</f>
         <v>136</v>
       </c>
       <c r="E247">
@@ -20697,7 +20723,7 @@
         <v>155</v>
       </c>
       <c r="E248">
-        <f t="shared" ref="E248:E249" si="54">E247</f>
+        <f t="shared" ref="E248:E249" si="56">E247</f>
         <v>21</v>
       </c>
       <c r="F248">
@@ -20757,7 +20783,7 @@
         <v>178</v>
       </c>
       <c r="E249">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>21</v>
       </c>
       <c r="F249">
@@ -20765,7 +20791,7 @@
         <v>199</v>
       </c>
       <c r="G249">
-        <f t="shared" ref="G249" si="55">G248</f>
+        <f t="shared" ref="G249" si="57">G248</f>
         <v>26</v>
       </c>
       <c r="H249" t="s">
@@ -20873,11 +20899,11 @@
         <v>156</v>
       </c>
       <c r="E251">
-        <f t="shared" ref="E251:E252" si="56">E250</f>
+        <f t="shared" ref="E251:E252" si="58">E250</f>
         <v>19</v>
       </c>
       <c r="F251">
-        <f t="shared" ref="F251:F252" si="57">D251</f>
+        <f t="shared" ref="F251:F252" si="59">D251</f>
         <v>156</v>
       </c>
       <c r="G251">
@@ -20930,11 +20956,11 @@
         <v>178</v>
       </c>
       <c r="E252">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>19</v>
       </c>
       <c r="F252">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>178</v>
       </c>
       <c r="G252">
@@ -21112,7 +21138,7 @@
         <v>155</v>
       </c>
       <c r="G255">
-        <f t="shared" ref="G255:G257" si="58">E255+3</f>
+        <f t="shared" ref="G255:G257" si="60">E255+3</f>
         <v>43</v>
       </c>
       <c r="H255" t="s">
@@ -21172,7 +21198,7 @@
         <v>179</v>
       </c>
       <c r="G256">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>43</v>
       </c>
       <c r="H256" t="s">
@@ -21232,7 +21258,7 @@
         <v>199</v>
       </c>
       <c r="G257">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>43</v>
       </c>
       <c r="H257" t="s">
@@ -21280,7 +21306,7 @@
         <v>19</v>
       </c>
       <c r="D258">
-        <f t="shared" ref="D258:D269" si="59">D254</f>
+        <f t="shared" ref="D258:D269" si="61">D254</f>
         <v>89</v>
       </c>
       <c r="E258">
@@ -21288,7 +21314,7 @@
         <v>54</v>
       </c>
       <c r="F258">
-        <f t="shared" ref="F258:F269" si="60">F254</f>
+        <f t="shared" ref="F258:F269" si="62">F254</f>
         <v>135</v>
       </c>
       <c r="G258">
@@ -21340,7 +21366,7 @@
         <v>19</v>
       </c>
       <c r="D259">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>136</v>
       </c>
       <c r="E259">
@@ -21348,7 +21374,7 @@
         <v>55</v>
       </c>
       <c r="F259">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>155</v>
       </c>
       <c r="G259">
@@ -21400,7 +21426,7 @@
         <v>19</v>
       </c>
       <c r="D260">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>155</v>
       </c>
       <c r="E260">
@@ -21408,11 +21434,11 @@
         <v>55</v>
       </c>
       <c r="F260">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>179</v>
       </c>
       <c r="G260">
-        <f t="shared" ref="G260:G261" si="61">E260+3</f>
+        <f t="shared" ref="G260:G261" si="63">E260+3</f>
         <v>58</v>
       </c>
       <c r="H260" t="s">
@@ -21460,7 +21486,7 @@
         <v>19</v>
       </c>
       <c r="D261">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>178</v>
       </c>
       <c r="E261">
@@ -21468,11 +21494,11 @@
         <v>55</v>
       </c>
       <c r="F261">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>199</v>
       </c>
       <c r="G261">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>58</v>
       </c>
       <c r="H261" t="s">
@@ -21520,7 +21546,7 @@
         <v>19</v>
       </c>
       <c r="D262">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>89</v>
       </c>
       <c r="E262">
@@ -21528,7 +21554,7 @@
         <v>69</v>
       </c>
       <c r="F262">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>135</v>
       </c>
       <c r="G262">
@@ -21580,7 +21606,7 @@
         <v>19</v>
       </c>
       <c r="D263">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>136</v>
       </c>
       <c r="E263">
@@ -21588,11 +21614,11 @@
         <v>70</v>
       </c>
       <c r="F263">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>155</v>
       </c>
       <c r="G263">
-        <f t="shared" ref="G263:G265" si="62">E263+3</f>
+        <f t="shared" ref="G263:G265" si="64">E263+3</f>
         <v>73</v>
       </c>
       <c r="H263" t="s">
@@ -21640,7 +21666,7 @@
         <v>19</v>
       </c>
       <c r="D264">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>155</v>
       </c>
       <c r="E264">
@@ -21648,11 +21674,11 @@
         <v>70</v>
       </c>
       <c r="F264">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>179</v>
       </c>
       <c r="G264">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>73</v>
       </c>
       <c r="H264" t="s">
@@ -21700,7 +21726,7 @@
         <v>19</v>
       </c>
       <c r="D265">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>178</v>
       </c>
       <c r="E265">
@@ -21708,11 +21734,11 @@
         <v>70</v>
       </c>
       <c r="F265">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>199</v>
       </c>
       <c r="G265">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>73</v>
       </c>
       <c r="H265" t="s">
@@ -21760,7 +21786,7 @@
         <v>19</v>
       </c>
       <c r="D266">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>89</v>
       </c>
       <c r="E266">
@@ -21768,7 +21794,7 @@
         <v>84</v>
       </c>
       <c r="F266">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>135</v>
       </c>
       <c r="G266">
@@ -21820,7 +21846,7 @@
         <v>19</v>
       </c>
       <c r="D267">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>136</v>
       </c>
       <c r="E267">
@@ -21828,11 +21854,11 @@
         <v>85</v>
       </c>
       <c r="F267">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>155</v>
       </c>
       <c r="G267">
-        <f t="shared" ref="G267:G269" si="63">E267+3</f>
+        <f t="shared" ref="G267:G269" si="65">E267+3</f>
         <v>88</v>
       </c>
       <c r="H267" t="s">
@@ -21880,7 +21906,7 @@
         <v>19</v>
       </c>
       <c r="D268">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>155</v>
       </c>
       <c r="E268">
@@ -21888,11 +21914,11 @@
         <v>85</v>
       </c>
       <c r="F268">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>179</v>
       </c>
       <c r="G268">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>88</v>
       </c>
       <c r="H268" t="s">
@@ -21940,7 +21966,7 @@
         <v>19</v>
       </c>
       <c r="D269">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>178</v>
       </c>
       <c r="E269">
@@ -21948,11 +21974,11 @@
         <v>85</v>
       </c>
       <c r="F269">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>199</v>
       </c>
       <c r="G269">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>88</v>
       </c>
       <c r="H269" t="s">
@@ -22233,7 +22259,7 @@
         <v>19</v>
       </c>
       <c r="D274">
-        <f t="shared" ref="D274" si="64">D277-1</f>
+        <f t="shared" ref="D274" si="66">D277-1</f>
         <v>136</v>
       </c>
       <c r="E274">
@@ -22297,7 +22323,7 @@
         <v>155</v>
       </c>
       <c r="E275">
-        <f t="shared" ref="E275:E276" si="65">E274</f>
+        <f t="shared" ref="E275:E276" si="67">E274</f>
         <v>112</v>
       </c>
       <c r="F275">
@@ -22357,7 +22383,7 @@
         <v>178</v>
       </c>
       <c r="E276">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>112</v>
       </c>
       <c r="F276">
@@ -22365,7 +22391,7 @@
         <v>199</v>
       </c>
       <c r="G276">
-        <f t="shared" ref="G276" si="66">G275</f>
+        <f t="shared" ref="G276" si="68">G275</f>
         <v>117</v>
       </c>
       <c r="H276" t="s">
@@ -22474,11 +22500,11 @@
         <v>156</v>
       </c>
       <c r="E278">
-        <f t="shared" ref="E278:E279" si="67">E277</f>
+        <f t="shared" ref="E278:E279" si="69">E277</f>
         <v>110</v>
       </c>
       <c r="F278">
-        <f t="shared" ref="F278:F279" si="68">D278</f>
+        <f t="shared" ref="F278:F279" si="70">D278</f>
         <v>156</v>
       </c>
       <c r="G278">
@@ -22531,11 +22557,11 @@
         <v>178</v>
       </c>
       <c r="E279">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>110</v>
       </c>
       <c r="F279">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>178</v>
       </c>
       <c r="G279">
@@ -22713,7 +22739,7 @@
         <v>155</v>
       </c>
       <c r="G282">
-        <f t="shared" ref="G282:G284" si="69">E282+3</f>
+        <f t="shared" ref="G282:G284" si="71">E282+3</f>
         <v>134</v>
       </c>
       <c r="H282" t="s">
@@ -22773,7 +22799,7 @@
         <v>179</v>
       </c>
       <c r="G283">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>134</v>
       </c>
       <c r="H283" t="s">
@@ -22833,7 +22859,7 @@
         <v>199</v>
       </c>
       <c r="G284">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>134</v>
       </c>
       <c r="H284" t="s">
@@ -28277,11 +28303,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E123" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34447,7 +34473,7 @@
         <v>1519</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>1520</v>
+        <v>1585</v>
       </c>
       <c r="D123" s="10" t="s">
         <v>1520</v>

</xml_diff>

<commit_message>
minor layout update (avoiding word 'optimise' in thresholds header, to avoid British/US English inconsistencies)
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4386" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F2C2A0-6F88-40F5-BB88-C3A04BE6D602}"/>
+  <xr:revisionPtr revIDLastSave="4389" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44273BA7-D333-4E7D-A459-C782218610C8}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="0" windowWidth="14850" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4145" uniqueCount="1604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4145" uniqueCount="1606">
   <si>
     <t>name</t>
   </si>
@@ -4964,6 +4964,12 @@
   </si>
   <si>
     <t>adabcf</t>
+  </si>
+  <si>
+    <t>Urban design thresholds to promote walking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 2022 Lancet Global Health Series found that to achieve at least 80% probability of engaging in any walking for transport, an average urban neighbourhood would need a population density of at least about 5700 people km², and street connectivity of at least 100 intersections per km². Preliminary evidence showed that street intersection density above 250 per km² and ultra-dense neighbourhoods ( &gt; 15,000 persons per km²) may have decreasing benefits for physical activity. This is an important topic for future research. </t>
   </si>
 </sst>
 </file>
@@ -5542,7 +5548,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5608,9 +5614,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6045,7 +6048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6382,7 +6385,7 @@
         <v>200</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G5:G6" si="1">E6+3</f>
+        <f t="shared" ref="G6" si="1">E6+3</f>
         <v>13</v>
       </c>
       <c r="H6" t="s">
@@ -10319,7 +10322,7 @@
         <v>0</v>
       </c>
       <c r="N72" t="str">
-        <f>$N$71</f>
+        <f t="shared" ref="N72:N79" si="12">$N$71</f>
         <v>d0d8dd</v>
       </c>
       <c r="O72" t="s">
@@ -10349,7 +10352,7 @@
         <v>19</v>
       </c>
       <c r="D73">
-        <f t="shared" ref="D73" si="12">D76-1</f>
+        <f t="shared" ref="D73" si="13">D76-1</f>
         <v>113</v>
       </c>
       <c r="E73">
@@ -10380,7 +10383,7 @@
         <v>0</v>
       </c>
       <c r="N73" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O73" t="s">
@@ -10414,7 +10417,7 @@
         <v>140</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:E78" si="13">E73</f>
+        <f t="shared" ref="E74:E78" si="14">E73</f>
         <v>178</v>
       </c>
       <c r="F74">
@@ -10441,7 +10444,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O74" t="s">
@@ -10475,7 +10478,7 @@
         <v>168</v>
       </c>
       <c r="E75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>178</v>
       </c>
       <c r="F75">
@@ -10483,7 +10486,7 @@
         <v>194</v>
       </c>
       <c r="G75">
-        <f t="shared" ref="G75" si="14">G74</f>
+        <f t="shared" ref="G75" si="15">G74</f>
         <v>183</v>
       </c>
       <c r="H75" t="s">
@@ -10502,7 +10505,7 @@
         <v>0</v>
       </c>
       <c r="N75" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O75" t="s">
@@ -10562,7 +10565,7 @@
         <v>21</v>
       </c>
       <c r="N76" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O76" t="s">
@@ -10596,11 +10599,11 @@
         <v>141</v>
       </c>
       <c r="E77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176</v>
       </c>
       <c r="F77">
-        <f t="shared" ref="F77:F78" si="15">D77</f>
+        <f t="shared" ref="F77:F78" si="16">D77</f>
         <v>141</v>
       </c>
       <c r="G77">
@@ -10623,7 +10626,7 @@
         <v>21</v>
       </c>
       <c r="N77" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O77" t="s">
@@ -10657,11 +10660,11 @@
         <v>168</v>
       </c>
       <c r="E78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176</v>
       </c>
       <c r="F78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>168</v>
       </c>
       <c r="G78">
@@ -10684,7 +10687,7 @@
         <v>21</v>
       </c>
       <c r="N78" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O78" t="s">
@@ -10743,7 +10746,7 @@
         <v>21</v>
       </c>
       <c r="N79" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="12"/>
         <v>d0d8dd</v>
       </c>
       <c r="O79" t="s">
@@ -10862,7 +10865,7 @@
         <v>0</v>
       </c>
       <c r="N81" t="str">
-        <f>$N$71</f>
+        <f t="shared" ref="N81:N100" si="17">$N$71</f>
         <v>d0d8dd</v>
       </c>
       <c r="O81" t="s">
@@ -10904,7 +10907,7 @@
         <v>140</v>
       </c>
       <c r="G82">
-        <f t="shared" ref="G82:G100" si="16">E82+3</f>
+        <f t="shared" ref="G82:G100" si="18">E82+3</f>
         <v>200</v>
       </c>
       <c r="H82" t="s">
@@ -10923,7 +10926,7 @@
         <v>0</v>
       </c>
       <c r="N82" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O82" t="s">
@@ -10965,7 +10968,7 @@
         <v>169</v>
       </c>
       <c r="G83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>200</v>
       </c>
       <c r="H83" t="s">
@@ -10984,7 +10987,7 @@
         <v>0</v>
       </c>
       <c r="N83" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O83" t="s">
@@ -11026,7 +11029,7 @@
         <v>194</v>
       </c>
       <c r="G84">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>200</v>
       </c>
       <c r="H84" t="s">
@@ -11045,7 +11048,7 @@
         <v>0</v>
       </c>
       <c r="N84" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O84" t="s">
@@ -11075,7 +11078,7 @@
         <v>19</v>
       </c>
       <c r="D85">
-        <f t="shared" ref="D85:D100" si="17">D81</f>
+        <f t="shared" ref="D85:D100" si="19">D81</f>
         <v>14</v>
       </c>
       <c r="E85">
@@ -11083,7 +11086,7 @@
         <v>212</v>
       </c>
       <c r="F85">
-        <f t="shared" ref="F85:F100" si="18">F81</f>
+        <f t="shared" ref="F85:F100" si="20">F81</f>
         <v>112</v>
       </c>
       <c r="G85">
@@ -11106,7 +11109,7 @@
         <v>0</v>
       </c>
       <c r="N85" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O85" t="s">
@@ -11136,7 +11139,7 @@
         <v>19</v>
       </c>
       <c r="D86">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>113</v>
       </c>
       <c r="E86">
@@ -11144,7 +11147,7 @@
         <v>213</v>
       </c>
       <c r="F86">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>140</v>
       </c>
       <c r="G86">
@@ -11167,7 +11170,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O86" t="s">
@@ -11197,7 +11200,7 @@
         <v>19</v>
       </c>
       <c r="D87">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>140</v>
       </c>
       <c r="E87">
@@ -11205,11 +11208,11 @@
         <v>213</v>
       </c>
       <c r="F87">
+        <f t="shared" si="20"/>
+        <v>169</v>
+      </c>
+      <c r="G87">
         <f t="shared" si="18"/>
-        <v>169</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="16"/>
         <v>216</v>
       </c>
       <c r="H87" t="s">
@@ -11228,7 +11231,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O87" t="s">
@@ -11258,7 +11261,7 @@
         <v>19</v>
       </c>
       <c r="D88">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>168</v>
       </c>
       <c r="E88">
@@ -11266,11 +11269,11 @@
         <v>213</v>
       </c>
       <c r="F88">
+        <f t="shared" si="20"/>
+        <v>194</v>
+      </c>
+      <c r="G88">
         <f t="shared" si="18"/>
-        <v>194</v>
-      </c>
-      <c r="G88">
-        <f t="shared" si="16"/>
         <v>216</v>
       </c>
       <c r="H88" t="s">
@@ -11289,7 +11292,7 @@
         <v>0</v>
       </c>
       <c r="N88" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O88" t="s">
@@ -11319,7 +11322,7 @@
         <v>19</v>
       </c>
       <c r="D89">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>14</v>
       </c>
       <c r="E89">
@@ -11327,7 +11330,7 @@
         <v>228</v>
       </c>
       <c r="F89">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>112</v>
       </c>
       <c r="G89">
@@ -11350,7 +11353,7 @@
         <v>0</v>
       </c>
       <c r="N89" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O89" t="s">
@@ -11380,7 +11383,7 @@
         <v>19</v>
       </c>
       <c r="D90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>113</v>
       </c>
       <c r="E90">
@@ -11388,11 +11391,11 @@
         <v>229</v>
       </c>
       <c r="F90">
+        <f t="shared" si="20"/>
+        <v>140</v>
+      </c>
+      <c r="G90">
         <f t="shared" si="18"/>
-        <v>140</v>
-      </c>
-      <c r="G90">
-        <f t="shared" si="16"/>
         <v>232</v>
       </c>
       <c r="H90" t="s">
@@ -11411,7 +11414,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O90" t="s">
@@ -11441,7 +11444,7 @@
         <v>19</v>
       </c>
       <c r="D91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>140</v>
       </c>
       <c r="E91">
@@ -11449,11 +11452,11 @@
         <v>229</v>
       </c>
       <c r="F91">
+        <f t="shared" si="20"/>
+        <v>169</v>
+      </c>
+      <c r="G91">
         <f t="shared" si="18"/>
-        <v>169</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="16"/>
         <v>232</v>
       </c>
       <c r="H91" t="s">
@@ -11472,7 +11475,7 @@
         <v>0</v>
       </c>
       <c r="N91" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O91" t="s">
@@ -11502,7 +11505,7 @@
         <v>19</v>
       </c>
       <c r="D92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>168</v>
       </c>
       <c r="E92">
@@ -11510,11 +11513,11 @@
         <v>229</v>
       </c>
       <c r="F92">
+        <f t="shared" si="20"/>
+        <v>194</v>
+      </c>
+      <c r="G92">
         <f t="shared" si="18"/>
-        <v>194</v>
-      </c>
-      <c r="G92">
-        <f t="shared" si="16"/>
         <v>232</v>
       </c>
       <c r="H92" t="s">
@@ -11533,7 +11536,7 @@
         <v>0</v>
       </c>
       <c r="N92" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O92" t="s">
@@ -11563,7 +11566,7 @@
         <v>19</v>
       </c>
       <c r="D93">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>14</v>
       </c>
       <c r="E93">
@@ -11571,7 +11574,7 @@
         <v>244</v>
       </c>
       <c r="F93">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>112</v>
       </c>
       <c r="G93">
@@ -11594,7 +11597,7 @@
         <v>0</v>
       </c>
       <c r="N93" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O93" t="s">
@@ -11624,7 +11627,7 @@
         <v>19</v>
       </c>
       <c r="D94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>113</v>
       </c>
       <c r="E94">
@@ -11632,11 +11635,11 @@
         <v>245</v>
       </c>
       <c r="F94">
+        <f t="shared" si="20"/>
+        <v>140</v>
+      </c>
+      <c r="G94">
         <f t="shared" si="18"/>
-        <v>140</v>
-      </c>
-      <c r="G94">
-        <f t="shared" si="16"/>
         <v>248</v>
       </c>
       <c r="H94" t="s">
@@ -11655,7 +11658,7 @@
         <v>0</v>
       </c>
       <c r="N94" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O94" t="s">
@@ -11685,7 +11688,7 @@
         <v>19</v>
       </c>
       <c r="D95">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>140</v>
       </c>
       <c r="E95">
@@ -11693,11 +11696,11 @@
         <v>245</v>
       </c>
       <c r="F95">
+        <f t="shared" si="20"/>
+        <v>169</v>
+      </c>
+      <c r="G95">
         <f t="shared" si="18"/>
-        <v>169</v>
-      </c>
-      <c r="G95">
-        <f t="shared" si="16"/>
         <v>248</v>
       </c>
       <c r="H95" t="s">
@@ -11716,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="N95" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O95" t="s">
@@ -11746,7 +11749,7 @@
         <v>19</v>
       </c>
       <c r="D96">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>168</v>
       </c>
       <c r="E96">
@@ -11754,11 +11757,11 @@
         <v>245</v>
       </c>
       <c r="F96">
+        <f t="shared" si="20"/>
+        <v>194</v>
+      </c>
+      <c r="G96">
         <f t="shared" si="18"/>
-        <v>194</v>
-      </c>
-      <c r="G96">
-        <f t="shared" si="16"/>
         <v>248</v>
       </c>
       <c r="H96" t="s">
@@ -11777,7 +11780,7 @@
         <v>0</v>
       </c>
       <c r="N96" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O96" t="s">
@@ -11807,7 +11810,7 @@
         <v>19</v>
       </c>
       <c r="D97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>14</v>
       </c>
       <c r="E97">
@@ -11815,7 +11818,7 @@
         <v>260</v>
       </c>
       <c r="F97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>112</v>
       </c>
       <c r="G97">
@@ -11838,7 +11841,7 @@
         <v>0</v>
       </c>
       <c r="N97" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O97" t="s">
@@ -11868,7 +11871,7 @@
         <v>19</v>
       </c>
       <c r="D98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>113</v>
       </c>
       <c r="E98">
@@ -11876,11 +11879,11 @@
         <v>261</v>
       </c>
       <c r="F98">
+        <f t="shared" si="20"/>
+        <v>140</v>
+      </c>
+      <c r="G98">
         <f t="shared" si="18"/>
-        <v>140</v>
-      </c>
-      <c r="G98">
-        <f t="shared" si="16"/>
         <v>264</v>
       </c>
       <c r="H98" t="s">
@@ -11899,7 +11902,7 @@
         <v>0</v>
       </c>
       <c r="N98" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O98" t="s">
@@ -11929,7 +11932,7 @@
         <v>19</v>
       </c>
       <c r="D99">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>140</v>
       </c>
       <c r="E99">
@@ -11937,11 +11940,11 @@
         <v>261</v>
       </c>
       <c r="F99">
+        <f t="shared" si="20"/>
+        <v>169</v>
+      </c>
+      <c r="G99">
         <f t="shared" si="18"/>
-        <v>169</v>
-      </c>
-      <c r="G99">
-        <f t="shared" si="16"/>
         <v>264</v>
       </c>
       <c r="H99" t="s">
@@ -11960,7 +11963,7 @@
         <v>0</v>
       </c>
       <c r="N99" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O99" t="s">
@@ -11990,7 +11993,7 @@
         <v>19</v>
       </c>
       <c r="D100">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>168</v>
       </c>
       <c r="E100">
@@ -11998,11 +12001,11 @@
         <v>261</v>
       </c>
       <c r="F100">
+        <f t="shared" si="20"/>
+        <v>194</v>
+      </c>
+      <c r="G100">
         <f t="shared" si="18"/>
-        <v>194</v>
-      </c>
-      <c r="G100">
-        <f t="shared" si="16"/>
         <v>264</v>
       </c>
       <c r="H100" t="s">
@@ -12021,7 +12024,7 @@
         <v>0</v>
       </c>
       <c r="N100" t="str">
-        <f>$N$71</f>
+        <f t="shared" si="17"/>
         <v>d0d8dd</v>
       </c>
       <c r="O100" t="s">
@@ -12746,7 +12749,7 @@
         <v>19</v>
       </c>
       <c r="D113">
-        <f t="shared" ref="D113" si="19">D116-1</f>
+        <f t="shared" ref="D113" si="21">D116-1</f>
         <v>113</v>
       </c>
       <c r="E113">
@@ -12810,7 +12813,7 @@
         <v>140</v>
       </c>
       <c r="E114">
-        <f t="shared" ref="E114:E115" si="20">E113</f>
+        <f t="shared" ref="E114:E115" si="22">E113</f>
         <v>32</v>
       </c>
       <c r="F114">
@@ -12870,7 +12873,7 @@
         <v>168</v>
       </c>
       <c r="E115">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>32</v>
       </c>
       <c r="F115">
@@ -12878,7 +12881,7 @@
         <v>194</v>
       </c>
       <c r="G115">
-        <f t="shared" ref="G115" si="21">G114</f>
+        <f t="shared" ref="G115" si="23">G114</f>
         <v>37</v>
       </c>
       <c r="H115" t="s">
@@ -12989,11 +12992,11 @@
         <v>141</v>
       </c>
       <c r="E117">
-        <f t="shared" ref="E117:E118" si="22">E116</f>
+        <f t="shared" ref="E117:E118" si="24">E116</f>
         <v>30</v>
       </c>
       <c r="F117">
-        <f t="shared" ref="F117:F118" si="23">D117</f>
+        <f t="shared" ref="F117:F118" si="25">D117</f>
         <v>141</v>
       </c>
       <c r="G117">
@@ -13049,11 +13052,11 @@
         <v>168</v>
       </c>
       <c r="E118">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>30</v>
       </c>
       <c r="F118">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>168</v>
       </c>
       <c r="G118">
@@ -13293,7 +13296,7 @@
         <v>140</v>
       </c>
       <c r="G122">
-        <f t="shared" ref="G122:G124" si="24">E122+3</f>
+        <f t="shared" ref="G122:G124" si="26">E122+3</f>
         <v>54</v>
       </c>
       <c r="H122" t="s">
@@ -13353,7 +13356,7 @@
         <v>169</v>
       </c>
       <c r="G123">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>54</v>
       </c>
       <c r="H123" t="s">
@@ -13413,7 +13416,7 @@
         <v>194</v>
       </c>
       <c r="G124">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>54</v>
       </c>
       <c r="H124" t="s">
@@ -13461,7 +13464,7 @@
         <v>19</v>
       </c>
       <c r="D125">
-        <f t="shared" ref="D125:D156" si="25">D121</f>
+        <f t="shared" ref="D125:D156" si="27">D121</f>
         <v>14</v>
       </c>
       <c r="E125">
@@ -13469,7 +13472,7 @@
         <v>62</v>
       </c>
       <c r="F125">
-        <f t="shared" ref="F125:F156" si="26">F121</f>
+        <f t="shared" ref="F125:F156" si="28">F121</f>
         <v>112</v>
       </c>
       <c r="G125">
@@ -13521,7 +13524,7 @@
         <v>19</v>
       </c>
       <c r="D126">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E126">
@@ -13529,7 +13532,7 @@
         <v>63</v>
       </c>
       <c r="F126">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G126">
@@ -13581,7 +13584,7 @@
         <v>19</v>
       </c>
       <c r="D127">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E127">
@@ -13589,11 +13592,11 @@
         <v>63</v>
       </c>
       <c r="F127">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G127">
-        <f t="shared" ref="G127:G128" si="27">E127+3</f>
+        <f t="shared" ref="G127:G128" si="29">E127+3</f>
         <v>66</v>
       </c>
       <c r="H127" t="s">
@@ -13641,7 +13644,7 @@
         <v>19</v>
       </c>
       <c r="D128">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E128">
@@ -13649,11 +13652,11 @@
         <v>63</v>
       </c>
       <c r="F128">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G128">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>66</v>
       </c>
       <c r="H128" t="s">
@@ -13701,7 +13704,7 @@
         <v>19</v>
       </c>
       <c r="D129">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E129">
@@ -13709,7 +13712,7 @@
         <v>74</v>
       </c>
       <c r="F129">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G129">
@@ -13761,7 +13764,7 @@
         <v>19</v>
       </c>
       <c r="D130">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E130">
@@ -13769,11 +13772,11 @@
         <v>75</v>
       </c>
       <c r="F130">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G130">
-        <f t="shared" ref="G130:G132" si="28">E130+3</f>
+        <f t="shared" ref="G130:G132" si="30">E130+3</f>
         <v>78</v>
       </c>
       <c r="H130" t="s">
@@ -13821,7 +13824,7 @@
         <v>19</v>
       </c>
       <c r="D131">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E131">
@@ -13829,11 +13832,11 @@
         <v>75</v>
       </c>
       <c r="F131">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G131">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>78</v>
       </c>
       <c r="H131" t="s">
@@ -13881,7 +13884,7 @@
         <v>19</v>
       </c>
       <c r="D132">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E132">
@@ -13889,11 +13892,11 @@
         <v>75</v>
       </c>
       <c r="F132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>78</v>
       </c>
       <c r="H132" t="s">
@@ -13941,7 +13944,7 @@
         <v>19</v>
       </c>
       <c r="D133">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E133">
@@ -13949,7 +13952,7 @@
         <v>86</v>
       </c>
       <c r="F133">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G133">
@@ -14001,7 +14004,7 @@
         <v>19</v>
       </c>
       <c r="D134">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E134">
@@ -14009,11 +14012,11 @@
         <v>87</v>
       </c>
       <c r="F134">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G134">
-        <f t="shared" ref="G134:G136" si="29">E134+3</f>
+        <f t="shared" ref="G134:G136" si="31">E134+3</f>
         <v>90</v>
       </c>
       <c r="H134" t="s">
@@ -14061,7 +14064,7 @@
         <v>19</v>
       </c>
       <c r="D135">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E135">
@@ -14069,11 +14072,11 @@
         <v>87</v>
       </c>
       <c r="F135">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G135">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>90</v>
       </c>
       <c r="H135" t="s">
@@ -14121,7 +14124,7 @@
         <v>19</v>
       </c>
       <c r="D136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E136">
@@ -14129,11 +14132,11 @@
         <v>87</v>
       </c>
       <c r="F136">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G136">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>90</v>
       </c>
       <c r="H136" t="s">
@@ -14181,7 +14184,7 @@
         <v>19</v>
       </c>
       <c r="D137">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E137">
@@ -14189,7 +14192,7 @@
         <v>98</v>
       </c>
       <c r="F137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G137">
@@ -14241,7 +14244,7 @@
         <v>19</v>
       </c>
       <c r="D138">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E138">
@@ -14249,11 +14252,11 @@
         <v>99</v>
       </c>
       <c r="F138">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G138">
-        <f t="shared" ref="G138:G140" si="30">E138+3</f>
+        <f t="shared" ref="G138:G140" si="32">E138+3</f>
         <v>102</v>
       </c>
       <c r="H138" t="s">
@@ -14301,7 +14304,7 @@
         <v>19</v>
       </c>
       <c r="D139">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E139">
@@ -14309,11 +14312,11 @@
         <v>99</v>
       </c>
       <c r="F139">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G139">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>102</v>
       </c>
       <c r="H139" t="s">
@@ -14361,7 +14364,7 @@
         <v>19</v>
       </c>
       <c r="D140">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E140">
@@ -14369,11 +14372,11 @@
         <v>99</v>
       </c>
       <c r="F140">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G140">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>102</v>
       </c>
       <c r="H140" t="s">
@@ -14421,7 +14424,7 @@
         <v>19</v>
       </c>
       <c r="D141">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E141">
@@ -14429,7 +14432,7 @@
         <v>110</v>
       </c>
       <c r="F141">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G141">
@@ -14481,7 +14484,7 @@
         <v>19</v>
       </c>
       <c r="D142">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E142">
@@ -14489,11 +14492,11 @@
         <v>111</v>
       </c>
       <c r="F142">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G142">
-        <f t="shared" ref="G142:G144" si="31">E142+3</f>
+        <f t="shared" ref="G142:G144" si="33">E142+3</f>
         <v>114</v>
       </c>
       <c r="H142" t="s">
@@ -14541,7 +14544,7 @@
         <v>19</v>
       </c>
       <c r="D143">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E143">
@@ -14549,11 +14552,11 @@
         <v>111</v>
       </c>
       <c r="F143">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G143">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>114</v>
       </c>
       <c r="H143" t="s">
@@ -14601,7 +14604,7 @@
         <v>19</v>
       </c>
       <c r="D144">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E144">
@@ -14609,11 +14612,11 @@
         <v>111</v>
       </c>
       <c r="F144">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G144">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>114</v>
       </c>
       <c r="H144" t="s">
@@ -14661,7 +14664,7 @@
         <v>19</v>
       </c>
       <c r="D145">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E145">
@@ -14669,7 +14672,7 @@
         <v>122</v>
       </c>
       <c r="F145">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G145">
@@ -14721,7 +14724,7 @@
         <v>19</v>
       </c>
       <c r="D146">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E146">
@@ -14729,11 +14732,11 @@
         <v>123</v>
       </c>
       <c r="F146">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G146">
-        <f t="shared" ref="G146:G148" si="32">E146+3</f>
+        <f t="shared" ref="G146:G148" si="34">E146+3</f>
         <v>126</v>
       </c>
       <c r="H146" t="s">
@@ -14781,7 +14784,7 @@
         <v>19</v>
       </c>
       <c r="D147">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E147">
@@ -14789,11 +14792,11 @@
         <v>123</v>
       </c>
       <c r="F147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G147">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>126</v>
       </c>
       <c r="H147" t="s">
@@ -14841,7 +14844,7 @@
         <v>19</v>
       </c>
       <c r="D148">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E148">
@@ -14849,11 +14852,11 @@
         <v>123</v>
       </c>
       <c r="F148">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G148">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>126</v>
       </c>
       <c r="H148" t="s">
@@ -14902,7 +14905,7 @@
         <v>19</v>
       </c>
       <c r="D149">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E149">
@@ -14910,7 +14913,7 @@
         <v>134</v>
       </c>
       <c r="F149">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G149">
@@ -14963,7 +14966,7 @@
         <v>19</v>
       </c>
       <c r="D150">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E150">
@@ -14971,11 +14974,11 @@
         <v>135</v>
       </c>
       <c r="F150">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G150">
-        <f t="shared" ref="G150:G152" si="33">E150+3</f>
+        <f t="shared" ref="G150:G152" si="35">E150+3</f>
         <v>138</v>
       </c>
       <c r="H150" t="s">
@@ -15024,7 +15027,7 @@
         <v>19</v>
       </c>
       <c r="D151">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E151">
@@ -15032,11 +15035,11 @@
         <v>135</v>
       </c>
       <c r="F151">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G151">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>138</v>
       </c>
       <c r="H151" t="s">
@@ -15085,7 +15088,7 @@
         <v>19</v>
       </c>
       <c r="D152">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E152">
@@ -15093,11 +15096,11 @@
         <v>135</v>
       </c>
       <c r="F152">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>138</v>
       </c>
       <c r="H152" t="s">
@@ -15146,7 +15149,7 @@
         <v>19</v>
       </c>
       <c r="D153">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="E153">
@@ -15154,7 +15157,7 @@
         <v>146</v>
       </c>
       <c r="F153">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>112</v>
       </c>
       <c r="G153">
@@ -15207,7 +15210,7 @@
         <v>19</v>
       </c>
       <c r="D154">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>113</v>
       </c>
       <c r="E154">
@@ -15215,11 +15218,11 @@
         <v>147</v>
       </c>
       <c r="F154">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>140</v>
       </c>
       <c r="G154">
-        <f t="shared" ref="G154:G156" si="34">E154+3</f>
+        <f t="shared" ref="G154:G156" si="36">E154+3</f>
         <v>150</v>
       </c>
       <c r="H154" t="s">
@@ -15268,7 +15271,7 @@
         <v>19</v>
       </c>
       <c r="D155">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>140</v>
       </c>
       <c r="E155">
@@ -15276,11 +15279,11 @@
         <v>147</v>
       </c>
       <c r="F155">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>169</v>
       </c>
       <c r="G155">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>150</v>
       </c>
       <c r="H155" t="s">
@@ -15329,7 +15332,7 @@
         <v>19</v>
       </c>
       <c r="D156">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>168</v>
       </c>
       <c r="E156">
@@ -15337,11 +15340,11 @@
         <v>147</v>
       </c>
       <c r="F156">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>194</v>
       </c>
       <c r="G156">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>150</v>
       </c>
       <c r="H156" t="s">
@@ -15390,7 +15393,7 @@
         <v>19</v>
       </c>
       <c r="D157">
-        <f t="shared" ref="D157:D184" si="35">D153</f>
+        <f t="shared" ref="D157:D184" si="37">D153</f>
         <v>14</v>
       </c>
       <c r="E157">
@@ -15398,7 +15401,7 @@
         <v>158</v>
       </c>
       <c r="F157">
-        <f t="shared" ref="F157:F188" si="36">F153</f>
+        <f t="shared" ref="F157:F188" si="38">F153</f>
         <v>112</v>
       </c>
       <c r="G157">
@@ -15451,7 +15454,7 @@
         <v>19</v>
       </c>
       <c r="D158">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E158">
@@ -15459,11 +15462,11 @@
         <v>159</v>
       </c>
       <c r="F158">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G158">
-        <f t="shared" ref="G158:G160" si="37">E158+3</f>
+        <f t="shared" ref="G158:G160" si="39">E158+3</f>
         <v>162</v>
       </c>
       <c r="H158" t="s">
@@ -15512,7 +15515,7 @@
         <v>19</v>
       </c>
       <c r="D159">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E159">
@@ -15520,11 +15523,11 @@
         <v>159</v>
       </c>
       <c r="F159">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G159">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>162</v>
       </c>
       <c r="H159" t="s">
@@ -15573,7 +15576,7 @@
         <v>19</v>
       </c>
       <c r="D160">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E160">
@@ -15581,11 +15584,11 @@
         <v>159</v>
       </c>
       <c r="F160">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G160">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>162</v>
       </c>
       <c r="H160" t="s">
@@ -15634,7 +15637,7 @@
         <v>19</v>
       </c>
       <c r="D161">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E161">
@@ -15642,7 +15645,7 @@
         <v>170</v>
       </c>
       <c r="F161">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G161">
@@ -15695,7 +15698,7 @@
         <v>19</v>
       </c>
       <c r="D162">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E162">
@@ -15703,11 +15706,11 @@
         <v>171</v>
       </c>
       <c r="F162">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G162">
-        <f t="shared" ref="G162:G164" si="38">E162+3</f>
+        <f t="shared" ref="G162:G164" si="40">E162+3</f>
         <v>174</v>
       </c>
       <c r="H162" t="s">
@@ -15756,7 +15759,7 @@
         <v>19</v>
       </c>
       <c r="D163">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E163">
@@ -15764,11 +15767,11 @@
         <v>171</v>
       </c>
       <c r="F163">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G163">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>174</v>
       </c>
       <c r="H163" t="s">
@@ -15817,7 +15820,7 @@
         <v>19</v>
       </c>
       <c r="D164">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E164">
@@ -15825,11 +15828,11 @@
         <v>171</v>
       </c>
       <c r="F164">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G164">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>174</v>
       </c>
       <c r="H164" t="s">
@@ -15878,7 +15881,7 @@
         <v>19</v>
       </c>
       <c r="D165">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E165">
@@ -15886,7 +15889,7 @@
         <v>182</v>
       </c>
       <c r="F165">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G165">
@@ -15939,7 +15942,7 @@
         <v>19</v>
       </c>
       <c r="D166">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E166">
@@ -15947,11 +15950,11 @@
         <v>183</v>
       </c>
       <c r="F166">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G166">
-        <f t="shared" ref="G166:G168" si="39">E166+3</f>
+        <f t="shared" ref="G166:G168" si="41">E166+3</f>
         <v>186</v>
       </c>
       <c r="H166" t="s">
@@ -16000,7 +16003,7 @@
         <v>19</v>
       </c>
       <c r="D167">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E167">
@@ -16008,11 +16011,11 @@
         <v>183</v>
       </c>
       <c r="F167">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G167">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>186</v>
       </c>
       <c r="H167" t="s">
@@ -16061,7 +16064,7 @@
         <v>19</v>
       </c>
       <c r="D168">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E168">
@@ -16069,11 +16072,11 @@
         <v>183</v>
       </c>
       <c r="F168">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G168">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>186</v>
       </c>
       <c r="H168" t="s">
@@ -16122,7 +16125,7 @@
         <v>19</v>
       </c>
       <c r="D169">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E169">
@@ -16130,7 +16133,7 @@
         <v>194</v>
       </c>
       <c r="F169">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G169">
@@ -16183,7 +16186,7 @@
         <v>19</v>
       </c>
       <c r="D170">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E170">
@@ -16191,11 +16194,11 @@
         <v>195</v>
       </c>
       <c r="F170">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G170">
-        <f t="shared" ref="G170:G172" si="40">E170+3</f>
+        <f t="shared" ref="G170:G172" si="42">E170+3</f>
         <v>198</v>
       </c>
       <c r="H170" t="s">
@@ -16244,7 +16247,7 @@
         <v>19</v>
       </c>
       <c r="D171">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E171">
@@ -16252,11 +16255,11 @@
         <v>195</v>
       </c>
       <c r="F171">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G171">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>198</v>
       </c>
       <c r="H171" t="s">
@@ -16305,7 +16308,7 @@
         <v>19</v>
       </c>
       <c r="D172">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E172">
@@ -16313,11 +16316,11 @@
         <v>195</v>
       </c>
       <c r="F172">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G172">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>198</v>
       </c>
       <c r="H172" t="s">
@@ -16366,7 +16369,7 @@
         <v>19</v>
       </c>
       <c r="D173">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E173">
@@ -16374,7 +16377,7 @@
         <v>206</v>
       </c>
       <c r="F173">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G173">
@@ -16427,7 +16430,7 @@
         <v>19</v>
       </c>
       <c r="D174">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E174">
@@ -16435,11 +16438,11 @@
         <v>207</v>
       </c>
       <c r="F174">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G174">
-        <f t="shared" ref="G174:G176" si="41">E174+3</f>
+        <f t="shared" ref="G174:G176" si="43">E174+3</f>
         <v>210</v>
       </c>
       <c r="H174" t="s">
@@ -16488,7 +16491,7 @@
         <v>19</v>
       </c>
       <c r="D175">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E175">
@@ -16496,11 +16499,11 @@
         <v>207</v>
       </c>
       <c r="F175">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G175">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>210</v>
       </c>
       <c r="H175" t="s">
@@ -16549,7 +16552,7 @@
         <v>19</v>
       </c>
       <c r="D176">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E176">
@@ -16557,11 +16560,11 @@
         <v>207</v>
       </c>
       <c r="F176">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G176">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>210</v>
       </c>
       <c r="H176" t="s">
@@ -16610,7 +16613,7 @@
         <v>19</v>
       </c>
       <c r="D177">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E177">
@@ -16618,7 +16621,7 @@
         <v>218</v>
       </c>
       <c r="F177">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G177">
@@ -16671,7 +16674,7 @@
         <v>19</v>
       </c>
       <c r="D178">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E178">
@@ -16679,11 +16682,11 @@
         <v>219</v>
       </c>
       <c r="F178">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G178">
-        <f t="shared" ref="G178:G180" si="42">E178+3</f>
+        <f t="shared" ref="G178:G180" si="44">E178+3</f>
         <v>222</v>
       </c>
       <c r="H178" t="s">
@@ -16732,7 +16735,7 @@
         <v>19</v>
       </c>
       <c r="D179">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E179">
@@ -16740,11 +16743,11 @@
         <v>219</v>
       </c>
       <c r="F179">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G179">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>222</v>
       </c>
       <c r="H179" t="s">
@@ -16793,7 +16796,7 @@
         <v>19</v>
       </c>
       <c r="D180">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E180">
@@ -16801,11 +16804,11 @@
         <v>219</v>
       </c>
       <c r="F180">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G180">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>222</v>
       </c>
       <c r="H180" t="s">
@@ -16854,7 +16857,7 @@
         <v>19</v>
       </c>
       <c r="D181">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="E181">
@@ -16862,7 +16865,7 @@
         <v>230</v>
       </c>
       <c r="F181">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G181">
@@ -16915,7 +16918,7 @@
         <v>19</v>
       </c>
       <c r="D182">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>113</v>
       </c>
       <c r="E182">
@@ -16923,11 +16926,11 @@
         <v>231</v>
       </c>
       <c r="F182">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G182">
-        <f t="shared" ref="G182:G184" si="43">E182+3</f>
+        <f t="shared" ref="G182:G184" si="45">E182+3</f>
         <v>234</v>
       </c>
       <c r="H182" t="s">
@@ -16976,7 +16979,7 @@
         <v>19</v>
       </c>
       <c r="D183">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>140</v>
       </c>
       <c r="E183">
@@ -16984,11 +16987,11 @@
         <v>231</v>
       </c>
       <c r="F183">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G183">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>234</v>
       </c>
       <c r="H183" t="s">
@@ -17037,7 +17040,7 @@
         <v>19</v>
       </c>
       <c r="D184">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>168</v>
       </c>
       <c r="E184">
@@ -17045,11 +17048,11 @@
         <v>231</v>
       </c>
       <c r="F184">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G184">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>234</v>
       </c>
       <c r="H184" t="s">
@@ -17098,7 +17101,7 @@
         <v>19</v>
       </c>
       <c r="D185">
-        <f t="shared" ref="D185" si="44">D181</f>
+        <f t="shared" ref="D185" si="46">D181</f>
         <v>14</v>
       </c>
       <c r="E185">
@@ -17106,7 +17109,7 @@
         <v>242</v>
       </c>
       <c r="F185">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>112</v>
       </c>
       <c r="G185">
@@ -17167,11 +17170,11 @@
         <v>243</v>
       </c>
       <c r="F186">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>140</v>
       </c>
       <c r="G186">
-        <f t="shared" ref="G186:G188" si="45">E186+3</f>
+        <f t="shared" ref="G186:G188" si="47">E186+3</f>
         <v>246</v>
       </c>
       <c r="H186" t="s">
@@ -17228,11 +17231,11 @@
         <v>243</v>
       </c>
       <c r="F187">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>169</v>
       </c>
       <c r="G187">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>246</v>
       </c>
       <c r="H187" t="s">
@@ -17289,11 +17292,11 @@
         <v>243</v>
       </c>
       <c r="F188">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>194</v>
       </c>
       <c r="G188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>246</v>
       </c>
       <c r="H188" t="s">
@@ -18400,7 +18403,7 @@
         <v>19</v>
       </c>
       <c r="D207">
-        <f t="shared" ref="D207" si="46">D210-1</f>
+        <f t="shared" ref="D207" si="48">D210-1</f>
         <v>146</v>
       </c>
       <c r="E207">
@@ -18464,7 +18467,7 @@
         <v>165</v>
       </c>
       <c r="E208">
-        <f t="shared" ref="E208:E212" si="47">E207</f>
+        <f t="shared" ref="E208:E212" si="49">E207</f>
         <v>92</v>
       </c>
       <c r="F208">
@@ -18524,7 +18527,7 @@
         <v>188</v>
       </c>
       <c r="E209">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>92</v>
       </c>
       <c r="F209">
@@ -18532,7 +18535,7 @@
         <v>209</v>
       </c>
       <c r="G209">
-        <f t="shared" ref="G209" si="48">G208</f>
+        <f t="shared" ref="G209" si="50">G208</f>
         <v>97</v>
       </c>
       <c r="H209" t="s">
@@ -18641,11 +18644,11 @@
         <v>166</v>
       </c>
       <c r="E211">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>92</v>
       </c>
       <c r="F211">
-        <f t="shared" ref="F211:F212" si="49">D211</f>
+        <f t="shared" ref="F211:F212" si="51">D211</f>
         <v>166</v>
       </c>
       <c r="G211">
@@ -18698,11 +18701,11 @@
         <v>188</v>
       </c>
       <c r="E212">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>92</v>
       </c>
       <c r="F212">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>188</v>
       </c>
       <c r="G212">
@@ -18879,7 +18882,7 @@
         <v>165</v>
       </c>
       <c r="G215">
-        <f t="shared" ref="G215:G217" si="50">E215+3</f>
+        <f t="shared" ref="G215:G217" si="52">E215+3</f>
         <v>114</v>
       </c>
       <c r="H215" t="s">
@@ -18939,7 +18942,7 @@
         <v>189</v>
       </c>
       <c r="G216">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>114</v>
       </c>
       <c r="H216" t="s">
@@ -18999,7 +19002,7 @@
         <v>209</v>
       </c>
       <c r="G217">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>114</v>
       </c>
       <c r="H217" t="s">
@@ -19118,7 +19121,7 @@
         <v>165</v>
       </c>
       <c r="G219">
-        <f t="shared" ref="G219:G221" si="51">E219+3</f>
+        <f t="shared" ref="G219:G221" si="53">E219+3</f>
         <v>132</v>
       </c>
       <c r="H219" t="s">
@@ -19178,7 +19181,7 @@
         <v>189</v>
       </c>
       <c r="G220">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>132</v>
       </c>
       <c r="H220" t="s">
@@ -19238,7 +19241,7 @@
         <v>209</v>
       </c>
       <c r="G221">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>132</v>
       </c>
       <c r="H221" t="s">
@@ -19357,7 +19360,7 @@
         <v>165</v>
       </c>
       <c r="G223">
-        <f t="shared" ref="G223:G225" si="52">E223+3</f>
+        <f t="shared" ref="G223:G225" si="54">E223+3</f>
         <v>150</v>
       </c>
       <c r="H223" t="s">
@@ -19417,7 +19420,7 @@
         <v>189</v>
       </c>
       <c r="G224">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>150</v>
       </c>
       <c r="H224" t="s">
@@ -19477,7 +19480,7 @@
         <v>209</v>
       </c>
       <c r="G225">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>150</v>
       </c>
       <c r="H225" t="s">
@@ -19535,7 +19538,7 @@
         <v>100</v>
       </c>
       <c r="G226">
-        <f t="shared" ref="G226" si="53">E226+3</f>
+        <f t="shared" ref="G226" si="55">E226+3</f>
         <v>163</v>
       </c>
       <c r="H226" t="s">
@@ -19878,7 +19881,7 @@
         <v>19</v>
       </c>
       <c r="D232">
-        <f t="shared" ref="D232" si="54">D235-1</f>
+        <f t="shared" ref="D232" si="56">D235-1</f>
         <v>146</v>
       </c>
       <c r="E232">
@@ -19942,7 +19945,7 @@
         <v>165</v>
       </c>
       <c r="E233">
-        <f t="shared" ref="E233:E237" si="55">E232</f>
+        <f t="shared" ref="E233:E237" si="57">E232</f>
         <v>233</v>
       </c>
       <c r="F233">
@@ -20002,7 +20005,7 @@
         <v>188</v>
       </c>
       <c r="E234">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>233</v>
       </c>
       <c r="F234">
@@ -20010,7 +20013,7 @@
         <v>209</v>
       </c>
       <c r="G234">
-        <f t="shared" ref="G234" si="56">G233</f>
+        <f t="shared" ref="G234" si="58">G233</f>
         <v>238</v>
       </c>
       <c r="H234" t="s">
@@ -20119,11 +20122,11 @@
         <v>166</v>
       </c>
       <c r="E236">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>233</v>
       </c>
       <c r="F236">
-        <f t="shared" ref="F236:F237" si="57">D236</f>
+        <f t="shared" ref="F236:F237" si="59">D236</f>
         <v>166</v>
       </c>
       <c r="G236">
@@ -20176,11 +20179,11 @@
         <v>188</v>
       </c>
       <c r="E237">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>233</v>
       </c>
       <c r="F237">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>188</v>
       </c>
       <c r="G237">
@@ -20357,7 +20360,7 @@
         <v>165</v>
       </c>
       <c r="G240">
-        <f t="shared" ref="G240:G242" si="58">E240+3</f>
+        <f t="shared" ref="G240:G242" si="60">E240+3</f>
         <v>255</v>
       </c>
       <c r="H240" t="s">
@@ -20417,7 +20420,7 @@
         <v>189</v>
       </c>
       <c r="G241">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>255</v>
       </c>
       <c r="H241" t="s">
@@ -20477,7 +20480,7 @@
         <v>209</v>
       </c>
       <c r="G242">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>255</v>
       </c>
       <c r="H242" t="s">
@@ -20754,7 +20757,7 @@
         <v>19</v>
       </c>
       <c r="D247">
-        <f t="shared" ref="D247" si="59">D250-1</f>
+        <f t="shared" ref="D247" si="61">D250-1</f>
         <v>136</v>
       </c>
       <c r="E247">
@@ -20818,7 +20821,7 @@
         <v>155</v>
       </c>
       <c r="E248">
-        <f t="shared" ref="E248:E249" si="60">E247</f>
+        <f t="shared" ref="E248:E249" si="62">E247</f>
         <v>21</v>
       </c>
       <c r="F248">
@@ -20878,7 +20881,7 @@
         <v>178</v>
       </c>
       <c r="E249">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>21</v>
       </c>
       <c r="F249">
@@ -20886,7 +20889,7 @@
         <v>199</v>
       </c>
       <c r="G249">
-        <f t="shared" ref="G249" si="61">G248</f>
+        <f t="shared" ref="G249" si="63">G248</f>
         <v>26</v>
       </c>
       <c r="H249" t="s">
@@ -20994,11 +20997,11 @@
         <v>156</v>
       </c>
       <c r="E251">
-        <f t="shared" ref="E251:E252" si="62">E250</f>
+        <f t="shared" ref="E251:E252" si="64">E250</f>
         <v>19</v>
       </c>
       <c r="F251">
-        <f t="shared" ref="F251:F252" si="63">D251</f>
+        <f t="shared" ref="F251:F252" si="65">D251</f>
         <v>156</v>
       </c>
       <c r="G251">
@@ -21051,11 +21054,11 @@
         <v>178</v>
       </c>
       <c r="E252">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>19</v>
       </c>
       <c r="F252">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>178</v>
       </c>
       <c r="G252">
@@ -21233,7 +21236,7 @@
         <v>155</v>
       </c>
       <c r="G255">
-        <f t="shared" ref="G255:G257" si="64">E255+3</f>
+        <f t="shared" ref="G255:G257" si="66">E255+3</f>
         <v>43</v>
       </c>
       <c r="H255" t="s">
@@ -21293,7 +21296,7 @@
         <v>179</v>
       </c>
       <c r="G256">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>43</v>
       </c>
       <c r="H256" t="s">
@@ -21353,7 +21356,7 @@
         <v>199</v>
       </c>
       <c r="G257">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>43</v>
       </c>
       <c r="H257" t="s">
@@ -21401,7 +21404,7 @@
         <v>19</v>
       </c>
       <c r="D258">
-        <f t="shared" ref="D258:D269" si="65">D254</f>
+        <f t="shared" ref="D258:D269" si="67">D254</f>
         <v>89</v>
       </c>
       <c r="E258">
@@ -21409,7 +21412,7 @@
         <v>54</v>
       </c>
       <c r="F258">
-        <f t="shared" ref="F258:F269" si="66">F254</f>
+        <f t="shared" ref="F258:F269" si="68">F254</f>
         <v>135</v>
       </c>
       <c r="G258">
@@ -21461,7 +21464,7 @@
         <v>19</v>
       </c>
       <c r="D259">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>136</v>
       </c>
       <c r="E259">
@@ -21469,7 +21472,7 @@
         <v>55</v>
       </c>
       <c r="F259">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>155</v>
       </c>
       <c r="G259">
@@ -21521,7 +21524,7 @@
         <v>19</v>
       </c>
       <c r="D260">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>155</v>
       </c>
       <c r="E260">
@@ -21529,11 +21532,11 @@
         <v>55</v>
       </c>
       <c r="F260">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>179</v>
       </c>
       <c r="G260">
-        <f t="shared" ref="G260:G261" si="67">E260+3</f>
+        <f t="shared" ref="G260:G261" si="69">E260+3</f>
         <v>58</v>
       </c>
       <c r="H260" t="s">
@@ -21581,7 +21584,7 @@
         <v>19</v>
       </c>
       <c r="D261">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>178</v>
       </c>
       <c r="E261">
@@ -21589,11 +21592,11 @@
         <v>55</v>
       </c>
       <c r="F261">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>199</v>
       </c>
       <c r="G261">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>58</v>
       </c>
       <c r="H261" t="s">
@@ -21641,7 +21644,7 @@
         <v>19</v>
       </c>
       <c r="D262">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>89</v>
       </c>
       <c r="E262">
@@ -21649,7 +21652,7 @@
         <v>69</v>
       </c>
       <c r="F262">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>135</v>
       </c>
       <c r="G262">
@@ -21701,7 +21704,7 @@
         <v>19</v>
       </c>
       <c r="D263">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>136</v>
       </c>
       <c r="E263">
@@ -21709,11 +21712,11 @@
         <v>70</v>
       </c>
       <c r="F263">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>155</v>
       </c>
       <c r="G263">
-        <f t="shared" ref="G263:G265" si="68">E263+3</f>
+        <f t="shared" ref="G263:G265" si="70">E263+3</f>
         <v>73</v>
       </c>
       <c r="H263" t="s">
@@ -21761,7 +21764,7 @@
         <v>19</v>
       </c>
       <c r="D264">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>155</v>
       </c>
       <c r="E264">
@@ -21769,11 +21772,11 @@
         <v>70</v>
       </c>
       <c r="F264">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>179</v>
       </c>
       <c r="G264">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>73</v>
       </c>
       <c r="H264" t="s">
@@ -21821,7 +21824,7 @@
         <v>19</v>
       </c>
       <c r="D265">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>178</v>
       </c>
       <c r="E265">
@@ -21829,11 +21832,11 @@
         <v>70</v>
       </c>
       <c r="F265">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>199</v>
       </c>
       <c r="G265">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>73</v>
       </c>
       <c r="H265" t="s">
@@ -21881,7 +21884,7 @@
         <v>19</v>
       </c>
       <c r="D266">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>89</v>
       </c>
       <c r="E266">
@@ -21889,7 +21892,7 @@
         <v>84</v>
       </c>
       <c r="F266">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>135</v>
       </c>
       <c r="G266">
@@ -21941,7 +21944,7 @@
         <v>19</v>
       </c>
       <c r="D267">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>136</v>
       </c>
       <c r="E267">
@@ -21949,11 +21952,11 @@
         <v>85</v>
       </c>
       <c r="F267">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>155</v>
       </c>
       <c r="G267">
-        <f t="shared" ref="G267:G269" si="69">E267+3</f>
+        <f t="shared" ref="G267:G269" si="71">E267+3</f>
         <v>88</v>
       </c>
       <c r="H267" t="s">
@@ -22001,7 +22004,7 @@
         <v>19</v>
       </c>
       <c r="D268">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>155</v>
       </c>
       <c r="E268">
@@ -22009,11 +22012,11 @@
         <v>85</v>
       </c>
       <c r="F268">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>179</v>
       </c>
       <c r="G268">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>88</v>
       </c>
       <c r="H268" t="s">
@@ -22061,7 +22064,7 @@
         <v>19</v>
       </c>
       <c r="D269">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>178</v>
       </c>
       <c r="E269">
@@ -22069,11 +22072,11 @@
         <v>85</v>
       </c>
       <c r="F269">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>199</v>
       </c>
       <c r="G269">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>88</v>
       </c>
       <c r="H269" t="s">
@@ -22354,7 +22357,7 @@
         <v>19</v>
       </c>
       <c r="D274">
-        <f t="shared" ref="D274" si="70">D277-1</f>
+        <f t="shared" ref="D274" si="72">D277-1</f>
         <v>136</v>
       </c>
       <c r="E274">
@@ -22418,7 +22421,7 @@
         <v>155</v>
       </c>
       <c r="E275">
-        <f t="shared" ref="E275:E276" si="71">E274</f>
+        <f t="shared" ref="E275:E276" si="73">E274</f>
         <v>112</v>
       </c>
       <c r="F275">
@@ -22478,7 +22481,7 @@
         <v>178</v>
       </c>
       <c r="E276">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>112</v>
       </c>
       <c r="F276">
@@ -22486,7 +22489,7 @@
         <v>199</v>
       </c>
       <c r="G276">
-        <f t="shared" ref="G276" si="72">G275</f>
+        <f t="shared" ref="G276" si="74">G275</f>
         <v>117</v>
       </c>
       <c r="H276" t="s">
@@ -22595,11 +22598,11 @@
         <v>156</v>
       </c>
       <c r="E278">
-        <f t="shared" ref="E278:E279" si="73">E277</f>
+        <f t="shared" ref="E278:E279" si="75">E277</f>
         <v>110</v>
       </c>
       <c r="F278">
-        <f t="shared" ref="F278:F279" si="74">D278</f>
+        <f t="shared" ref="F278:F279" si="76">D278</f>
         <v>156</v>
       </c>
       <c r="G278">
@@ -22652,11 +22655,11 @@
         <v>178</v>
       </c>
       <c r="E279">
-        <f t="shared" si="73"/>
+        <f t="shared" si="75"/>
         <v>110</v>
       </c>
       <c r="F279">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>178</v>
       </c>
       <c r="G279">
@@ -22834,7 +22837,7 @@
         <v>155</v>
       </c>
       <c r="G282">
-        <f t="shared" ref="G282:G284" si="75">E282+3</f>
+        <f t="shared" ref="G282:G284" si="77">E282+3</f>
         <v>134</v>
       </c>
       <c r="H282" t="s">
@@ -22894,7 +22897,7 @@
         <v>179</v>
       </c>
       <c r="G283">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>134</v>
       </c>
       <c r="H283" t="s">
@@ -22954,7 +22957,7 @@
         <v>199</v>
       </c>
       <c r="G284">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>134</v>
       </c>
       <c r="H284" t="s">
@@ -28573,11 +28576,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V148"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32583,7 +32586,7 @@
         <v>1453</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>1538</v>
+        <v>1604</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>1538</v>
@@ -32607,7 +32610,7 @@
       <c r="U77" s="8"/>
       <c r="V77" s="8"/>
     </row>
-    <row r="78" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>77</v>
       </c>
@@ -32615,7 +32618,7 @@
         <v>1454</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>1522</v>
+        <v>1605</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>1522</v>
@@ -32843,8 +32846,6 @@
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="8"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
       <c r="H83" s="9"/>
       <c r="I83" s="8"/>
       <c r="J83" s="16"/>
@@ -35739,25 +35740,25 @@
   <conditionalFormatting sqref="B7:B11">
     <cfRule type="duplicateValues" dxfId="7" priority="108"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B82:B83">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B84:B148 B1:B6 B12:B81">
-    <cfRule type="duplicateValues" dxfId="6" priority="136"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="136"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B82:B83">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82:V83 B54:C81 D54:M58 N54:V78 B56:V58 B1:V53">
+  <conditionalFormatting sqref="B1:V53 D54:M58 N54:V78 B54:C81 B56:V58 B82:V83">
     <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L59:M78 D59:K81 L79:V81 D84:E85 H84:V85 E84:K94 B84:C148 D86:D92 N86:V92 L86:M94 D91:E91 H91:V91 D93:V94 E95:M98 D95:D105 N95:V105 D99:V124 D125:D130 M125:M130 N125:V142 E127:K130 L128:L130 D131:M133 D134:K142 D143:V146 D147:K148 N147:V148 L148:M148">
-    <cfRule type="containsBlanks" dxfId="3" priority="19">
-      <formula>LEN(TRIM(B59))=0</formula>
+  <conditionalFormatting sqref="E125:L127 L142:L147">
+    <cfRule type="containsBlanks" dxfId="3" priority="71">
+      <formula>LEN(TRIM(E125))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E125:L127 L142:L147">
-    <cfRule type="containsBlanks" dxfId="2" priority="71">
-      <formula>LEN(TRIM(E125))=0</formula>
+  <conditionalFormatting sqref="L59:M78 D59:K81 L79:V81 D84:E85 H84:V85 E84:K94 B84:C148 D86:D92 N86:V92 L86:M94 D91:E91 H91:V91 D93:V94 E95:M98 D95:D105 N95:V105 D99:V124 D125:D130 M125:M130 N125:V142 E127:K130 L128:L130 D131:M133 D134:K142 D143:V146 D147:K148 N147:V148 L148:M148">
+    <cfRule type="containsBlanks" dxfId="2" priority="19">
+      <formula>LEN(TRIM(B59))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L134:M141">

</xml_diff>

<commit_message>
updated new report template layouts
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6522" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50537D98-BA6A-43C4-A074-693D4EA1D679}"/>
+  <xr:revisionPtr revIDLastSave="6543" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{727B0BFF-E41C-46CC-AD7E-834DB1DFBE80}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -6261,11 +6261,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T332"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E124" sqref="E124"/>
+      <selection pane="bottomRight" activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10386,14 +10386,14 @@
         <v>30</v>
       </c>
       <c r="E70">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F70">
         <v>170</v>
       </c>
       <c r="G70">
-        <f>G73+16</f>
-        <v>169</v>
+        <f>G73+12</f>
+        <v>152</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -10444,8 +10444,8 @@
         <v>40</v>
       </c>
       <c r="E71">
-        <f>E70+16</f>
-        <v>91</v>
+        <f>E70+8</f>
+        <v>93</v>
       </c>
       <c r="F71">
         <f>F70-10</f>
@@ -10453,7 +10453,7 @@
       </c>
       <c r="G71">
         <f>E71+5</f>
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H71" t="s">
         <v>109</v>
@@ -10504,8 +10504,8 @@
         <v>40</v>
       </c>
       <c r="E72">
-        <f>G71+16</f>
-        <v>112</v>
+        <f>G71+8</f>
+        <v>106</v>
       </c>
       <c r="F72">
         <f>F73</f>
@@ -10513,7 +10513,7 @@
       </c>
       <c r="G72">
         <f>E72+8</f>
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H72" t="s">
         <v>109</v>
@@ -10564,22 +10564,22 @@
         <v>40</v>
       </c>
       <c r="E73">
-        <f>G72+16</f>
-        <v>136</v>
+        <f>G72+20</f>
+        <v>134</v>
       </c>
       <c r="F73">
         <f>F71</f>
         <v>160</v>
       </c>
       <c r="G73">
-        <f>E73+17</f>
-        <v>153</v>
+        <f>E73+6</f>
+        <v>140</v>
       </c>
       <c r="H73" t="s">
         <v>109</v>
       </c>
       <c r="I73">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J73">
         <v>1</v>
@@ -10626,15 +10626,15 @@
         <v>30</v>
       </c>
       <c r="E74">
-        <f>G70+16</f>
-        <v>185</v>
+        <f>G70+30</f>
+        <v>182</v>
       </c>
       <c r="F74">
         <v>170</v>
       </c>
       <c r="G74">
-        <f>G77+16</f>
-        <v>279</v>
+        <f>G77+12</f>
+        <v>249</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -10685,8 +10685,8 @@
         <v>40</v>
       </c>
       <c r="E75">
-        <f>E74+16</f>
-        <v>201</v>
+        <f>E74+8</f>
+        <v>190</v>
       </c>
       <c r="F75">
         <f>F74-10</f>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="G75">
         <f>E75+5</f>
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H75" t="s">
         <v>109</v>
@@ -10745,8 +10745,8 @@
         <v>40</v>
       </c>
       <c r="E76">
-        <f>G75+16</f>
-        <v>222</v>
+        <f>G75+8</f>
+        <v>203</v>
       </c>
       <c r="F76">
         <f>F77</f>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="G76">
         <f>E76+8</f>
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="H76" t="s">
         <v>109</v>
@@ -10805,22 +10805,22 @@
         <v>40</v>
       </c>
       <c r="E77">
-        <f>G76+16</f>
-        <v>246</v>
+        <f>G76+20</f>
+        <v>231</v>
       </c>
       <c r="F77">
         <f>F75</f>
         <v>160</v>
       </c>
       <c r="G77">
-        <f>E77+17</f>
-        <v>263</v>
+        <f>E77+6</f>
+        <v>237</v>
       </c>
       <c r="H77" t="s">
         <v>109</v>
       </c>
       <c r="I77">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J77">
         <v>1</v>
@@ -26178,11 +26178,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275ED209-18EA-43FD-841F-C491018348BF}">
   <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50080,10 +50080,10 @@
   <dimension ref="A1:V177"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C106" sqref="C106"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tentative package updates to address #382, #383, #406, #411, #413 (docker rebuild pending availability of new packages, but updated dockerfile in anticipation of this); and minor update towards #367, and help support dev towards this
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6616" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{925DE9D1-E04C-4720-A04C-DFA69E230E9C}"/>
+  <xr:revisionPtr revIDLastSave="6617" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52FEEFD-CEB4-41F8-9F28-C4A2895DFCD4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -5071,9 +5071,6 @@
     <t xml:space="preserve">Edit the 'Demographics and health equity' section of the region configuration file to highlight socio-economic demographic characteristics and key health challenges and inequities present in this urban area. </t>
   </si>
   <si>
-    <t>Environmental hazards that may impact the urban area over the coming decade may include: {policy_checklist_hazards}.</t>
-  </si>
-  <si>
     <t>context</t>
   </si>
   <si>
@@ -5180,6 +5177,9 @@
   </si>
   <si>
     <t>Policy checklist data could not be loaded and have been skipped.  See https://healthysustainablecities.github.io/software/#Policy-checklist</t>
+  </si>
+  <si>
+    <t>Environmental hazards that may impact the urban area over the coming decade include: {policy_checklist_hazards}.</t>
   </si>
 </sst>
 </file>
@@ -9371,7 +9371,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -9543,7 +9543,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B56">
         <v>-999</v>
@@ -9576,7 +9576,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="O56" t="s">
         <v>25</v>
@@ -9596,7 +9596,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -9651,7 +9651,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -9711,7 +9711,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -9772,7 +9772,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -9833,7 +9833,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -9890,7 +9890,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -9947,7 +9947,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -19714,7 +19714,7 @@
         <v>0</v>
       </c>
       <c r="M225" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="N225" t="s">
         <v>21</v>
@@ -28961,7 +28961,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -29130,7 +29130,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B55">
         <v>-999</v>
@@ -29163,7 +29163,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="O55" t="s">
         <v>25</v>
@@ -29183,7 +29183,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -29238,7 +29238,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -29294,7 +29294,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -29351,7 +29351,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -29408,7 +29408,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -29465,7 +29465,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -29522,7 +29522,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -29752,7 +29752,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -29792,7 +29792,7 @@
         <v>25</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="Q66">
         <v>1</v>
@@ -32077,7 +32077,7 @@
         <v>0</v>
       </c>
       <c r="M105" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="N105" t="s">
         <v>21</v>
@@ -49465,7 +49465,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50002,10 +50002,10 @@
         <v>77</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1672</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>1673</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
@@ -50403,7 +50403,7 @@
         <v>1291</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1638</v>
+        <v>1673</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -50577,13 +50577,13 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -50607,13 +50607,13 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>1639</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>1640</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -50637,13 +50637,13 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -50667,13 +50667,13 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -50697,13 +50697,13 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -50727,13 +50727,13 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -50757,13 +50757,13 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -50787,13 +50787,13 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -50817,13 +50817,13 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -50847,13 +50847,13 @@
     </row>
     <row r="37" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>1560</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -50877,13 +50877,13 @@
     </row>
     <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -50910,10 +50910,10 @@
         <v>78</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -50940,10 +50940,10 @@
         <v>78</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -50970,10 +50970,10 @@
         <v>78</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -51000,10 +51000,10 @@
         <v>78</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -51030,10 +51030,10 @@
         <v>78</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -54372,10 +54372,10 @@
         <v>77</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="8"/>
@@ -57341,7 +57341,7 @@
         <v>1490</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>1491</v>
@@ -57366,7 +57366,7 @@
         <v>1492</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>1493</v>
@@ -57380,7 +57380,7 @@
         <v>566</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>562</v>

</xml_diff>

<commit_message>
updated access profile image, including refactoring code for easier generation of image (to support dev work, but now for users generally --- can generate access profile direclty as r.access_profile(); also experimnted with adding a plot() helper function that could have a niche use, used as r.plot(plot='access_profile') --- its more wordy, but if run without any command, it lists the various plot types available and how to run them, and allows passing of keyword arguments.  The access profile legend is not centered under plot, in spirit of #367.  To allow this, plot is now 10cm x 8 cm (extra height for legend space).  The interquartile range has been added to legend too, along with '(Box 1)' reference.
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6617" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52FEEFD-CEB4-41F8-9F28-C4A2895DFCD4}"/>
+  <xr:revisionPtr revIDLastSave="6626" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0017A7-3ABB-45B3-8B91-D266109FB365}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="1674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="1676">
   <si>
     <t>name</t>
   </si>
@@ -5180,6 +5180,16 @@
   </si>
   <si>
     <t>Environmental hazards that may impact the urban area over the coming decade include: {policy_checklist_hazards}.</t>
+  </si>
+  <si>
+    <t>% of
+population
+with access
+within 500m
+to:</t>
+  </si>
+  <si>
+    <t>Median and interquartile range for 25 cities internationally (Box 1)</t>
   </si>
 </sst>
 </file>
@@ -6248,11 +6258,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T328"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13131,14 +13141,14 @@
       </c>
       <c r="E116">
         <f>G118+8</f>
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="F116">
         <v>208</v>
       </c>
       <c r="G116">
         <f>E116+8</f>
-        <v>248</v>
+        <v>293</v>
       </c>
       <c r="H116" t="s">
         <v>109</v>
@@ -13251,8 +13261,8 @@
         <v>196</v>
       </c>
       <c r="G118">
-        <f>E118+(F118-D118)</f>
-        <v>232</v>
+        <f>INT(E118+(F118-D118)/80*100)</f>
+        <v>277</v>
       </c>
       <c r="H118" t="s">
         <v>109</v>
@@ -25925,10 +25935,10 @@
   <dimension ref="A1:T124"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30405,8 +30415,8 @@
         <v>196</v>
       </c>
       <c r="G77">
-        <f>E77+(F77-D77)</f>
-        <v>215</v>
+        <f>INT(E77+(F77-D77)/80*100)</f>
+        <v>260</v>
       </c>
       <c r="H77" t="s">
         <v>109</v>
@@ -30512,14 +30522,14 @@
       </c>
       <c r="E79">
         <f>G77</f>
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="F79">
         <v>196</v>
       </c>
       <c r="G79">
         <f>E79+5</f>
-        <v>220</v>
+        <v>265</v>
       </c>
       <c r="H79" t="s">
         <v>109</v>
@@ -30570,14 +30580,14 @@
       </c>
       <c r="E80">
         <f>G79+8</f>
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="F80">
         <v>196</v>
       </c>
       <c r="G80">
         <f>E80+5</f>
-        <v>233</v>
+        <v>278</v>
       </c>
       <c r="H80" t="s">
         <v>109</v>
@@ -49461,11 +49471,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52343,7 +52353,7 @@
         <v>96</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1504</v>
+        <v>1674</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>1504</v>
@@ -52527,7 +52537,7 @@
       <c r="U70" s="8"/>
       <c r="V70" s="8"/>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>78</v>
       </c>
@@ -52535,7 +52545,7 @@
         <v>110</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>346</v>
+        <v>1675</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>346</v>

</xml_diff>

<commit_message>
updated report citation and file name towards #367
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6626" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0017A7-3ABB-45B3-8B91-D266109FB365}"/>
+  <xr:revisionPtr revIDLastSave="6635" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B713A6-D4F4-43C0-9631-36287A5EBCE4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -5059,9 +5059,6 @@
     <t>Box 1: The Lancet Global Health Series study of 25 cities internationally</t>
   </si>
   <si>
-    <t>A 1000 Cities Challenge report</t>
-  </si>
-  <si>
     <t>Levels of government</t>
   </si>
   <si>
@@ -5190,6 +5187,9 @@
   </si>
   <si>
     <t>Median and interquartile range for 25 cities internationally (Box 1)</t>
+  </si>
+  <si>
+    <t>1000 Cities Challenge report</t>
   </si>
 </sst>
 </file>
@@ -6258,8 +6258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T328"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G118" sqref="G118"/>
@@ -9381,7 +9381,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -9553,7 +9553,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B56">
         <v>-999</v>
@@ -9586,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="O56" t="s">
         <v>25</v>
@@ -9606,7 +9606,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -9661,7 +9661,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -9721,7 +9721,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -9782,7 +9782,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -9900,7 +9900,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -9957,7 +9957,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -19724,7 +19724,7 @@
         <v>0</v>
       </c>
       <c r="M225" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="N225" t="s">
         <v>21</v>
@@ -28971,7 +28971,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -29140,7 +29140,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B55">
         <v>-999</v>
@@ -29173,7 +29173,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="O55" t="s">
         <v>25</v>
@@ -29193,7 +29193,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -29248,7 +29248,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -29304,7 +29304,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -29361,7 +29361,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -29418,7 +29418,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -29475,7 +29475,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -29532,7 +29532,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -29762,7 +29762,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -29802,7 +29802,7 @@
         <v>25</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="Q66">
         <v>1</v>
@@ -32087,7 +32087,7 @@
         <v>0</v>
       </c>
       <c r="M105" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="N105" t="s">
         <v>21</v>
@@ -49471,11 +49471,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V178"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E64" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49823,7 +49823,7 @@
         <v>228</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1634</v>
+        <v>1675</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1511</v>
@@ -50012,10 +50012,10 @@
         <v>77</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1671</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>1672</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
@@ -50233,7 +50233,7 @@
         <v>1286</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -50323,7 +50323,7 @@
         <v>1285</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -50383,7 +50383,7 @@
         <v>1289</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -50413,7 +50413,7 @@
         <v>1291</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -50587,13 +50587,13 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -50617,13 +50617,13 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>1638</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>1639</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -50647,13 +50647,13 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -50677,13 +50677,13 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -50707,13 +50707,13 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -50737,13 +50737,13 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -50767,13 +50767,13 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -50797,13 +50797,13 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -50827,13 +50827,13 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -50857,13 +50857,13 @@
     </row>
     <row r="37" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>1560</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -50887,13 +50887,13 @@
     </row>
     <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -50920,10 +50920,10 @@
         <v>78</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -50950,10 +50950,10 @@
         <v>78</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -50980,10 +50980,10 @@
         <v>78</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -51010,10 +51010,10 @@
         <v>78</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -51040,10 +51040,10 @@
         <v>78</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -52353,7 +52353,7 @@
         <v>96</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>1504</v>
@@ -52545,7 +52545,7 @@
         <v>110</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>346</v>
@@ -54382,10 +54382,10 @@
         <v>77</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="8"/>
@@ -57351,7 +57351,7 @@
         <v>1490</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>1491</v>
@@ -57376,7 +57376,7 @@
         <v>1492</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>1493</v>
@@ -57390,7 +57390,7 @@
         <v>566</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>562</v>

</xml_diff>

<commit_message>
made names for disasters in English lower case
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8986" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34FEC520-5C13-4E38-B4EC-ADD247E582CB}"/>
+  <xr:revisionPtr revIDLastSave="8990" documentId="114_{57517418-E3A8-4D24-9644-27D04334BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E73745-08E2-417E-A5E7-97ECC830B987}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9944" uniqueCount="5098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9944" uniqueCount="5107">
   <si>
     <t>name</t>
   </si>
@@ -15381,6 +15381,33 @@
   </si>
   <si>
     <t>김지윤, 하재현</t>
+  </si>
+  <si>
+    <t>severe storms</t>
+  </si>
+  <si>
+    <t>floods</t>
+  </si>
+  <si>
+    <t>bushfires/wildfires</t>
+  </si>
+  <si>
+    <t>heatwaves</t>
+  </si>
+  <si>
+    <t>extreme cold</t>
+  </si>
+  <si>
+    <t>typhoons</t>
+  </si>
+  <si>
+    <t>hurricanes</t>
+  </si>
+  <si>
+    <t>cyclones</t>
+  </si>
+  <si>
+    <t>earthquakes</t>
   </si>
 </sst>
 </file>
@@ -59748,10 +59775,10 @@
   <dimension ref="A1:AG164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62700,7 +62727,7 @@
         <v>1014</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1014</v>
+        <v>5098</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>3038</v>
@@ -62801,7 +62828,7 @@
         <v>1006</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1006</v>
+        <v>5099</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>3039</v>
@@ -62902,7 +62929,7 @@
         <v>1007</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1007</v>
+        <v>5100</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>3040</v>
@@ -63003,7 +63030,7 @@
         <v>1008</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1008</v>
+        <v>5101</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>3041</v>
@@ -63104,7 +63131,7 @@
         <v>1009</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1009</v>
+        <v>5102</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>3042</v>
@@ -63205,7 +63232,7 @@
         <v>1010</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1010</v>
+        <v>5103</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>3043</v>
@@ -63298,7 +63325,7 @@
         <v>4758</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>1005</v>
       </c>
@@ -63306,7 +63333,7 @@
         <v>1011</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1011</v>
+        <v>5104</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>3043</v>
@@ -63399,7 +63426,7 @@
         <v>4759</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>1005</v>
       </c>
@@ -63407,7 +63434,7 @@
         <v>1012</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1012</v>
+        <v>5105</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>3043</v>
@@ -63508,7 +63535,7 @@
         <v>1013</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1013</v>
+        <v>5106</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>3044</v>

</xml_diff>

<commit_message>
made sketch configuration gui able to handle lack of exceptions for specified languages
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A1EB00C-1ED7-49BD-84BB-F607FAF99466}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A3BEA3E-2177-44B8-A57E-CC05C194938F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59775,7 +59775,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59896,7 +59896,7 @@
         <v>183</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>3185</v>

</xml_diff>

<commit_message>
enhancements to address #478, specifically addressing correct shaping of Arabic and Persian text when producing matplotlib plots.
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A12F4CD4-4F39-4109-B822-7EBDA6728925}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3498787-AD8E-40BB-A68E-CF39D39D54D0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Translation Sign-off'!$A$4:$H$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -15559,9 +15558,6 @@
     <t>  {city_name} मा जनसङ्ख्याको {percent} अन्तर्राष्ट्रिय रूपमा २५ सहरहरूको औसतभन्दा माथि हिड्ने क्षमता स्कोरिङ भएको छिमेकमा बस्छन् (बक्स १)</t>
   </si>
   <si>
-    <t>{percent} از جمعیت شهر {city_name} در محله‌هایی زندگی می‌کنند که امتیاز پیاده‌پذیری آن‌ها بالاتر از {عدد} میانه ۲۵ شهر در سطح بین‌المللی است (کادر 1)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {percent} da população de {city_name} que vive em bairros com pontuação de caminhabilidade acima da mediana de 25 cidades em todo o mundo (Quadro 1)</t>
   </si>
   <si>
@@ -15689,7 +15685,10 @@
     <t>Amal Al Siyabi</t>
   </si>
   <si>
-    <t>أمل السيايب</t>
+    <t>أمل  السيابية</t>
+  </si>
+  <si>
+    <t>{percent} از جمعیت شهر {city_name} در محله‌هایی زندگی می‌کنند که امتیاز پیاده‌پذیری آن‌ها بالاتر از میانه ۲۵ شهر در سطح بین‌المللی است (کادر ۱)</t>
   </si>
 </sst>
 </file>
@@ -16329,7 +16328,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -16453,6 +16452,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -36551,10 +36553,10 @@
   <dimension ref="A1:T122"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60785,7 +60787,7 @@
         <v>999</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>5191</v>
+        <v>5190</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>4748</v>
@@ -62401,7 +62403,7 @@
         <v>1047</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>5192</v>
+        <v>5191</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1210</v>
@@ -66905,34 +66907,34 @@
         <v>5155</v>
       </c>
       <c r="X68" s="44" t="s">
+        <v>5199</v>
+      </c>
+      <c r="Y68" s="3" t="s">
         <v>5156</v>
       </c>
-      <c r="Y68" s="3" t="s">
+      <c r="Z68" s="3" t="s">
         <v>5157</v>
       </c>
-      <c r="Z68" s="3" t="s">
+      <c r="AA68" s="3" t="s">
         <v>5158</v>
       </c>
-      <c r="AA68" s="3" t="s">
+      <c r="AB68" s="3" t="s">
         <v>5159</v>
       </c>
-      <c r="AB68" s="3" t="s">
+      <c r="AC68" s="3" t="s">
         <v>5160</v>
       </c>
-      <c r="AC68" s="3" t="s">
+      <c r="AD68" s="3" t="s">
         <v>5161</v>
       </c>
-      <c r="AD68" s="3" t="s">
+      <c r="AE68" s="3" t="s">
         <v>5162</v>
       </c>
-      <c r="AE68" s="3" t="s">
+      <c r="AF68" s="3" t="s">
         <v>5163</v>
       </c>
-      <c r="AF68" s="3" t="s">
+      <c r="AG68" s="3" t="s">
         <v>5164</v>
-      </c>
-      <c r="AG68" s="3" t="s">
-        <v>5165</v>
       </c>
     </row>
     <row r="69" spans="1:33" ht="105" x14ac:dyDescent="0.25">
@@ -66997,7 +66999,7 @@
         <v>3707</v>
       </c>
       <c r="U69" s="3" t="s">
-        <v>5166</v>
+        <v>5165</v>
       </c>
       <c r="V69" s="3" t="s">
         <v>3365</v>
@@ -68054,64 +68056,64 @@
         <v>968</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>5167</v>
+        <v>5166</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>3040</v>
       </c>
       <c r="E80" s="8" t="s">
+        <v>5167</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>5170</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>5171</v>
+      </c>
+      <c r="H80" s="16" t="s">
+        <v>5172</v>
+      </c>
+      <c r="I80" s="8" t="s">
+        <v>5169</v>
+      </c>
+      <c r="J80" s="16" t="s">
         <v>5168</v>
       </c>
-      <c r="F80" s="9" t="s">
-        <v>5171</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>5172</v>
-      </c>
-      <c r="H80" s="16" t="s">
+      <c r="K80" s="20" t="s">
         <v>5173</v>
       </c>
-      <c r="I80" s="8" t="s">
-        <v>5170</v>
-      </c>
-      <c r="J80" s="16" t="s">
-        <v>5169</v>
-      </c>
-      <c r="K80" s="20" t="s">
+      <c r="L80" s="8" t="s">
         <v>5174</v>
-      </c>
-      <c r="L80" s="8" t="s">
-        <v>5175</v>
       </c>
       <c r="M80" s="8" t="s">
         <v>3544</v>
       </c>
       <c r="N80" s="8" t="s">
+        <v>5175</v>
+      </c>
+      <c r="O80" s="8" t="s">
         <v>5176</v>
       </c>
-      <c r="O80" s="8" t="s">
+      <c r="P80" s="8" t="s">
         <v>5177</v>
-      </c>
-      <c r="P80" s="8" t="s">
-        <v>5178</v>
       </c>
       <c r="Q80" s="8" t="s">
         <v>3155</v>
       </c>
       <c r="R80" s="8" t="s">
+        <v>5178</v>
+      </c>
+      <c r="S80" s="8" t="s">
         <v>5179</v>
       </c>
-      <c r="S80" s="8" t="s">
+      <c r="T80" s="3" t="s">
         <v>5180</v>
       </c>
-      <c r="T80" s="3" t="s">
+      <c r="U80" s="3" t="s">
         <v>5181</v>
       </c>
-      <c r="U80" s="3" t="s">
+      <c r="V80" s="3" t="s">
         <v>5182</v>
-      </c>
-      <c r="V80" s="3" t="s">
-        <v>5183</v>
       </c>
       <c r="W80" s="3" t="s">
         <v>2849</v>
@@ -68120,16 +68122,16 @@
         <v>4579</v>
       </c>
       <c r="Y80" s="3" t="s">
+        <v>5183</v>
+      </c>
+      <c r="Z80" s="3" t="s">
         <v>5184</v>
       </c>
-      <c r="Z80" s="3" t="s">
+      <c r="AA80" s="3" t="s">
         <v>5185</v>
       </c>
-      <c r="AA80" s="3" t="s">
+      <c r="AB80" s="3" t="s">
         <v>5186</v>
-      </c>
-      <c r="AB80" s="3" t="s">
-        <v>5187</v>
       </c>
       <c r="AC80" s="3" t="s">
         <v>1986</v>
@@ -68138,13 +68140,13 @@
         <v>4342</v>
       </c>
       <c r="AE80" s="3" t="s">
+        <v>5187</v>
+      </c>
+      <c r="AF80" s="3" t="s">
         <v>5188</v>
       </c>
-      <c r="AF80" s="3" t="s">
+      <c r="AG80" s="3" t="s">
         <v>5189</v>
-      </c>
-      <c r="AG80" s="3" t="s">
-        <v>5190</v>
       </c>
     </row>
     <row r="81" spans="1:33" ht="45" x14ac:dyDescent="0.25">
@@ -68461,7 +68463,7 @@
         <v>986</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>5193</v>
+        <v>5192</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>5029</v>
@@ -69269,7 +69271,7 @@
         <v>948</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>5194</v>
+        <v>5193</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>4755</v>
@@ -69471,7 +69473,7 @@
         <v>953</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>5195</v>
+        <v>5194</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>5026</v>
@@ -69572,7 +69574,7 @@
         <v>975</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>5196</v>
+        <v>5195</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>4757</v>
@@ -73814,7 +73816,7 @@
         <v>958</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>5197</v>
+        <v>5196</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>1266</v>
@@ -74217,7 +74219,7 @@
       <c r="C141" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D141" s="11" t="s">
+      <c r="D141" s="46" t="s">
         <v>3094</v>
       </c>
       <c r="E141" s="11" t="s">
@@ -74621,7 +74623,7 @@
       <c r="C145" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D145" s="11" t="s">
+      <c r="D145" s="46" t="s">
         <v>3098</v>
       </c>
       <c r="E145" s="11" t="s">
@@ -76841,7 +76843,7 @@
         <v>383</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>5199</v>
+        <v>5198</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>671</v>
@@ -76932,7 +76934,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76947,16 +76949,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>2174</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -76968,42 +76970,42 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>3346</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>1055</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>3124</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>3127</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48" t="s">
         <v>4744</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="48" t="s">
         <v>3129</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="48" t="s">
         <v>4745</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="41" t="s">
         <v>3128</v>
       </c>
       <c r="E3" s="41" t="s">
         <v>3130</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
@@ -77035,10 +77037,10 @@
         <v>4636</v>
       </c>
       <c r="G5" s="29" t="s">
+        <v>5197</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>5198</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>5199</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated report generation implementation for #567
</commit_message>
<xml_diff>
--- a/process/configuration/templates/_report_configuration.xlsx
+++ b/process/configuration/templates/_report_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8710D541-4BFA-40E9-ADBA-B03B56B8C7E9}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="13_ncr:1_{974DC119-FBC5-4146-98A2-4FA425A99853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2CB6AE8-3DF6-4959-82E0-3ED1F9FAED3F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy_spatial" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10081" uniqueCount="5205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10132" uniqueCount="5214">
   <si>
     <t>name</t>
   </si>
@@ -15703,7 +15703,34 @@
     <t>Tree canopy and urban greening</t>
   </si>
   <si>
-    <t>Climate disaster risk reduction policies</t>
+    <t>Adaptation and disaster risk reduction</t>
+  </si>
+  <si>
+    <t>policy_checklist7_title</t>
+  </si>
+  <si>
+    <t>policy_checklist7_text1</t>
+  </si>
+  <si>
+    <t>policy_checklist7_text1_response1</t>
+  </si>
+  <si>
+    <t>policy_checklist7_text1_response2</t>
+  </si>
+  <si>
+    <t>policy_checklist7_text1_response3</t>
+  </si>
+  <si>
+    <t>policy_checklist6_text2</t>
+  </si>
+  <si>
+    <t>policy_checklist6_text2_response1</t>
+  </si>
+  <si>
+    <t>policy_checklist6_text2_response2</t>
+  </si>
+  <si>
+    <t>policy_checklist6_text2_response3</t>
   </si>
 </sst>
 </file>
@@ -35000,7 +35027,7 @@
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>889</v>
+        <v>5205</v>
       </c>
       <c r="B304">
         <v>19</v>
@@ -35543,7 +35570,7 @@
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>890</v>
+        <v>5206</v>
       </c>
       <c r="B313">
         <v>19</v>
@@ -35604,7 +35631,7 @@
     </row>
     <row r="314" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>891</v>
+        <v>5207</v>
       </c>
       <c r="B314">
         <v>19</v>
@@ -35665,7 +35692,7 @@
     </row>
     <row r="315" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>892</v>
+        <v>5208</v>
       </c>
       <c r="B315">
         <v>19</v>
@@ -35726,7 +35753,7 @@
     </row>
     <row r="316" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>893</v>
+        <v>5209</v>
       </c>
       <c r="B316">
         <v>19</v>
@@ -43737,13 +43764,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157E4220-B397-4E83-B139-F607B348A6E7}">
-  <dimension ref="A1:T272"/>
+  <dimension ref="A1:T282"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D241" sqref="D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56772,14 +56799,14 @@
         <v>0</v>
       </c>
       <c r="E218">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F218">
         <v>210</v>
       </c>
       <c r="G218">
-        <f>G243+15</f>
-        <v>213</v>
+        <f>G235+15</f>
+        <v>148</v>
       </c>
       <c r="I218">
         <v>0</v>
@@ -56831,14 +56858,14 @@
       </c>
       <c r="E219">
         <f>E218+5</f>
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="F219">
         <v>196</v>
       </c>
       <c r="G219">
         <f>E219+3</f>
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="H219" t="s">
         <v>102</v>
@@ -56856,7 +56883,7 @@
         <v>0</v>
       </c>
       <c r="N219" t="str">
-        <f t="shared" ref="N219:N243" si="56">$N$76</f>
+        <f t="shared" ref="N219:N253" si="56">$N$76</f>
         <v>d0d8dd</v>
       </c>
       <c r="O219" t="s">
@@ -56891,7 +56918,7 @@
       </c>
       <c r="E220">
         <f>E218+2</f>
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="F220">
         <f>D224-1</f>
@@ -56899,7 +56926,7 @@
       </c>
       <c r="G220">
         <f>E220+5</f>
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H220" t="s">
         <v>102</v>
@@ -56952,7 +56979,7 @@
       </c>
       <c r="E221">
         <f t="shared" ref="E221:E225" si="58">E220</f>
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="F221">
         <f>D225+1</f>
@@ -56960,7 +56987,7 @@
       </c>
       <c r="G221">
         <f>G220</f>
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H221" t="s">
         <v>102</v>
@@ -57013,7 +57040,7 @@
       </c>
       <c r="E222">
         <f t="shared" si="58"/>
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="F222">
         <f>D222+26</f>
@@ -57021,7 +57048,7 @@
       </c>
       <c r="G222">
         <f t="shared" ref="G222" si="59">G221</f>
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H222" t="s">
         <v>102</v>
@@ -57073,7 +57100,7 @@
       </c>
       <c r="E223">
         <f>E218</f>
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F223">
         <f>D223</f>
@@ -57081,7 +57108,7 @@
       </c>
       <c r="G223">
         <f>G218</f>
-        <v>213</v>
+        <v>148</v>
       </c>
       <c r="I223">
         <v>0.5</v>
@@ -57134,7 +57161,7 @@
       </c>
       <c r="E224">
         <f t="shared" si="58"/>
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F224">
         <f t="shared" ref="F224:F225" si="60">D224</f>
@@ -57142,7 +57169,7 @@
       </c>
       <c r="G224">
         <f>G223</f>
-        <v>213</v>
+        <v>148</v>
       </c>
       <c r="I224">
         <v>0.5</v>
@@ -57195,7 +57222,7 @@
       </c>
       <c r="E225">
         <f t="shared" si="58"/>
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F225">
         <f t="shared" si="60"/>
@@ -57203,7 +57230,7 @@
       </c>
       <c r="G225">
         <f>G224</f>
-        <v>213</v>
+        <v>148</v>
       </c>
       <c r="I225">
         <v>0.5</v>
@@ -57255,14 +57282,14 @@
       </c>
       <c r="E226">
         <f>E220+25</f>
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="F226">
         <v>196</v>
       </c>
       <c r="G226">
         <f>E226</f>
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="I226">
         <v>0.5</v>
@@ -57314,14 +57341,14 @@
       </c>
       <c r="E227">
         <f>G218+2</f>
-        <v>215</v>
+        <v>150</v>
       </c>
       <c r="F227">
         <v>196</v>
       </c>
       <c r="G227">
         <f>E227+4</f>
-        <v>219</v>
+        <v>154</v>
       </c>
       <c r="H227" t="s">
         <v>102</v>
@@ -57372,7 +57399,7 @@
       </c>
       <c r="E228">
         <f>E226+2</f>
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="F228">
         <f>D223-2</f>
@@ -57380,7 +57407,7 @@
       </c>
       <c r="G228">
         <f>E228+5</f>
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="H228" t="s">
         <v>102</v>
@@ -57433,7 +57460,7 @@
       </c>
       <c r="E229">
         <f>E228+1</f>
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F229">
         <f>F220</f>
@@ -57441,7 +57468,7 @@
       </c>
       <c r="G229">
         <f t="shared" ref="G229:G231" si="61">E229+3</f>
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="H229" t="s">
         <v>20</v>
@@ -57494,7 +57521,7 @@
       </c>
       <c r="E230">
         <f>E229</f>
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F230">
         <f>F221</f>
@@ -57502,7 +57529,7 @@
       </c>
       <c r="G230">
         <f t="shared" si="61"/>
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="H230" t="s">
         <v>20</v>
@@ -57555,7 +57582,7 @@
       </c>
       <c r="E231">
         <f>E230</f>
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F231">
         <f>F222</f>
@@ -57563,7 +57590,7 @@
       </c>
       <c r="G231">
         <f t="shared" si="61"/>
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="H231" t="s">
         <v>20</v>
@@ -57611,20 +57638,20 @@
         <v>19</v>
       </c>
       <c r="D232">
-        <f t="shared" ref="D232:D243" si="62">D228</f>
+        <f t="shared" ref="D232:D235" si="62">D228</f>
         <v>14</v>
       </c>
       <c r="E232">
         <f>E228+15</f>
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="F232">
-        <f t="shared" ref="F232:F243" si="63">F228</f>
+        <f t="shared" ref="F232:F235" si="63">F228</f>
         <v>112</v>
       </c>
       <c r="G232">
         <f>E232+5</f>
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="H232" t="s">
         <v>102</v>
@@ -57677,7 +57704,7 @@
       </c>
       <c r="E233">
         <f>E232+1</f>
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F233">
         <f t="shared" si="63"/>
@@ -57685,7 +57712,7 @@
       </c>
       <c r="G233">
         <f>E233+3</f>
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="H233" t="s">
         <v>20</v>
@@ -57738,7 +57765,7 @@
       </c>
       <c r="E234">
         <f>E233</f>
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F234">
         <f t="shared" si="63"/>
@@ -57746,7 +57773,7 @@
       </c>
       <c r="G234">
         <f t="shared" ref="G234:G235" si="64">E234+3</f>
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="H234" t="s">
         <v>20</v>
@@ -57799,7 +57826,7 @@
       </c>
       <c r="E235">
         <f>E234</f>
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F235">
         <f t="shared" si="63"/>
@@ -57807,7 +57834,7 @@
       </c>
       <c r="G235">
         <f t="shared" si="64"/>
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="H235" t="s">
         <v>20</v>
@@ -57846,38 +57873,32 @@
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>857</v>
+        <v>888</v>
       </c>
       <c r="B236">
         <v>10</v>
       </c>
       <c r="C236" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D236">
-        <f t="shared" si="62"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E236">
-        <f>E232+15</f>
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="F236">
-        <f t="shared" si="63"/>
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="G236">
-        <f>E236+5</f>
-        <v>184</v>
-      </c>
-      <c r="H236" t="s">
-        <v>102</v>
+        <f>G253+15</f>
+        <v>253</v>
       </c>
       <c r="I236">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J236">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K236">
         <v>0</v>
@@ -57885,18 +57906,21 @@
       <c r="L236">
         <v>0</v>
       </c>
-      <c r="N236" t="str">
-        <f t="shared" si="56"/>
+      <c r="M236" t="str">
+        <f>$N$76</f>
         <v>d0d8dd</v>
+      </c>
+      <c r="N236" t="s">
+        <v>928</v>
       </c>
       <c r="O236" t="s">
         <v>25</v>
       </c>
       <c r="Q236">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S236" t="s">
         <v>119</v>
@@ -57907,7 +57931,7 @@
     </row>
     <row r="237" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>858</v>
+        <v>889</v>
       </c>
       <c r="B237">
         <v>10</v>
@@ -57916,26 +57940,24 @@
         <v>19</v>
       </c>
       <c r="D237">
-        <f t="shared" si="62"/>
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="E237">
-        <f>E236+1</f>
-        <v>180</v>
+        <f>E236+5</f>
+        <v>195</v>
       </c>
       <c r="F237">
-        <f t="shared" si="63"/>
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="G237">
-        <f t="shared" ref="G237:G239" si="65">E237+3</f>
-        <v>183</v>
+        <f>E237+3</f>
+        <v>198</v>
       </c>
       <c r="H237" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="I237">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J237">
         <v>1</v>
@@ -57951,10 +57973,10 @@
         <v>d0d8dd</v>
       </c>
       <c r="O237" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R237" t="b">
         <v>0</v>
@@ -57968,7 +57990,7 @@
     </row>
     <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>859</v>
+        <v>774</v>
       </c>
       <c r="B238">
         <v>10</v>
@@ -57977,26 +57999,26 @@
         <v>19</v>
       </c>
       <c r="D238">
-        <f t="shared" si="62"/>
+        <f t="shared" ref="D238" si="65">D241-1</f>
+        <v>113</v>
+      </c>
+      <c r="E238">
+        <f>E236+2</f>
+        <v>192</v>
+      </c>
+      <c r="F238">
+        <f>D242-1</f>
         <v>140</v>
       </c>
-      <c r="E238">
-        <f>E237</f>
-        <v>180</v>
-      </c>
-      <c r="F238">
-        <f t="shared" si="63"/>
-        <v>169</v>
-      </c>
       <c r="G238">
-        <f t="shared" si="65"/>
-        <v>183</v>
+        <f>E238+5</f>
+        <v>197</v>
       </c>
       <c r="H238" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="I238">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J238">
         <v>1</v>
@@ -58015,10 +58037,10 @@
         <v>27</v>
       </c>
       <c r="Q238">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R238" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S238" t="s">
         <v>119</v>
@@ -58029,7 +58051,7 @@
     </row>
     <row r="239" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>860</v>
+        <v>775</v>
       </c>
       <c r="B239">
         <v>10</v>
@@ -58038,26 +58060,26 @@
         <v>19</v>
       </c>
       <c r="D239">
-        <f t="shared" si="62"/>
-        <v>168</v>
+        <f>D242-1</f>
+        <v>140</v>
       </c>
       <c r="E239">
-        <f>E238</f>
-        <v>180</v>
+        <f t="shared" ref="E239:E243" si="66">E238</f>
+        <v>192</v>
       </c>
       <c r="F239">
-        <f t="shared" si="63"/>
-        <v>194</v>
+        <f>D243+1</f>
+        <v>169</v>
       </c>
       <c r="G239">
-        <f t="shared" si="65"/>
-        <v>183</v>
+        <f>G238</f>
+        <v>197</v>
       </c>
       <c r="H239" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="I239">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J239">
         <v>1</v>
@@ -58076,10 +58098,10 @@
         <v>27</v>
       </c>
       <c r="Q239">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R239" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S239" t="s">
         <v>119</v>
@@ -58090,7 +58112,7 @@
     </row>
     <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>861</v>
+        <v>776</v>
       </c>
       <c r="B240">
         <v>10</v>
@@ -58099,29 +58121,29 @@
         <v>19</v>
       </c>
       <c r="D240">
-        <f t="shared" si="62"/>
-        <v>14</v>
+        <f>D243</f>
+        <v>168</v>
       </c>
       <c r="E240">
-        <f>E236+15</f>
+        <f t="shared" si="66"/>
+        <v>192</v>
+      </c>
+      <c r="F240">
+        <f>D240+26</f>
         <v>194</v>
       </c>
-      <c r="F240">
-        <f t="shared" si="63"/>
-        <v>112</v>
-      </c>
       <c r="G240">
-        <f>E240+5</f>
-        <v>199</v>
+        <f t="shared" ref="G240" si="67">G239</f>
+        <v>197</v>
       </c>
       <c r="H240" t="s">
         <v>102</v>
       </c>
       <c r="I240">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J240">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K240">
         <v>0</v>
@@ -58134,7 +58156,7 @@
         <v>d0d8dd</v>
       </c>
       <c r="O240" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q240">
         <v>3</v>
@@ -58151,54 +58173,53 @@
     </row>
     <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>862</v>
+        <v>44</v>
       </c>
       <c r="B241">
         <v>10</v>
       </c>
       <c r="C241" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D241">
-        <f t="shared" si="62"/>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E241">
-        <f>E240+1</f>
-        <v>195</v>
+        <f>E236</f>
+        <v>190</v>
       </c>
       <c r="F241">
-        <f t="shared" si="63"/>
-        <v>140</v>
+        <f>D241</f>
+        <v>114</v>
       </c>
       <c r="G241">
-        <f t="shared" ref="G241:G243" si="66">E241+3</f>
-        <v>198</v>
-      </c>
-      <c r="H241" t="s">
-        <v>20</v>
+        <f>G236</f>
+        <v>253</v>
       </c>
       <c r="I241">
-        <v>16</v>
+        <v>0.5</v>
       </c>
       <c r="J241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K241">
         <v>0</v>
       </c>
       <c r="L241">
         <v>0</v>
+      </c>
+      <c r="M241" t="s">
+        <v>21</v>
       </c>
       <c r="N241" t="str">
         <f t="shared" si="56"/>
         <v>d0d8dd</v>
       </c>
       <c r="O241" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q241">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R241" t="b">
         <v>0</v>
@@ -58212,54 +58233,54 @@
     </row>
     <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>863</v>
+        <v>45</v>
       </c>
       <c r="B242">
         <v>10</v>
       </c>
       <c r="C242" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D242">
-        <f t="shared" si="62"/>
-        <v>140</v>
+        <f>D241+27</f>
+        <v>141</v>
       </c>
       <c r="E242">
-        <f>E241</f>
-        <v>195</v>
+        <f t="shared" si="66"/>
+        <v>190</v>
       </c>
       <c r="F242">
-        <f t="shared" si="63"/>
-        <v>169</v>
+        <f t="shared" ref="F242:F243" si="68">D242</f>
+        <v>141</v>
       </c>
       <c r="G242">
-        <f t="shared" si="66"/>
-        <v>198</v>
-      </c>
-      <c r="H242" t="s">
-        <v>20</v>
+        <f>G241</f>
+        <v>253</v>
       </c>
       <c r="I242">
-        <v>16</v>
+        <v>0.5</v>
       </c>
       <c r="J242">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K242">
         <v>0</v>
       </c>
       <c r="L242">
         <v>0</v>
+      </c>
+      <c r="M242" t="s">
+        <v>21</v>
       </c>
       <c r="N242" t="str">
         <f t="shared" si="56"/>
         <v>d0d8dd</v>
       </c>
       <c r="O242" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q242">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R242" t="b">
         <v>0</v>
@@ -58273,54 +58294,54 @@
     </row>
     <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>864</v>
+        <v>46</v>
       </c>
       <c r="B243">
         <v>10</v>
       </c>
       <c r="C243" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D243">
-        <f t="shared" si="62"/>
+        <f>D242+27</f>
         <v>168</v>
       </c>
       <c r="E243">
-        <f>E242</f>
-        <v>195</v>
+        <f t="shared" si="66"/>
+        <v>190</v>
       </c>
       <c r="F243">
-        <f t="shared" si="63"/>
-        <v>194</v>
+        <f t="shared" si="68"/>
+        <v>168</v>
       </c>
       <c r="G243">
-        <f t="shared" si="66"/>
-        <v>198</v>
-      </c>
-      <c r="H243" t="s">
-        <v>20</v>
+        <f>G242</f>
+        <v>253</v>
       </c>
       <c r="I243">
-        <v>16</v>
+        <v>0.5</v>
       </c>
       <c r="J243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K243">
         <v>0</v>
       </c>
       <c r="L243">
         <v>0</v>
+      </c>
+      <c r="M243" t="s">
+        <v>21</v>
       </c>
       <c r="N243" t="str">
         <f t="shared" si="56"/>
         <v>d0d8dd</v>
       </c>
       <c r="O243" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q243">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R243" t="b">
         <v>0</v>
@@ -58334,35 +58355,33 @@
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>905</v>
+        <v>55</v>
       </c>
       <c r="B244">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C244" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D244">
         <v>14</v>
       </c>
       <c r="E244">
-        <v>20</v>
+        <f>E238+25</f>
+        <v>217</v>
       </c>
       <c r="F244">
         <v>196</v>
       </c>
       <c r="G244">
-        <f>E244+5</f>
-        <v>25</v>
-      </c>
-      <c r="H244" t="s">
-        <v>102</v>
+        <f>E244</f>
+        <v>217</v>
       </c>
       <c r="I244">
-        <v>14</v>
+        <v>0.5</v>
       </c>
       <c r="J244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K244">
         <v>0</v>
@@ -58370,17 +58389,21 @@
       <c r="L244">
         <v>0</v>
       </c>
-      <c r="N244" t="s">
+      <c r="M244" t="s">
         <v>21</v>
+      </c>
+      <c r="N244" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O244" t="s">
         <v>25</v>
       </c>
       <c r="Q244">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R244" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S244" t="s">
         <v>119</v>
@@ -58391,10 +58414,10 @@
     </row>
     <row r="245" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>906</v>
+        <v>930</v>
       </c>
       <c r="B245">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C245" t="s">
         <v>19</v>
@@ -58403,21 +58426,21 @@
         <v>14</v>
       </c>
       <c r="E245">
-        <f>G244+8</f>
-        <v>33</v>
+        <f>G236+2</f>
+        <v>255</v>
       </c>
       <c r="F245">
         <v>196</v>
       </c>
       <c r="G245">
-        <f>E245+5</f>
-        <v>38</v>
+        <f>E245+4</f>
+        <v>259</v>
       </c>
       <c r="H245" t="s">
         <v>102</v>
       </c>
       <c r="I245">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J245">
         <v>0</v>
@@ -58432,13 +58455,16 @@
         <v>21</v>
       </c>
       <c r="O245" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q245">
         <v>2</v>
       </c>
       <c r="R245" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S245" t="s">
+        <v>119</v>
       </c>
       <c r="T245">
         <v>0</v>
@@ -58446,655 +58472,653 @@
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
+        <v>890</v>
+      </c>
+      <c r="B246">
+        <v>10</v>
+      </c>
+      <c r="C246" t="s">
+        <v>19</v>
+      </c>
+      <c r="D246">
+        <v>14</v>
+      </c>
+      <c r="E246">
+        <f>E244+2</f>
+        <v>219</v>
+      </c>
+      <c r="F246">
+        <f>D241-2</f>
+        <v>112</v>
+      </c>
+      <c r="G246">
+        <f>E246+5</f>
+        <v>224</v>
+      </c>
+      <c r="H246" t="s">
+        <v>102</v>
+      </c>
+      <c r="I246">
+        <v>12</v>
+      </c>
+      <c r="J246">
+        <v>0</v>
+      </c>
+      <c r="K246">
+        <v>0</v>
+      </c>
+      <c r="L246">
+        <v>0</v>
+      </c>
+      <c r="N246" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O246" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q246">
+        <v>3</v>
+      </c>
+      <c r="R246" t="b">
+        <v>1</v>
+      </c>
+      <c r="S246" t="s">
+        <v>119</v>
+      </c>
+      <c r="T246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>891</v>
+      </c>
+      <c r="B247">
+        <v>10</v>
+      </c>
+      <c r="C247" t="s">
+        <v>19</v>
+      </c>
+      <c r="D247">
+        <f>D238</f>
+        <v>113</v>
+      </c>
+      <c r="E247">
+        <f>E246+1</f>
+        <v>220</v>
+      </c>
+      <c r="F247">
+        <f>F238</f>
+        <v>140</v>
+      </c>
+      <c r="G247">
+        <f t="shared" ref="G247:G249" si="69">E247+3</f>
+        <v>223</v>
+      </c>
+      <c r="H247" t="s">
+        <v>20</v>
+      </c>
+      <c r="I247">
+        <v>16</v>
+      </c>
+      <c r="J247">
+        <v>1</v>
+      </c>
+      <c r="K247">
+        <v>0</v>
+      </c>
+      <c r="L247">
+        <v>0</v>
+      </c>
+      <c r="N247" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O247" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q247">
+        <v>2</v>
+      </c>
+      <c r="R247" t="b">
+        <v>0</v>
+      </c>
+      <c r="S247" t="s">
+        <v>119</v>
+      </c>
+      <c r="T247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>892</v>
+      </c>
+      <c r="B248">
+        <v>10</v>
+      </c>
+      <c r="C248" t="s">
+        <v>19</v>
+      </c>
+      <c r="D248">
+        <f>D239</f>
+        <v>140</v>
+      </c>
+      <c r="E248">
+        <f>E247</f>
+        <v>220</v>
+      </c>
+      <c r="F248">
+        <f>F239</f>
+        <v>169</v>
+      </c>
+      <c r="G248">
+        <f t="shared" si="69"/>
+        <v>223</v>
+      </c>
+      <c r="H248" t="s">
+        <v>20</v>
+      </c>
+      <c r="I248">
+        <v>16</v>
+      </c>
+      <c r="J248">
+        <v>1</v>
+      </c>
+      <c r="K248">
+        <v>0</v>
+      </c>
+      <c r="L248">
+        <v>0</v>
+      </c>
+      <c r="N248" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O248" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q248">
+        <v>2</v>
+      </c>
+      <c r="R248" t="b">
+        <v>0</v>
+      </c>
+      <c r="S248" t="s">
+        <v>119</v>
+      </c>
+      <c r="T248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>893</v>
+      </c>
+      <c r="B249">
+        <v>10</v>
+      </c>
+      <c r="C249" t="s">
+        <v>19</v>
+      </c>
+      <c r="D249">
+        <f>D240</f>
+        <v>168</v>
+      </c>
+      <c r="E249">
+        <f>E248</f>
+        <v>220</v>
+      </c>
+      <c r="F249">
+        <f>F240</f>
+        <v>194</v>
+      </c>
+      <c r="G249">
+        <f t="shared" si="69"/>
+        <v>223</v>
+      </c>
+      <c r="H249" t="s">
+        <v>20</v>
+      </c>
+      <c r="I249">
+        <v>16</v>
+      </c>
+      <c r="J249">
+        <v>1</v>
+      </c>
+      <c r="K249">
+        <v>0</v>
+      </c>
+      <c r="L249">
+        <v>0</v>
+      </c>
+      <c r="N249" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O249" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q249">
+        <v>2</v>
+      </c>
+      <c r="R249" t="b">
+        <v>0</v>
+      </c>
+      <c r="S249" t="s">
+        <v>119</v>
+      </c>
+      <c r="T249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>5210</v>
+      </c>
+      <c r="B250">
+        <v>10</v>
+      </c>
+      <c r="C250" t="s">
+        <v>19</v>
+      </c>
+      <c r="D250">
+        <f t="shared" ref="D250:D253" si="70">D246</f>
+        <v>14</v>
+      </c>
+      <c r="E250">
+        <f>E246+15</f>
+        <v>234</v>
+      </c>
+      <c r="F250">
+        <f t="shared" ref="F250:F253" si="71">F246</f>
+        <v>112</v>
+      </c>
+      <c r="G250">
+        <f>E250+5</f>
+        <v>239</v>
+      </c>
+      <c r="H250" t="s">
+        <v>102</v>
+      </c>
+      <c r="I250">
+        <v>12</v>
+      </c>
+      <c r="J250">
+        <v>0</v>
+      </c>
+      <c r="K250">
+        <v>0</v>
+      </c>
+      <c r="L250">
+        <v>0</v>
+      </c>
+      <c r="N250" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O250" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q250">
+        <v>3</v>
+      </c>
+      <c r="R250" t="b">
+        <v>1</v>
+      </c>
+      <c r="S250" t="s">
+        <v>119</v>
+      </c>
+      <c r="T250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>5211</v>
+      </c>
+      <c r="B251">
+        <v>10</v>
+      </c>
+      <c r="C251" t="s">
+        <v>19</v>
+      </c>
+      <c r="D251">
+        <f t="shared" si="70"/>
+        <v>113</v>
+      </c>
+      <c r="E251">
+        <f>E250+1</f>
+        <v>235</v>
+      </c>
+      <c r="F251">
+        <f t="shared" si="71"/>
+        <v>140</v>
+      </c>
+      <c r="G251">
+        <f>E251+3</f>
+        <v>238</v>
+      </c>
+      <c r="H251" t="s">
+        <v>20</v>
+      </c>
+      <c r="I251">
+        <v>16</v>
+      </c>
+      <c r="J251">
+        <v>1</v>
+      </c>
+      <c r="K251">
+        <v>0</v>
+      </c>
+      <c r="L251">
+        <v>0</v>
+      </c>
+      <c r="N251" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O251" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q251">
+        <v>2</v>
+      </c>
+      <c r="R251" t="b">
+        <v>0</v>
+      </c>
+      <c r="S251" t="s">
+        <v>119</v>
+      </c>
+      <c r="T251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>5212</v>
+      </c>
+      <c r="B252">
+        <v>10</v>
+      </c>
+      <c r="C252" t="s">
+        <v>19</v>
+      </c>
+      <c r="D252">
+        <f t="shared" si="70"/>
+        <v>140</v>
+      </c>
+      <c r="E252">
+        <f>E251</f>
+        <v>235</v>
+      </c>
+      <c r="F252">
+        <f t="shared" si="71"/>
+        <v>169</v>
+      </c>
+      <c r="G252">
+        <f t="shared" ref="G252:G253" si="72">E252+3</f>
+        <v>238</v>
+      </c>
+      <c r="H252" t="s">
+        <v>20</v>
+      </c>
+      <c r="I252">
+        <v>16</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+      <c r="K252">
+        <v>0</v>
+      </c>
+      <c r="L252">
+        <v>0</v>
+      </c>
+      <c r="N252" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O252" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q252">
+        <v>2</v>
+      </c>
+      <c r="R252" t="b">
+        <v>0</v>
+      </c>
+      <c r="S252" t="s">
+        <v>119</v>
+      </c>
+      <c r="T252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>5213</v>
+      </c>
+      <c r="B253">
+        <v>10</v>
+      </c>
+      <c r="C253" t="s">
+        <v>19</v>
+      </c>
+      <c r="D253">
+        <f t="shared" si="70"/>
+        <v>168</v>
+      </c>
+      <c r="E253">
+        <f>E252</f>
+        <v>235</v>
+      </c>
+      <c r="F253">
+        <f t="shared" si="71"/>
+        <v>194</v>
+      </c>
+      <c r="G253">
+        <f t="shared" si="72"/>
+        <v>238</v>
+      </c>
+      <c r="H253" t="s">
+        <v>20</v>
+      </c>
+      <c r="I253">
+        <v>16</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+      <c r="K253">
+        <v>0</v>
+      </c>
+      <c r="L253">
+        <v>0</v>
+      </c>
+      <c r="N253" t="str">
+        <f t="shared" si="56"/>
+        <v>d0d8dd</v>
+      </c>
+      <c r="O253" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q253">
+        <v>2</v>
+      </c>
+      <c r="R253" t="b">
+        <v>0</v>
+      </c>
+      <c r="S253" t="s">
+        <v>119</v>
+      </c>
+      <c r="T253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>905</v>
+      </c>
+      <c r="B254">
+        <v>11</v>
+      </c>
+      <c r="C254" t="s">
+        <v>19</v>
+      </c>
+      <c r="D254">
+        <v>14</v>
+      </c>
+      <c r="E254">
+        <v>20</v>
+      </c>
+      <c r="F254">
+        <v>196</v>
+      </c>
+      <c r="G254">
+        <f>E254+5</f>
+        <v>25</v>
+      </c>
+      <c r="H254" t="s">
+        <v>102</v>
+      </c>
+      <c r="I254">
+        <v>14</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+      <c r="K254">
+        <v>0</v>
+      </c>
+      <c r="L254">
+        <v>0</v>
+      </c>
+      <c r="N254" t="s">
+        <v>21</v>
+      </c>
+      <c r="O254" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q254">
+        <v>2</v>
+      </c>
+      <c r="R254" t="b">
+        <v>1</v>
+      </c>
+      <c r="S254" t="s">
+        <v>119</v>
+      </c>
+      <c r="T254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>906</v>
+      </c>
+      <c r="B255">
+        <v>11</v>
+      </c>
+      <c r="C255" t="s">
+        <v>19</v>
+      </c>
+      <c r="D255">
+        <v>14</v>
+      </c>
+      <c r="E255">
+        <f>G254+8</f>
+        <v>33</v>
+      </c>
+      <c r="F255">
+        <v>196</v>
+      </c>
+      <c r="G255">
+        <f>E255+5</f>
+        <v>38</v>
+      </c>
+      <c r="H255" t="s">
+        <v>102</v>
+      </c>
+      <c r="I255">
+        <v>12</v>
+      </c>
+      <c r="J255">
+        <v>0</v>
+      </c>
+      <c r="K255">
+        <v>0</v>
+      </c>
+      <c r="L255">
+        <v>0</v>
+      </c>
+      <c r="N255" t="s">
+        <v>21</v>
+      </c>
+      <c r="O255" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q255">
+        <v>2</v>
+      </c>
+      <c r="R255" t="b">
+        <v>1</v>
+      </c>
+      <c r="T255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>888</v>
       </c>
-      <c r="B246">
+      <c r="B256">
         <v>11</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C256" t="s">
         <v>26</v>
       </c>
-      <c r="D246">
-        <v>0</v>
-      </c>
-      <c r="E246">
+      <c r="D256">
+        <v>0</v>
+      </c>
+      <c r="E256">
         <v>75</v>
       </c>
-      <c r="F246">
+      <c r="F256">
         <v>210</v>
       </c>
-      <c r="G246">
-        <f>G259+15</f>
+      <c r="G256">
+        <f>G269+15</f>
         <v>123</v>
       </c>
-      <c r="I246">
-        <v>0</v>
-      </c>
-      <c r="J246">
-        <v>1</v>
-      </c>
-      <c r="K246">
-        <v>0</v>
-      </c>
-      <c r="L246">
-        <v>0</v>
-      </c>
-      <c r="M246" t="str">
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <v>1</v>
+      </c>
+      <c r="K256">
+        <v>0</v>
+      </c>
+      <c r="L256">
+        <v>0</v>
+      </c>
+      <c r="M256" t="str">
         <f>$N$76</f>
         <v>d0d8dd</v>
       </c>
-      <c r="N246" t="s">
+      <c r="N256" t="s">
         <v>928</v>
-      </c>
-      <c r="O246" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q246">
-        <v>1</v>
-      </c>
-      <c r="R246" t="b">
-        <v>0</v>
-      </c>
-      <c r="S246" t="s">
-        <v>119</v>
-      </c>
-      <c r="T246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>889</v>
-      </c>
-      <c r="B247">
-        <v>11</v>
-      </c>
-      <c r="C247" t="s">
-        <v>19</v>
-      </c>
-      <c r="D247">
-        <v>14</v>
-      </c>
-      <c r="E247">
-        <f>E246+5</f>
-        <v>80</v>
-      </c>
-      <c r="F247">
-        <v>196</v>
-      </c>
-      <c r="G247">
-        <f>E247+3</f>
-        <v>83</v>
-      </c>
-      <c r="H247" t="s">
-        <v>102</v>
-      </c>
-      <c r="I247">
-        <v>12</v>
-      </c>
-      <c r="J247">
-        <v>1</v>
-      </c>
-      <c r="K247">
-        <v>0</v>
-      </c>
-      <c r="L247">
-        <v>0</v>
-      </c>
-      <c r="N247" t="str">
-        <f t="shared" ref="N247:N254" si="67">$N$76</f>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O247" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q247">
-        <v>3</v>
-      </c>
-      <c r="R247" t="b">
-        <v>0</v>
-      </c>
-      <c r="S247" t="s">
-        <v>119</v>
-      </c>
-      <c r="T247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>774</v>
-      </c>
-      <c r="B248">
-        <v>11</v>
-      </c>
-      <c r="C248" t="s">
-        <v>19</v>
-      </c>
-      <c r="D248">
-        <f t="shared" ref="D248" si="68">D251-1</f>
-        <v>113</v>
-      </c>
-      <c r="E248">
-        <f>E246+2</f>
-        <v>77</v>
-      </c>
-      <c r="F248">
-        <f>D252-1</f>
-        <v>140</v>
-      </c>
-      <c r="G248">
-        <f>E248+5</f>
-        <v>82</v>
-      </c>
-      <c r="H248" t="s">
-        <v>102</v>
-      </c>
-      <c r="I248">
-        <v>10</v>
-      </c>
-      <c r="J248">
-        <v>1</v>
-      </c>
-      <c r="K248">
-        <v>0</v>
-      </c>
-      <c r="L248">
-        <v>0</v>
-      </c>
-      <c r="N248" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O248" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q248">
-        <v>3</v>
-      </c>
-      <c r="R248" t="b">
-        <v>1</v>
-      </c>
-      <c r="S248" t="s">
-        <v>119</v>
-      </c>
-      <c r="T248">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>775</v>
-      </c>
-      <c r="B249">
-        <v>11</v>
-      </c>
-      <c r="C249" t="s">
-        <v>19</v>
-      </c>
-      <c r="D249">
-        <f>D252-1</f>
-        <v>140</v>
-      </c>
-      <c r="E249">
-        <f t="shared" ref="E249:E253" si="69">E248</f>
-        <v>77</v>
-      </c>
-      <c r="F249">
-        <f>D253+1</f>
-        <v>169</v>
-      </c>
-      <c r="G249">
-        <f>G248</f>
-        <v>82</v>
-      </c>
-      <c r="H249" t="s">
-        <v>102</v>
-      </c>
-      <c r="I249">
-        <v>10</v>
-      </c>
-      <c r="J249">
-        <v>1</v>
-      </c>
-      <c r="K249">
-        <v>0</v>
-      </c>
-      <c r="L249">
-        <v>0</v>
-      </c>
-      <c r="N249" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O249" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q249">
-        <v>3</v>
-      </c>
-      <c r="R249" t="b">
-        <v>1</v>
-      </c>
-      <c r="S249" t="s">
-        <v>119</v>
-      </c>
-      <c r="T249">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>776</v>
-      </c>
-      <c r="B250">
-        <v>11</v>
-      </c>
-      <c r="C250" t="s">
-        <v>19</v>
-      </c>
-      <c r="D250">
-        <f>D253</f>
-        <v>168</v>
-      </c>
-      <c r="E250">
-        <f t="shared" si="69"/>
-        <v>77</v>
-      </c>
-      <c r="F250">
-        <f>D250+26</f>
-        <v>194</v>
-      </c>
-      <c r="G250">
-        <f t="shared" ref="G250" si="70">G249</f>
-        <v>82</v>
-      </c>
-      <c r="H250" t="s">
-        <v>102</v>
-      </c>
-      <c r="I250">
-        <v>10</v>
-      </c>
-      <c r="J250">
-        <v>1</v>
-      </c>
-      <c r="K250">
-        <v>0</v>
-      </c>
-      <c r="L250">
-        <v>0</v>
-      </c>
-      <c r="N250" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O250" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q250">
-        <v>3</v>
-      </c>
-      <c r="R250" t="b">
-        <v>1</v>
-      </c>
-      <c r="S250" t="s">
-        <v>119</v>
-      </c>
-      <c r="T250">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>44</v>
-      </c>
-      <c r="B251">
-        <v>11</v>
-      </c>
-      <c r="C251" t="s">
-        <v>25</v>
-      </c>
-      <c r="D251">
-        <v>114</v>
-      </c>
-      <c r="E251">
-        <f>E246</f>
-        <v>75</v>
-      </c>
-      <c r="F251">
-        <f>D251</f>
-        <v>114</v>
-      </c>
-      <c r="G251">
-        <f>G246</f>
-        <v>123</v>
-      </c>
-      <c r="I251">
-        <v>0.5</v>
-      </c>
-      <c r="J251">
-        <v>0</v>
-      </c>
-      <c r="K251">
-        <v>0</v>
-      </c>
-      <c r="L251">
-        <v>0</v>
-      </c>
-      <c r="M251" t="s">
-        <v>21</v>
-      </c>
-      <c r="N251" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O251" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q251">
-        <v>4</v>
-      </c>
-      <c r="R251" t="b">
-        <v>0</v>
-      </c>
-      <c r="S251" t="s">
-        <v>119</v>
-      </c>
-      <c r="T251">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>45</v>
-      </c>
-      <c r="B252">
-        <v>11</v>
-      </c>
-      <c r="C252" t="s">
-        <v>25</v>
-      </c>
-      <c r="D252">
-        <f>D251+27</f>
-        <v>141</v>
-      </c>
-      <c r="E252">
-        <f t="shared" si="69"/>
-        <v>75</v>
-      </c>
-      <c r="F252">
-        <f t="shared" ref="F252:F253" si="71">D252</f>
-        <v>141</v>
-      </c>
-      <c r="G252">
-        <f>G251</f>
-        <v>123</v>
-      </c>
-      <c r="I252">
-        <v>0.5</v>
-      </c>
-      <c r="J252">
-        <v>0</v>
-      </c>
-      <c r="K252">
-        <v>0</v>
-      </c>
-      <c r="L252">
-        <v>0</v>
-      </c>
-      <c r="M252" t="s">
-        <v>21</v>
-      </c>
-      <c r="N252" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O252" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q252">
-        <v>4</v>
-      </c>
-      <c r="R252" t="b">
-        <v>0</v>
-      </c>
-      <c r="S252" t="s">
-        <v>119</v>
-      </c>
-      <c r="T252">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>46</v>
-      </c>
-      <c r="B253">
-        <v>11</v>
-      </c>
-      <c r="C253" t="s">
-        <v>25</v>
-      </c>
-      <c r="D253">
-        <f>D252+27</f>
-        <v>168</v>
-      </c>
-      <c r="E253">
-        <f t="shared" si="69"/>
-        <v>75</v>
-      </c>
-      <c r="F253">
-        <f t="shared" si="71"/>
-        <v>168</v>
-      </c>
-      <c r="G253">
-        <f>G252</f>
-        <v>123</v>
-      </c>
-      <c r="I253">
-        <v>0.5</v>
-      </c>
-      <c r="J253">
-        <v>0</v>
-      </c>
-      <c r="K253">
-        <v>0</v>
-      </c>
-      <c r="L253">
-        <v>0</v>
-      </c>
-      <c r="M253" t="s">
-        <v>21</v>
-      </c>
-      <c r="N253" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O253" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q253">
-        <v>4</v>
-      </c>
-      <c r="R253" t="b">
-        <v>0</v>
-      </c>
-      <c r="S253" t="s">
-        <v>119</v>
-      </c>
-      <c r="T253">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>55</v>
-      </c>
-      <c r="B254">
-        <v>11</v>
-      </c>
-      <c r="C254" t="s">
-        <v>25</v>
-      </c>
-      <c r="D254">
-        <v>14</v>
-      </c>
-      <c r="E254">
-        <f>E248+25</f>
-        <v>102</v>
-      </c>
-      <c r="F254">
-        <v>196</v>
-      </c>
-      <c r="G254">
-        <f>E254</f>
-        <v>102</v>
-      </c>
-      <c r="I254">
-        <v>0.5</v>
-      </c>
-      <c r="J254">
-        <v>0</v>
-      </c>
-      <c r="K254">
-        <v>0</v>
-      </c>
-      <c r="L254">
-        <v>0</v>
-      </c>
-      <c r="M254" t="s">
-        <v>21</v>
-      </c>
-      <c r="N254" t="str">
-        <f t="shared" si="67"/>
-        <v>d0d8dd</v>
-      </c>
-      <c r="O254" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q254">
-        <v>4</v>
-      </c>
-      <c r="R254" t="b">
-        <v>0</v>
-      </c>
-      <c r="S254" t="s">
-        <v>119</v>
-      </c>
-      <c r="T254">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>930</v>
-      </c>
-      <c r="B255">
-        <v>11</v>
-      </c>
-      <c r="C255" t="s">
-        <v>19</v>
-      </c>
-      <c r="D255">
-        <v>14</v>
-      </c>
-      <c r="E255">
-        <f>G246+2</f>
-        <v>125</v>
-      </c>
-      <c r="F255">
-        <v>196</v>
-      </c>
-      <c r="G255">
-        <f>E255+4</f>
-        <v>129</v>
-      </c>
-      <c r="H255" t="s">
-        <v>102</v>
-      </c>
-      <c r="I255">
-        <v>10</v>
-      </c>
-      <c r="J255">
-        <v>0</v>
-      </c>
-      <c r="K255">
-        <v>0</v>
-      </c>
-      <c r="L255">
-        <v>0</v>
-      </c>
-      <c r="N255" t="s">
-        <v>21</v>
-      </c>
-      <c r="O255" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q255">
-        <v>2</v>
-      </c>
-      <c r="R255" t="b">
-        <v>0</v>
-      </c>
-      <c r="S255" t="s">
-        <v>119</v>
-      </c>
-      <c r="T255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>890</v>
-      </c>
-      <c r="B256">
-        <v>11</v>
-      </c>
-      <c r="C256" t="s">
-        <v>19</v>
-      </c>
-      <c r="D256">
-        <v>14</v>
-      </c>
-      <c r="E256">
-        <f>E254+2</f>
-        <v>104</v>
-      </c>
-      <c r="F256">
-        <f>D251-2</f>
-        <v>112</v>
-      </c>
-      <c r="G256">
-        <f>E256+5</f>
-        <v>109</v>
-      </c>
-      <c r="H256" t="s">
-        <v>102</v>
-      </c>
-      <c r="I256">
-        <v>12</v>
-      </c>
-      <c r="J256">
-        <v>0</v>
-      </c>
-      <c r="K256">
-        <v>0</v>
-      </c>
-      <c r="L256">
-        <v>0</v>
-      </c>
-      <c r="N256" t="str">
-        <f t="shared" ref="N256:N259" si="72">$N$76</f>
-        <v>d0d8dd</v>
       </c>
       <c r="O256" t="s">
         <v>25</v>
       </c>
       <c r="Q256">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R256" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S256" t="s">
         <v>119</v>
@@ -59105,7 +59129,7 @@
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>891</v>
+        <v>5205</v>
       </c>
       <c r="B257">
         <v>11</v>
@@ -59114,26 +59138,24 @@
         <v>19</v>
       </c>
       <c r="D257">
-        <f>D248</f>
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="E257">
-        <f>E256+1</f>
-        <v>105</v>
+        <f>E256+5</f>
+        <v>80</v>
       </c>
       <c r="F257">
-        <f>F248</f>
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="G257">
-        <f t="shared" ref="G257:G259" si="73">E257+3</f>
-        <v>108</v>
+        <f>E257+3</f>
+        <v>83</v>
       </c>
       <c r="H257" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="I257">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J257">
         <v>1</v>
@@ -59145,14 +59167,14 @@
         <v>0</v>
       </c>
       <c r="N257" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" ref="N257:N264" si="73">$N$76</f>
         <v>d0d8dd</v>
       </c>
       <c r="O257" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q257">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R257" t="b">
         <v>0</v>
@@ -59166,7 +59188,7 @@
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>892</v>
+        <v>774</v>
       </c>
       <c r="B258">
         <v>11</v>
@@ -59175,48 +59197,48 @@
         <v>19</v>
       </c>
       <c r="D258">
-        <f>D249</f>
+        <f t="shared" ref="D258" si="74">D261-1</f>
+        <v>113</v>
+      </c>
+      <c r="E258">
+        <f>E256+2</f>
+        <v>77</v>
+      </c>
+      <c r="F258">
+        <f>D262-1</f>
         <v>140</v>
       </c>
-      <c r="E258">
-        <f>E257</f>
-        <v>105</v>
-      </c>
-      <c r="F258">
-        <f>F249</f>
-        <v>169</v>
-      </c>
       <c r="G258">
+        <f>E258+5</f>
+        <v>82</v>
+      </c>
+      <c r="H258" t="s">
+        <v>102</v>
+      </c>
+      <c r="I258">
+        <v>10</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+      <c r="K258">
+        <v>0</v>
+      </c>
+      <c r="L258">
+        <v>0</v>
+      </c>
+      <c r="N258" t="str">
         <f t="shared" si="73"/>
-        <v>108</v>
-      </c>
-      <c r="H258" t="s">
-        <v>20</v>
-      </c>
-      <c r="I258">
-        <v>16</v>
-      </c>
-      <c r="J258">
-        <v>1</v>
-      </c>
-      <c r="K258">
-        <v>0</v>
-      </c>
-      <c r="L258">
-        <v>0</v>
-      </c>
-      <c r="N258" t="str">
-        <f t="shared" si="72"/>
         <v>d0d8dd</v>
       </c>
       <c r="O258" t="s">
         <v>27</v>
       </c>
       <c r="Q258">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R258" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S258" t="s">
         <v>119</v>
@@ -59227,7 +59249,7 @@
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>893</v>
+        <v>775</v>
       </c>
       <c r="B259">
         <v>11</v>
@@ -59236,48 +59258,48 @@
         <v>19</v>
       </c>
       <c r="D259">
-        <f>D250</f>
-        <v>168</v>
+        <f>D262-1</f>
+        <v>140</v>
       </c>
       <c r="E259">
-        <f>E258</f>
-        <v>105</v>
+        <f t="shared" ref="E259:E263" si="75">E258</f>
+        <v>77</v>
       </c>
       <c r="F259">
-        <f>F250</f>
-        <v>194</v>
+        <f>D263+1</f>
+        <v>169</v>
       </c>
       <c r="G259">
+        <f>G258</f>
+        <v>82</v>
+      </c>
+      <c r="H259" t="s">
+        <v>102</v>
+      </c>
+      <c r="I259">
+        <v>10</v>
+      </c>
+      <c r="J259">
+        <v>1</v>
+      </c>
+      <c r="K259">
+        <v>0</v>
+      </c>
+      <c r="L259">
+        <v>0</v>
+      </c>
+      <c r="N259" t="str">
         <f t="shared" si="73"/>
-        <v>108</v>
-      </c>
-      <c r="H259" t="s">
-        <v>20</v>
-      </c>
-      <c r="I259">
-        <v>16</v>
-      </c>
-      <c r="J259">
-        <v>1</v>
-      </c>
-      <c r="K259">
-        <v>0</v>
-      </c>
-      <c r="L259">
-        <v>0</v>
-      </c>
-      <c r="N259" t="str">
-        <f t="shared" si="72"/>
         <v>d0d8dd</v>
       </c>
       <c r="O259" t="s">
         <v>27</v>
       </c>
       <c r="Q259">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R259" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S259" t="s">
         <v>119</v>
@@ -59288,32 +59310,38 @@
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>1037</v>
+        <v>776</v>
       </c>
       <c r="B260">
         <v>11</v>
       </c>
       <c r="C260" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D260">
-        <v>30</v>
+        <f>D263</f>
+        <v>168</v>
       </c>
       <c r="E260">
-        <v>130</v>
+        <f t="shared" si="75"/>
+        <v>77</v>
       </c>
       <c r="F260">
-        <v>180</v>
+        <f>D260+26</f>
+        <v>194</v>
       </c>
       <c r="G260">
-        <f>E260+(F260-D260)</f>
-        <v>280</v>
+        <f t="shared" ref="G260" si="76">G259</f>
+        <v>82</v>
+      </c>
+      <c r="H260" t="s">
+        <v>102</v>
       </c>
       <c r="I260">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J260">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K260">
         <v>0</v>
@@ -59321,17 +59349,18 @@
       <c r="L260">
         <v>0</v>
       </c>
-      <c r="N260" t="s">
-        <v>21</v>
+      <c r="N260" t="str">
+        <f t="shared" si="73"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O260" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q260">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R260" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S260" t="s">
         <v>119</v>
@@ -59342,56 +59371,56 @@
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1038</v>
+        <v>44</v>
       </c>
       <c r="B261">
         <v>11</v>
       </c>
       <c r="C261" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D261">
-        <f>D260</f>
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="E261">
-        <f>E260</f>
-        <v>130</v>
+        <f>E256</f>
+        <v>75</v>
       </c>
       <c r="F261">
-        <f>D261+100</f>
-        <v>130</v>
+        <f>D261</f>
+        <v>114</v>
       </c>
       <c r="G261">
-        <f>G260</f>
-        <v>280</v>
-      </c>
-      <c r="H261" t="s">
-        <v>102</v>
+        <f>G256</f>
+        <v>123</v>
       </c>
       <c r="I261">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="J261">
         <v>0</v>
       </c>
       <c r="K261">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L261">
         <v>0</v>
       </c>
-      <c r="N261" t="s">
+      <c r="M261" t="s">
         <v>21</v>
+      </c>
+      <c r="N261" t="str">
+        <f t="shared" si="73"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O261" t="s">
         <v>25</v>
       </c>
       <c r="Q261">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R261" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S261" t="s">
         <v>119</v>
@@ -59402,59 +59431,57 @@
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>1039</v>
+        <v>45</v>
       </c>
       <c r="B262">
         <v>11</v>
       </c>
       <c r="C262" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D262">
-        <f>D260</f>
-        <v>30</v>
+        <f>D261+27</f>
+        <v>141</v>
       </c>
       <c r="E262">
-        <f>G260</f>
-        <v>280</v>
+        <f t="shared" si="75"/>
+        <v>75</v>
       </c>
       <c r="F262">
-        <f>F260</f>
-        <v>180</v>
+        <f t="shared" ref="F262:F263" si="77">D262</f>
+        <v>141</v>
       </c>
       <c r="G262">
-        <f>E262+3</f>
-        <v>283</v>
-      </c>
-      <c r="H262" t="s">
-        <v>102</v>
+        <f>G261</f>
+        <v>123</v>
       </c>
       <c r="I262">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="J262">
         <v>0</v>
       </c>
       <c r="K262">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L262">
         <v>0</v>
       </c>
       <c r="M262" t="s">
-        <v>894</v>
-      </c>
-      <c r="N262" t="s">
         <v>21</v>
       </c>
+      <c r="N262" t="str">
+        <f t="shared" si="73"/>
+        <v>d0d8dd</v>
+      </c>
       <c r="O262" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q262">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R262" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S262" t="s">
         <v>119</v>
@@ -59465,35 +59492,35 @@
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="B263">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C263" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D263">
-        <v>14</v>
+        <f>D262+27</f>
+        <v>168</v>
       </c>
       <c r="E263">
-        <v>20</v>
+        <f t="shared" si="75"/>
+        <v>75</v>
       </c>
       <c r="F263">
-        <v>196</v>
+        <f t="shared" si="77"/>
+        <v>168</v>
       </c>
       <c r="G263">
-        <f>E263+5</f>
-        <v>25</v>
-      </c>
-      <c r="H263" t="s">
-        <v>102</v>
+        <f>G262</f>
+        <v>123</v>
       </c>
       <c r="I263">
-        <v>14</v>
+        <v>0.5</v>
       </c>
       <c r="J263">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -59501,17 +59528,21 @@
       <c r="L263">
         <v>0</v>
       </c>
-      <c r="N263" t="s">
+      <c r="M263" t="s">
         <v>21</v>
+      </c>
+      <c r="N263" t="str">
+        <f t="shared" si="73"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O263" t="s">
         <v>25</v>
       </c>
       <c r="Q263">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R263" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S263" t="s">
         <v>119</v>
@@ -59522,34 +59553,30 @@
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>5033</v>
+        <v>55</v>
       </c>
       <c r="B264">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C264" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D264">
         <v>14</v>
       </c>
       <c r="E264">
-        <f>G263+8</f>
-        <v>33</v>
+        <f>E258+25</f>
+        <v>102</v>
       </c>
       <c r="F264">
-        <f>$F$265</f>
         <v>196</v>
       </c>
       <c r="G264">
-        <f>E264+5</f>
-        <v>38</v>
-      </c>
-      <c r="H264" t="s">
+        <f>E264</f>
         <v>102</v>
       </c>
       <c r="I264">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="J264">
         <v>0</v>
@@ -59560,17 +59587,24 @@
       <c r="L264">
         <v>0</v>
       </c>
-      <c r="N264" t="s">
+      <c r="M264" t="s">
         <v>21</v>
+      </c>
+      <c r="N264" t="str">
+        <f t="shared" si="73"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O264" t="s">
         <v>25</v>
       </c>
       <c r="Q264">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R264" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S264" t="s">
+        <v>119</v>
       </c>
       <c r="T264">
         <v>0</v>
@@ -59578,29 +59612,33 @@
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>29</v>
+        <v>930</v>
       </c>
       <c r="B265">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C265" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D265">
         <v>14</v>
       </c>
       <c r="E265">
-        <v>200</v>
+        <f>G256+2</f>
+        <v>125</v>
       </c>
       <c r="F265">
         <v>196</v>
       </c>
       <c r="G265">
-        <f>E265</f>
-        <v>200</v>
+        <f>E265+4</f>
+        <v>129</v>
+      </c>
+      <c r="H265" t="s">
+        <v>102</v>
       </c>
       <c r="I265">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J265">
         <v>0</v>
@@ -59615,7 +59653,7 @@
         <v>21</v>
       </c>
       <c r="O265" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q265">
         <v>2</v>
@@ -59632,29 +59670,28 @@
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>334</v>
+        <v>5206</v>
       </c>
       <c r="B266">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C266" t="s">
         <v>19</v>
       </c>
       <c r="D266">
-        <f t="shared" ref="D266:D268" si="74">D265</f>
         <v>14</v>
       </c>
       <c r="E266">
-        <f>G265+8</f>
-        <v>208</v>
+        <f>E264+2</f>
+        <v>104</v>
       </c>
       <c r="F266">
-        <f>F265</f>
-        <v>196</v>
+        <f>D261-2</f>
+        <v>112</v>
       </c>
       <c r="G266">
-        <f>E266+4</f>
-        <v>212</v>
+        <f>E266+5</f>
+        <v>109</v>
       </c>
       <c r="H266" t="s">
         <v>102</v>
@@ -59663,7 +59700,7 @@
         <v>12</v>
       </c>
       <c r="J266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K266">
         <v>0</v>
@@ -59671,15 +59708,15 @@
       <c r="L266">
         <v>0</v>
       </c>
-      <c r="N266" t="s">
-        <v>21</v>
+      <c r="N266" t="str">
+        <f t="shared" ref="N266:N269" si="78">$N$76</f>
+        <v>d0d8dd</v>
       </c>
       <c r="O266" t="s">
         <v>25</v>
       </c>
-      <c r="P266" s="1"/>
       <c r="Q266">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R266" t="b">
         <v>1</v>
@@ -59693,38 +59730,38 @@
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>666</v>
+        <v>5207</v>
       </c>
       <c r="B267">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C267" t="s">
         <v>19</v>
       </c>
       <c r="D267">
-        <f t="shared" si="74"/>
-        <v>14</v>
+        <f>D258</f>
+        <v>113</v>
       </c>
       <c r="E267">
-        <f>G266+2</f>
-        <v>214</v>
+        <f>E266+1</f>
+        <v>105</v>
       </c>
       <c r="F267">
-        <f>F266</f>
-        <v>196</v>
+        <f>F258</f>
+        <v>140</v>
       </c>
       <c r="G267">
-        <f>E267+4</f>
-        <v>218</v>
+        <f t="shared" ref="G267:G269" si="79">E267+3</f>
+        <v>108</v>
       </c>
       <c r="H267" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="I267">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J267">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -59732,18 +59769,18 @@
       <c r="L267">
         <v>0</v>
       </c>
-      <c r="N267" t="s">
-        <v>21</v>
+      <c r="N267" t="str">
+        <f t="shared" si="78"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O267" t="s">
-        <v>25</v>
-      </c>
-      <c r="P267" s="1"/>
+        <v>27</v>
+      </c>
       <c r="Q267">
         <v>2</v>
       </c>
       <c r="R267" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S267" t="s">
         <v>119</v>
@@ -59752,37 +59789,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>944</v>
+        <v>5208</v>
       </c>
       <c r="B268">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C268" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D268">
-        <f t="shared" si="74"/>
-        <v>14</v>
+        <f>D259</f>
+        <v>140</v>
       </c>
       <c r="E268">
-        <f>G267+30</f>
-        <v>248</v>
+        <f>E267</f>
+        <v>105</v>
       </c>
       <c r="F268">
-        <f>D268+10</f>
-        <v>24</v>
+        <f>F259</f>
+        <v>169</v>
       </c>
       <c r="G268">
-        <f>E268+(F268-D268)</f>
-        <v>258</v>
+        <f t="shared" si="79"/>
+        <v>108</v>
+      </c>
+      <c r="H268" t="s">
+        <v>20</v>
       </c>
       <c r="I268">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J268">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K268">
         <v>0</v>
@@ -59790,60 +59830,60 @@
       <c r="L268">
         <v>0</v>
       </c>
-      <c r="M268" t="s">
-        <v>945</v>
-      </c>
-      <c r="N268" t="s">
-        <v>946</v>
+      <c r="N268" t="str">
+        <f t="shared" si="78"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O268" t="s">
-        <v>25</v>
-      </c>
-      <c r="P268" s="5" t="str">
-        <f>"configuration/assets/"&amp;A268&amp;".svg"</f>
-        <v>configuration/assets/cc.svg</v>
+        <v>27</v>
       </c>
       <c r="Q268">
         <v>2</v>
       </c>
       <c r="R268" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S268" t="s">
+        <v>119</v>
       </c>
       <c r="T268">
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>947</v>
+        <v>5209</v>
       </c>
       <c r="B269">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C269" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D269">
-        <f>F268+2</f>
-        <v>26</v>
+        <f>D260</f>
+        <v>168</v>
       </c>
       <c r="E269">
         <f>E268</f>
-        <v>248</v>
+        <v>105</v>
       </c>
       <c r="F269">
-        <f>D269+10</f>
-        <v>36</v>
+        <f>F260</f>
+        <v>194</v>
       </c>
       <c r="G269">
-        <f>E269+(F269-D269)</f>
-        <v>258</v>
+        <f t="shared" si="79"/>
+        <v>108</v>
+      </c>
+      <c r="H269" t="s">
+        <v>20</v>
       </c>
       <c r="I269">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J269">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K269">
         <v>0</v>
@@ -59851,57 +59891,51 @@
       <c r="L269">
         <v>0</v>
       </c>
-      <c r="M269" t="s">
-        <v>945</v>
-      </c>
-      <c r="N269" t="s">
-        <v>946</v>
+      <c r="N269" t="str">
+        <f t="shared" si="78"/>
+        <v>d0d8dd</v>
       </c>
       <c r="O269" t="s">
-        <v>25</v>
-      </c>
-      <c r="P269" s="5" t="str">
-        <f>"configuration/assets/"&amp;A269&amp;".svg"</f>
-        <v>configuration/assets/by.svg</v>
+        <v>27</v>
       </c>
       <c r="Q269">
         <v>2</v>
       </c>
       <c r="R269" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S269" t="s">
+        <v>119</v>
       </c>
       <c r="T269">
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>948</v>
+        <v>1037</v>
       </c>
       <c r="B270">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C270" t="s">
         <v>24</v>
       </c>
       <c r="D270">
-        <f>F269+2</f>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E270">
-        <f>E269</f>
-        <v>248</v>
+        <v>130</v>
       </c>
       <c r="F270">
-        <f>D270+10</f>
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="G270">
         <f>E270+(F270-D270)</f>
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="I270">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J270">
         <v>0</v>
@@ -59912,66 +59946,62 @@
       <c r="L270">
         <v>0</v>
       </c>
-      <c r="M270" t="s">
-        <v>945</v>
-      </c>
       <c r="N270" t="s">
-        <v>946</v>
+        <v>21</v>
       </c>
       <c r="O270" t="s">
         <v>25</v>
       </c>
-      <c r="P270" s="5" t="str">
-        <f>"configuration/assets/"&amp;A270&amp;".svg"</f>
-        <v>configuration/assets/nc.svg</v>
-      </c>
       <c r="Q270">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R270" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S270" t="s">
+        <v>119</v>
       </c>
       <c r="T270">
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>115</v>
+        <v>1038</v>
       </c>
       <c r="B271">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C271" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="D271">
-        <f>D268</f>
-        <v>14</v>
+        <f>D270</f>
+        <v>30</v>
       </c>
       <c r="E271">
-        <f>G268+5</f>
-        <v>263</v>
+        <f>E270</f>
+        <v>130</v>
       </c>
       <c r="F271">
-        <f>F267</f>
-        <v>196</v>
+        <f>D271+100</f>
+        <v>130</v>
       </c>
       <c r="G271">
-        <f>E271+3</f>
-        <v>266</v>
+        <f>G270</f>
+        <v>280</v>
       </c>
       <c r="H271" t="s">
         <v>102</v>
       </c>
       <c r="I271">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J271">
         <v>0</v>
       </c>
       <c r="K271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L271">
         <v>0</v>
@@ -59982,17 +60012,14 @@
       <c r="O271" t="s">
         <v>25</v>
       </c>
-      <c r="P271" s="5" t="s">
-        <v>949</v>
-      </c>
       <c r="Q271">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R271" t="b">
         <v>1</v>
       </c>
       <c r="S271" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T271">
         <v>0</v>
@@ -60000,57 +60027,655 @@
     </row>
     <row r="272" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>29</v>
+        <v>1039</v>
       </c>
       <c r="B272">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C272" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D272">
-        <f>D268</f>
-        <v>14</v>
+        <f>D270</f>
+        <v>30</v>
       </c>
       <c r="E272">
-        <f>G271+8</f>
-        <v>274</v>
+        <f>G270</f>
+        <v>280</v>
       </c>
       <c r="F272">
-        <v>196</v>
+        <f>F270</f>
+        <v>180</v>
       </c>
       <c r="G272">
-        <f>E272</f>
-        <v>274</v>
+        <f>E272+3</f>
+        <v>283</v>
+      </c>
+      <c r="H272" t="s">
+        <v>102</v>
       </c>
       <c r="I272">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J272">
         <v>0</v>
       </c>
       <c r="K272">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L272">
         <v>0</v>
+      </c>
+      <c r="M272" t="s">
+        <v>894</v>
       </c>
       <c r="N272" t="s">
         <v>21</v>
       </c>
       <c r="O272" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q272">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R272" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S272" t="s">
         <v>119</v>
       </c>
       <c r="T272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>127</v>
+      </c>
+      <c r="B273">
+        <v>12</v>
+      </c>
+      <c r="C273" t="s">
+        <v>19</v>
+      </c>
+      <c r="D273">
+        <v>14</v>
+      </c>
+      <c r="E273">
+        <v>20</v>
+      </c>
+      <c r="F273">
+        <v>196</v>
+      </c>
+      <c r="G273">
+        <f>E273+5</f>
+        <v>25</v>
+      </c>
+      <c r="H273" t="s">
+        <v>102</v>
+      </c>
+      <c r="I273">
+        <v>14</v>
+      </c>
+      <c r="J273">
+        <v>1</v>
+      </c>
+      <c r="K273">
+        <v>0</v>
+      </c>
+      <c r="L273">
+        <v>0</v>
+      </c>
+      <c r="N273" t="s">
+        <v>21</v>
+      </c>
+      <c r="O273" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q273">
+        <v>2</v>
+      </c>
+      <c r="R273" t="b">
+        <v>1</v>
+      </c>
+      <c r="S273" t="s">
+        <v>119</v>
+      </c>
+      <c r="T273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>5033</v>
+      </c>
+      <c r="B274">
+        <v>12</v>
+      </c>
+      <c r="C274" t="s">
+        <v>19</v>
+      </c>
+      <c r="D274">
+        <v>14</v>
+      </c>
+      <c r="E274">
+        <f>G273+8</f>
+        <v>33</v>
+      </c>
+      <c r="F274">
+        <f>$F$275</f>
+        <v>196</v>
+      </c>
+      <c r="G274">
+        <f>E274+5</f>
+        <v>38</v>
+      </c>
+      <c r="H274" t="s">
+        <v>102</v>
+      </c>
+      <c r="I274">
+        <v>12</v>
+      </c>
+      <c r="J274">
+        <v>0</v>
+      </c>
+      <c r="K274">
+        <v>0</v>
+      </c>
+      <c r="L274">
+        <v>0</v>
+      </c>
+      <c r="N274" t="s">
+        <v>21</v>
+      </c>
+      <c r="O274" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q274">
+        <v>2</v>
+      </c>
+      <c r="R274" t="b">
+        <v>1</v>
+      </c>
+      <c r="T274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>29</v>
+      </c>
+      <c r="B275">
+        <v>12</v>
+      </c>
+      <c r="C275" t="s">
+        <v>25</v>
+      </c>
+      <c r="D275">
+        <v>14</v>
+      </c>
+      <c r="E275">
+        <v>200</v>
+      </c>
+      <c r="F275">
+        <v>196</v>
+      </c>
+      <c r="G275">
+        <f>E275</f>
+        <v>200</v>
+      </c>
+      <c r="I275">
+        <v>0</v>
+      </c>
+      <c r="J275">
+        <v>0</v>
+      </c>
+      <c r="K275">
+        <v>0</v>
+      </c>
+      <c r="L275">
+        <v>0</v>
+      </c>
+      <c r="N275" t="s">
+        <v>21</v>
+      </c>
+      <c r="O275" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q275">
+        <v>2</v>
+      </c>
+      <c r="R275" t="b">
+        <v>0</v>
+      </c>
+      <c r="S275" t="s">
+        <v>119</v>
+      </c>
+      <c r="T275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>334</v>
+      </c>
+      <c r="B276">
+        <v>12</v>
+      </c>
+      <c r="C276" t="s">
+        <v>19</v>
+      </c>
+      <c r="D276">
+        <f t="shared" ref="D276:D278" si="80">D275</f>
+        <v>14</v>
+      </c>
+      <c r="E276">
+        <f>G275+8</f>
+        <v>208</v>
+      </c>
+      <c r="F276">
+        <f>F275</f>
+        <v>196</v>
+      </c>
+      <c r="G276">
+        <f>E276+4</f>
+        <v>212</v>
+      </c>
+      <c r="H276" t="s">
+        <v>102</v>
+      </c>
+      <c r="I276">
+        <v>12</v>
+      </c>
+      <c r="J276">
+        <v>1</v>
+      </c>
+      <c r="K276">
+        <v>0</v>
+      </c>
+      <c r="L276">
+        <v>0</v>
+      </c>
+      <c r="N276" t="s">
+        <v>21</v>
+      </c>
+      <c r="O276" t="s">
+        <v>25</v>
+      </c>
+      <c r="P276" s="1"/>
+      <c r="Q276">
+        <v>2</v>
+      </c>
+      <c r="R276" t="b">
+        <v>1</v>
+      </c>
+      <c r="S276" t="s">
+        <v>119</v>
+      </c>
+      <c r="T276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>666</v>
+      </c>
+      <c r="B277">
+        <v>12</v>
+      </c>
+      <c r="C277" t="s">
+        <v>19</v>
+      </c>
+      <c r="D277">
+        <f t="shared" si="80"/>
+        <v>14</v>
+      </c>
+      <c r="E277">
+        <f>G276+2</f>
+        <v>214</v>
+      </c>
+      <c r="F277">
+        <f>F276</f>
+        <v>196</v>
+      </c>
+      <c r="G277">
+        <f>E277+4</f>
+        <v>218</v>
+      </c>
+      <c r="H277" t="s">
+        <v>102</v>
+      </c>
+      <c r="I277">
+        <v>10</v>
+      </c>
+      <c r="J277">
+        <v>0</v>
+      </c>
+      <c r="K277">
+        <v>0</v>
+      </c>
+      <c r="L277">
+        <v>0</v>
+      </c>
+      <c r="N277" t="s">
+        <v>21</v>
+      </c>
+      <c r="O277" t="s">
+        <v>25</v>
+      </c>
+      <c r="P277" s="1"/>
+      <c r="Q277">
+        <v>2</v>
+      </c>
+      <c r="R277" t="b">
+        <v>1</v>
+      </c>
+      <c r="S277" t="s">
+        <v>119</v>
+      </c>
+      <c r="T277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>944</v>
+      </c>
+      <c r="B278">
+        <v>12</v>
+      </c>
+      <c r="C278" t="s">
+        <v>24</v>
+      </c>
+      <c r="D278">
+        <f t="shared" si="80"/>
+        <v>14</v>
+      </c>
+      <c r="E278">
+        <f>G277+30</f>
+        <v>248</v>
+      </c>
+      <c r="F278">
+        <f>D278+10</f>
+        <v>24</v>
+      </c>
+      <c r="G278">
+        <f>E278+(F278-D278)</f>
+        <v>258</v>
+      </c>
+      <c r="I278">
+        <v>12</v>
+      </c>
+      <c r="J278">
+        <v>0</v>
+      </c>
+      <c r="K278">
+        <v>0</v>
+      </c>
+      <c r="L278">
+        <v>0</v>
+      </c>
+      <c r="M278" t="s">
+        <v>945</v>
+      </c>
+      <c r="N278" t="s">
+        <v>946</v>
+      </c>
+      <c r="O278" t="s">
+        <v>25</v>
+      </c>
+      <c r="P278" s="5" t="str">
+        <f>"configuration/assets/"&amp;A278&amp;".svg"</f>
+        <v>configuration/assets/cc.svg</v>
+      </c>
+      <c r="Q278">
+        <v>2</v>
+      </c>
+      <c r="R278" t="b">
+        <v>1</v>
+      </c>
+      <c r="T278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>947</v>
+      </c>
+      <c r="B279">
+        <v>12</v>
+      </c>
+      <c r="C279" t="s">
+        <v>24</v>
+      </c>
+      <c r="D279">
+        <f>F278+2</f>
+        <v>26</v>
+      </c>
+      <c r="E279">
+        <f>E278</f>
+        <v>248</v>
+      </c>
+      <c r="F279">
+        <f>D279+10</f>
+        <v>36</v>
+      </c>
+      <c r="G279">
+        <f>E279+(F279-D279)</f>
+        <v>258</v>
+      </c>
+      <c r="I279">
+        <v>12</v>
+      </c>
+      <c r="J279">
+        <v>0</v>
+      </c>
+      <c r="K279">
+        <v>0</v>
+      </c>
+      <c r="L279">
+        <v>0</v>
+      </c>
+      <c r="M279" t="s">
+        <v>945</v>
+      </c>
+      <c r="N279" t="s">
+        <v>946</v>
+      </c>
+      <c r="O279" t="s">
+        <v>25</v>
+      </c>
+      <c r="P279" s="5" t="str">
+        <f>"configuration/assets/"&amp;A279&amp;".svg"</f>
+        <v>configuration/assets/by.svg</v>
+      </c>
+      <c r="Q279">
+        <v>2</v>
+      </c>
+      <c r="R279" t="b">
+        <v>1</v>
+      </c>
+      <c r="T279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>948</v>
+      </c>
+      <c r="B280">
+        <v>12</v>
+      </c>
+      <c r="C280" t="s">
+        <v>24</v>
+      </c>
+      <c r="D280">
+        <f>F279+2</f>
+        <v>38</v>
+      </c>
+      <c r="E280">
+        <f>E279</f>
+        <v>248</v>
+      </c>
+      <c r="F280">
+        <f>D280+10</f>
+        <v>48</v>
+      </c>
+      <c r="G280">
+        <f>E280+(F280-D280)</f>
+        <v>258</v>
+      </c>
+      <c r="I280">
+        <v>12</v>
+      </c>
+      <c r="J280">
+        <v>0</v>
+      </c>
+      <c r="K280">
+        <v>0</v>
+      </c>
+      <c r="L280">
+        <v>0</v>
+      </c>
+      <c r="M280" t="s">
+        <v>945</v>
+      </c>
+      <c r="N280" t="s">
+        <v>946</v>
+      </c>
+      <c r="O280" t="s">
+        <v>25</v>
+      </c>
+      <c r="P280" s="5" t="str">
+        <f>"configuration/assets/"&amp;A280&amp;".svg"</f>
+        <v>configuration/assets/nc.svg</v>
+      </c>
+      <c r="Q280">
+        <v>2</v>
+      </c>
+      <c r="R280" t="b">
+        <v>1</v>
+      </c>
+      <c r="T280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>115</v>
+      </c>
+      <c r="B281">
+        <v>12</v>
+      </c>
+      <c r="C281" t="s">
+        <v>116</v>
+      </c>
+      <c r="D281">
+        <f>D278</f>
+        <v>14</v>
+      </c>
+      <c r="E281">
+        <f>G278+5</f>
+        <v>263</v>
+      </c>
+      <c r="F281">
+        <f>F277</f>
+        <v>196</v>
+      </c>
+      <c r="G281">
+        <f>E281+3</f>
+        <v>266</v>
+      </c>
+      <c r="H281" t="s">
+        <v>102</v>
+      </c>
+      <c r="I281">
+        <v>10</v>
+      </c>
+      <c r="J281">
+        <v>0</v>
+      </c>
+      <c r="K281">
+        <v>0</v>
+      </c>
+      <c r="L281">
+        <v>0</v>
+      </c>
+      <c r="N281" t="s">
+        <v>21</v>
+      </c>
+      <c r="O281" t="s">
+        <v>25</v>
+      </c>
+      <c r="P281" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="Q281">
+        <v>2</v>
+      </c>
+      <c r="R281" t="b">
+        <v>1</v>
+      </c>
+      <c r="S281" t="s">
+        <v>118</v>
+      </c>
+      <c r="T281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>29</v>
+      </c>
+      <c r="B282">
+        <v>12</v>
+      </c>
+      <c r="C282" t="s">
+        <v>25</v>
+      </c>
+      <c r="D282">
+        <f>D278</f>
+        <v>14</v>
+      </c>
+      <c r="E282">
+        <f>G281+8</f>
+        <v>274</v>
+      </c>
+      <c r="F282">
+        <v>196</v>
+      </c>
+      <c r="G282">
+        <f>E282</f>
+        <v>274</v>
+      </c>
+      <c r="I282">
+        <v>0</v>
+      </c>
+      <c r="J282">
+        <v>0</v>
+      </c>
+      <c r="K282">
+        <v>0</v>
+      </c>
+      <c r="L282">
+        <v>0</v>
+      </c>
+      <c r="N282" t="s">
+        <v>21</v>
+      </c>
+      <c r="O282" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q282">
+        <v>2</v>
+      </c>
+      <c r="R282" t="b">
+        <v>0</v>
+      </c>
+      <c r="S282" t="s">
+        <v>119</v>
+      </c>
+      <c r="T282">
         <v>0</v>
       </c>
     </row>
@@ -60068,8 +60693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="W142" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="W136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B144" sqref="B144"/>
@@ -74428,10 +75053,10 @@
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
-        <v>786</v>
+        <v>899</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>5204</v>
+        <v>905</v>
       </c>
       <c r="C143" s="9" t="s">
         <v>905</v>
@@ -74633,7 +75258,7 @@
         <v>785</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>800</v>
+        <v>5204</v>
       </c>
       <c r="C145" s="9" t="s">
         <v>800</v>

</xml_diff>